<commit_message>
Fixed that the engines get wrongly counted.
</commit_message>
<xml_diff>
--- a/data/enhanced_vehicle_data.xlsx
+++ b/data/enhanced_vehicle_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -822,11 +822,7 @@
           <t>WEB83821751792509</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -880,7 +876,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -934,11 +930,7 @@
           <t>W1T70075084730571</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1104,7 +1096,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -1214,11 +1206,7 @@
           <t>WEB35019575171220</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1326,11 +1314,7 @@
           <t>WEB82176696345140</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1578,11 +1562,7 @@
           <t>W1T51066142888378</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1636,7 +1616,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -1774,11 +1754,7 @@
           <t>W1T42983246132574</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1858,11 +1834,7 @@
           <t>WDB97246638640936</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1972,7 +1944,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -1998,11 +1970,7 @@
           <t>W1T84920730738326</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2054,11 +2022,7 @@
           <t>W1T39073570795970</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>OM 924</t>
-        </is>
-      </c>
+      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2084,7 +2048,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -2166,11 +2130,7 @@
           <t>NMB85011258328792</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2532,7 +2492,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -2588,7 +2548,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -2644,7 +2604,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -2698,11 +2658,7 @@
           <t>NMB76915082126852</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2868,7 +2824,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -2950,11 +2906,7 @@
           <t>W1T95977627054218</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>OM 924</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3008,7 +2960,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -3090,11 +3042,7 @@
           <t>WDB55210210126674</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3232,7 +3180,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -3286,11 +3234,7 @@
           <t>NMB19508764326332</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3372,7 +3316,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -3510,11 +3454,7 @@
           <t>WDB15074727389501</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3538,11 +3478,7 @@
           <t>NMB91532838482279</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3566,11 +3502,7 @@
           <t>WDB82620166664538</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3624,7 +3556,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -3650,11 +3582,7 @@
           <t>W1T65408549768006</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -3680,7 +3608,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -3764,7 +3692,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -3818,11 +3746,7 @@
           <t>W1T14104931218774</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -3874,11 +3798,7 @@
           <t>W1T59495989046715</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -4042,11 +3962,7 @@
           <t>NMB97518139456297</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -4072,7 +3988,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -4184,7 +4100,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -4324,7 +4240,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -4436,7 +4352,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -4490,11 +4406,7 @@
           <t>NMB68675387124893</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4602,11 +4514,7 @@
           <t>WEB13675182237484</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -4630,11 +4538,7 @@
           <t>NMB18505876058372</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -4660,7 +4564,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -4714,11 +4618,7 @@
           <t>WDB64172908761989</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -4772,7 +4672,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -4938,11 +4838,7 @@
           <t>W1T24266360390931</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -5050,11 +4946,7 @@
           <t>W1T32194465952966</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -5134,11 +5026,7 @@
           <t>WEB34232221714881</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -5304,7 +5192,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -5414,11 +5302,7 @@
           <t>WEB15711131661916</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -5442,11 +5326,7 @@
           <t>NMB54295891596434</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -5470,11 +5350,7 @@
           <t>W1T94110442710354</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr">
-        <is>
-          <t>OM 926</t>
-        </is>
-      </c>
+      <c r="F180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -5526,11 +5402,7 @@
           <t>NMB48051423370057</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -5554,11 +5426,7 @@
           <t>WEB58983495409038</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -5752,7 +5620,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -5920,7 +5788,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -5946,11 +5814,7 @@
           <t>WDB63883626217463</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -6030,11 +5894,7 @@
           <t>NMB73188755928785</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -6058,11 +5918,7 @@
           <t>WDB22332639481138</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -6144,7 +6000,7 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -6228,7 +6084,7 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -6282,11 +6138,7 @@
           <t>NMB32370763079682</t>
         </is>
       </c>
-      <c r="F209" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -6394,11 +6246,7 @@
           <t>NMB74601920011870</t>
         </is>
       </c>
-      <c r="F213" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -6452,7 +6300,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -6478,11 +6326,7 @@
           <t>WDB10503953260521</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -6562,11 +6406,7 @@
           <t>WDB57094500721383</t>
         </is>
       </c>
-      <c r="F219" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -6648,7 +6488,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -6928,7 +6768,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -6954,11 +6794,7 @@
           <t>WDB52029786085800</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -6982,11 +6818,7 @@
           <t>NMB87558327145933</t>
         </is>
       </c>
-      <c r="F234" t="inlineStr">
-        <is>
-          <t>OM 924</t>
-        </is>
-      </c>
+      <c r="F234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -7066,11 +6898,7 @@
           <t>WDB19541968144805</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -7124,7 +6952,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -7206,11 +7034,7 @@
           <t>WEB89368702562927</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -7318,11 +7142,7 @@
           <t>W1T45624948667139</t>
         </is>
       </c>
-      <c r="F246" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -7404,7 +7224,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -7570,11 +7390,7 @@
           <t>NMB14264292803256</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -7654,11 +7470,7 @@
           <t>NMB72344209803907</t>
         </is>
       </c>
-      <c r="F258" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -7682,11 +7494,7 @@
           <t>WDB12124059592712</t>
         </is>
       </c>
-      <c r="F259" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -7710,11 +7518,7 @@
           <t>WDB55750311594623</t>
         </is>
       </c>
-      <c r="F260" t="inlineStr">
-        <is>
-          <t>OM 924</t>
-        </is>
-      </c>
+      <c r="F260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -7794,11 +7598,7 @@
           <t>NMB56309403508880</t>
         </is>
       </c>
-      <c r="F263" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -7880,7 +7680,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -7962,11 +7762,7 @@
           <t>WEB93654034433516</t>
         </is>
       </c>
-      <c r="F269" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -8130,11 +7926,7 @@
           <t>W1T94299307726332</t>
         </is>
       </c>
-      <c r="F275" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -8186,11 +7978,7 @@
           <t>WDB75619285356480</t>
         </is>
       </c>
-      <c r="F277" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -8244,7 +8032,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -8300,7 +8088,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -8494,11 +8282,7 @@
           <t>WEB32328699581060</t>
         </is>
       </c>
-      <c r="F288" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -8606,11 +8390,7 @@
           <t>WEB69534365810155</t>
         </is>
       </c>
-      <c r="F292" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -8804,7 +8584,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -8860,7 +8640,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -8970,11 +8750,7 @@
           <t>WEB44427941409731</t>
         </is>
       </c>
-      <c r="F305" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -9026,11 +8802,7 @@
           <t>NMB57245777102047</t>
         </is>
       </c>
-      <c r="F307" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -9084,7 +8856,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -9110,11 +8882,7 @@
           <t>NMB63209848145305</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr">
-        <is>
-          <t>OM 924</t>
-        </is>
-      </c>
+      <c r="F310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -9140,7 +8908,7 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -9194,11 +8962,7 @@
           <t>WDB48171558415910</t>
         </is>
       </c>
-      <c r="F313" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -9306,11 +9070,7 @@
           <t>WEB88998840436035</t>
         </is>
       </c>
-      <c r="F317" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -9334,11 +9094,7 @@
           <t>WEB28444563894252</t>
         </is>
       </c>
-      <c r="F318" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -9588,7 +9344,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -9614,11 +9370,7 @@
           <t>WDB13352840392563</t>
         </is>
       </c>
-      <c r="F328" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -9754,11 +9506,7 @@
           <t>WDB12615219228418</t>
         </is>
       </c>
-      <c r="F333" t="inlineStr">
-        <is>
-          <t>OM 926</t>
-        </is>
-      </c>
+      <c r="F333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -9784,7 +9532,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -9812,7 +9560,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -9922,11 +9670,7 @@
           <t>W1T79284647924366</t>
         </is>
       </c>
-      <c r="F339" t="inlineStr">
-        <is>
-          <t>OM 926</t>
-        </is>
-      </c>
+      <c r="F339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -9978,11 +9722,7 @@
           <t>WDB84682480100671</t>
         </is>
       </c>
-      <c r="F341" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -10036,7 +9776,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -10176,7 +9916,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -10622,11 +10362,7 @@
           <t>NMB51770054164375</t>
         </is>
       </c>
-      <c r="F364" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -10650,11 +10386,7 @@
           <t>W1T67469030136596</t>
         </is>
       </c>
-      <c r="F365" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -10680,7 +10412,7 @@
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -10874,11 +10606,7 @@
           <t>WEB37895016015571</t>
         </is>
       </c>
-      <c r="F373" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -10902,11 +10630,7 @@
           <t>W1T99649061460893</t>
         </is>
       </c>
-      <c r="F374" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -10958,11 +10682,7 @@
           <t>WEB43800996951988</t>
         </is>
       </c>
-      <c r="F376" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -11100,7 +10820,7 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -11154,11 +10874,7 @@
           <t>WEB37379629070027</t>
         </is>
       </c>
-      <c r="F383" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -11350,11 +11066,7 @@
           <t>WDB81949956077542</t>
         </is>
       </c>
-      <c r="F390" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F390" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -11520,7 +11232,7 @@
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>M 936G</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -11604,7 +11316,7 @@
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 473</t>
         </is>
       </c>
     </row>
@@ -11630,11 +11342,7 @@
           <t>WDB47139503886394</t>
         </is>
       </c>
-      <c r="F400" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -11688,7 +11396,7 @@
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -11770,11 +11478,7 @@
           <t>NMB21050253684912</t>
         </is>
       </c>
-      <c r="F405" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F405" t="inlineStr"/>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -11938,11 +11642,7 @@
           <t>NMB31881944007447</t>
         </is>
       </c>
-      <c r="F411" t="inlineStr">
-        <is>
-          <t>M 936G</t>
-        </is>
-      </c>
+      <c r="F411" t="inlineStr"/>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -11968,7 +11668,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 936</t>
         </is>
       </c>
     </row>
@@ -12106,11 +11806,7 @@
           <t>WDB17777585978238</t>
         </is>
       </c>
-      <c r="F417" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F417" t="inlineStr"/>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -12248,7 +11944,7 @@
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 471</t>
         </is>
       </c>
     </row>
@@ -12358,11 +12054,7 @@
           <t>NMB60659679802754</t>
         </is>
       </c>
-      <c r="F426" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F426" t="inlineStr"/>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -12386,11 +12078,7 @@
           <t>WEB22860781682238</t>
         </is>
       </c>
-      <c r="F427" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F427" t="inlineStr"/>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
@@ -12638,11 +12326,7 @@
           <t>W1T23222616356329</t>
         </is>
       </c>
-      <c r="F436" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F436" t="inlineStr"/>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
@@ -12694,11 +12378,7 @@
           <t>NMB82174401589591</t>
         </is>
       </c>
-      <c r="F438" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F438" t="inlineStr"/>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
@@ -12864,7 +12544,7 @@
       </c>
       <c r="F444" t="inlineStr">
         <is>
-          <t>OM 924</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -12920,7 +12600,7 @@
       </c>
       <c r="F446" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 934</t>
         </is>
       </c>
     </row>
@@ -12946,11 +12626,7 @@
           <t>NMB16209071001147</t>
         </is>
       </c>
-      <c r="F447" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F447" t="inlineStr"/>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
@@ -13002,11 +12678,7 @@
           <t>WEB65168982529271</t>
         </is>
       </c>
-      <c r="F449" t="inlineStr">
-        <is>
-          <t>OM 460</t>
-        </is>
-      </c>
+      <c r="F449" t="inlineStr"/>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
@@ -13228,7 +12900,7 @@
       </c>
       <c r="F457" t="inlineStr">
         <is>
-          <t>OM 926</t>
+          <t>OM 470</t>
         </is>
       </c>
     </row>
@@ -13534,11 +13206,7 @@
           <t>W1T98661055753711</t>
         </is>
       </c>
-      <c r="F468" t="inlineStr">
-        <is>
-          <t>OM 926</t>
-        </is>
-      </c>
+      <c r="F468" t="inlineStr"/>
     </row>
     <row r="469">
       <c r="A469" s="1" t="n">

</xml_diff>

<commit_message>
Implemented a function that cleans the column sales_code_array so there are no more vehicles with 2 engines. Also implemented a function that allows the user to choose if the ETL-Pipeline should report what is filtered.
</commit_message>
<xml_diff>
--- a/data/enhanced_vehicle_data.xlsx
+++ b/data/enhanced_vehicle_data.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Z5E, M3E, A4S, Y1R, F5E, J3Y, X4M, J1Z, M5X, V8O, M6O, M8Q, C0E, D2C, B1A, M5N, P1C, C9Q, U2T, P6H, Z2K, P5X, R8N, E9C, A2M, V1D, Y3E, Q5L, F6O, W7Z, Z2R, Z2B, F7S, V9Q, B9Y, Q5B, N0D, W0U, P4A, N4Y, N5U, V0X, U7G, D4W, W6O, K1O, E4L, C9W, D6R, Q1G, A5W, G0U, A4H, Q4X, E1T, U2K, O5Y, L2L, V7Z, T3P, C5S, Z6A, Z7N, K1C, A6J, X1F, Z2L, D7F, W7J, R1A, M0I, Q7I, F9L, Z6N, P2C, K6Q, O2M, E2F, X1Q, R2T, W3W, Q8V, R4L, E5W, Z2A, K5L, Z2I, G5Z, K3W, K1D, C2R, E2T, V4D, W7L, I7X, D7L, P0V, F8D, W3T, W2F, Z9J, A1J, Z0T, B2D, J1O, V2J, V1I, Q8X, F0X, D4S, W9I, Z4J, F6N, Z0I, C8C, K1P, N8I, D6Z, G2B, F8F, E1M, S1M, T2D, N7M, A5B, S1S, W0F, P1L, J3N, V9H, S1R, F3Y, H8W, N3J, E2A, Z4T, F1U, S1Y, D6J, A5Y, U3S, Z3Z, L9V, R1V, Z3L</t>
+          <t>Z5E, M3E, A4S, Y1R, F5E, J3Y, X4M, J1Z, M5X, V8O, M6O, M8Q, C0E, D2C, B1A, M5N, P1C, C9Q, U2T, P6H, Z2K, P5X, R8N, E9C, A2M, V1D, Y3E, Q5L, F6O, W7Z, Z2R, Z2B, F7S, V9Q, B9Y, Q5B, N0D, W0U, P4A, N4Y, N5U, V0X, U7G, D4W, W6O, K1O, E4L, C9W, D6R, Q1G, A5W, G0U, A4H, Q4X, E1T, U2K, O5Y, L2L, V7Z, T3P, C5S, Z6A, Z7N, K1C, A6J, X1F, Z2L, D7F, W7J, R1A, Q7I, F9L, Z6N, P2C, K6Q, O2M, E2F, X1Q, R2T, W3W, Q8V, R4L, E5W, Z2A, K5L, Z2I, G5Z, K3W, K1D, C2R, E2T, V4D, W7L, I7X, D7L, P0V, F8D, W3T, W2F, Z9J, A1J, Z0T, B2D, J1O, V2J, V1I, Q8X, F0X, D4S, W9I, Z4J, F6N, Z0I, C8C, K1P, N8I, D6Z, G2B, F8F, E1M, S1M, T2D, N7M, A5B, S1S, W0F, P1L, J3N, V9H, S1R, F3Y, H8W, N3J, E2A, Z4T, F1U, S1Y, D6J, A5Y, U3S, Z3Z, L9V, R1V, Z3L</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Z5D, M2N, K1X, Q2Z, G0W, F0S, F0K, E4M, V2H, A6A, Z1X, Q1D, A5F, E9C, Q5G, O1E, F5C, X4K, F1Z, F6O, E3I, R5E, O7Y, C9V, P9G, B2G, N3B, C7F, Z0Z, A4B, D9Z, C5S, A2Z, U3D, K2M, T1E, F7I, K3B, B2Z, M0D, W0T, A4K, V1X, V6U, D1J, Z5P, N7P, I1C, S8J, F0F, B4Z, A1Y, Q1U, Z4B, F6V, E0F, K5E, F2Y, H8U, D3H, F5I, P2Z, K1R, F7R, C2T, Y4V, P8F, U1P, N5F, Z8F, F5B, D2F, A6F, Q7E, Y3I, K7S, W0I, I6F, I6X, E1Q, R1B, P0S, Z8P, J3E, P9B, Q5S, Z9E, O4P, E1K, V6C, N8P, O1V, M5N, D7Z, I6C, Z3O, L3Z, Y9Y, C0T, B1C, R5A, G0C, I5G, W3R, J8Z, A5W, Q5Y, U1U, C6A, F9A, C6X, K6D, S1F, J3F, O2N, O2I, C0S, Q0F, N9X, J3C, V7U, N4W, W2V, C8I, E4S, T1O, P2V, D5P, V7S, D6X, C6Y, F6K, D1D, V2U, L1T, N2D, D2U, P7M, Z8S, C7T, O1H, R2M, R7F, E3R, O2L, Z9H, D4Q, Y1Z, I2N, U2Y, D6Z, A1D, E5Z, U2G, D3N, D7D, A1Z, M0U, X3A, Z5H, T5V, W2I, V8A, P0Z, A5E, F9R, P8T, M9O, X3U, E5D, K5A, H1L, P2J, Z0Y, P9E, D3O, R1Z, D6P, Y4F, J9D, H1V, G0G, L9A, Q2Y, C1L, E4Y, R6V, I1I, Z2X, F2P, F2E, Z3X, T2S, E3Z, X1Z, G5Z, W7J, V6H, L1B, V6Z, W6F, Y4I, Z7R, Q2E, F0M, A4G, F2M, Z5A, C1G, Z2P, Z9Y, K2C, Z3H, C3A, N8Q, Z1H, M7K, R6C, A1F, K6E, W0G, U3S, Z0F, V7Z, S5R, K3T, I4U, E3K, G2D, P9A, D1L, F5A, J1X, P5Z, Z1C, O2F, F8M, A1W, O1B, J6Z, O5U, D6C, B5D, V2L, U2U, R1G, F9L, I2B, L1L, F4I, N7K, W7Y, L9I</t>
+          <t>Z5D, M2N, K1X, Q2Z, G0W, F0S, F0K, E4M, V2H, A6A, Z1X, Q1D, A5F, E9C, Q5G, O1E, F5C, X4K, F1Z, F6O, E3I, R5E, O7Y, C9V, P9G, B2G, N3B, C7F, Z0Z, A4B, D9Z, C5S, A2Z, U3D, K2M, T1E, F7I, K3B, B2Z, M0D, W0T, A4K, V1X, V6U, D1J, Z5P, N7P, I1C, S8J, F0F, B4Z, A1Y, Q1U, Z4B, F6V, E0F, K5E, F2Y, H8U, D3H, F5I, P2Z, K1R, F7R, C2T, Y4V, P8F, U1P, N5F, Z8F, F5B, D2F, A6F, Q7E, Y3I, K7S, W0I, I6F, I6X, E1Q, R1B, P0S, Z8P, J3E, P9B, Q5S, Z9E, O4P, E1K, V6C, N8P, O1V, M5N, D7Z, I6C, Z3O, L3Z, Y9Y, C0T, B1C, R5A, G0C, I5G, W3R, J8Z, A5W, Q5Y, U1U, C6A, F9A, C6X, K6D, S1F, J3F, O2N, O2I, C0S, Q0F, N9X, J3C, V7U, N4W, W2V, C8I, E4S, T1O, P2V, D5P, V7S, D6X, C6Y, F6K, D1D, V2U, L1T, N2D, D2U, P7M, Z8S, C7T, O1H, R2M, R7F, E3R, O2L, Z9H, D4Q, Y1Z, I2N, U2Y, D6Z, A1D, E5Z, U2G, D3N, D7D, A1Z, M0U, X3A, Z5H, T5V, W2I, V8A, P0Z, A5E, F9R, P8T, M9O, X3U, E5D, K5A, H1L, P2J, Z0Y, P9E, D3O, R1Z, D6P, Y4F, J9D, H1V, G0G, L9A, Q2Y, C1L, E4Y, R6V, I1I, Z2X, F2P, F2E, Z3X, T2S, E3Z, X1Z, G5Z, W7J, V6H, L1B, V6Z, W6F, Y4I, Z7R, Q2E, F0M, A4G, F2M, C1G, Z2P, Z9Y, K2C, Z3H, C3A, N8Q, Z1H, M7K, R6C, A1F, K6E, W0G, U3S, Z0F, V7Z, S5R, K3T, I4U, E3K, G2D, P9A, D1L, F5A, J1X, P5Z, Z1C, O2F, F8M, A1W, O1B, J6Z, O5U, D6C, B5D, V2L, U2U, R1G, F9L, I2B, L1L, F4I, N7K, W7Y, L9I</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -822,7 +822,11 @@
           <t>WEB83821751792509</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -866,7 +870,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Z5E, M3E, E1N, P4U, Z6M, A5J, F0K, D0V, P8Z, Z2O, D3Z, M8Q, N7G, L4B, K0V, A5D, A1L, F9C, I6D, F6L, C0F, O1X, C2O, Z5O, C2G, B5J, R4Z, D0R, J6Y, J9D, X3P, Z6I, E3S, W5Q, A6B, R1W, S8J, E2I, Z4R, D3B, O4A, K5E, Z7I, C9J, I1F, I2V, W9C, E5D, C0X, K5G, V7J, H6A, S5B, L9Y, J3K, W5N, K0W, Z3I, C2J, W9Q, K7R, E6H, N8K, K0P, G1E, D3F, F7X, B5K, P6Z, B2C, R5I, A4L, Z9V, Z4H, W6N, V7G, C3K, A2A, F4Y, J1O, K2K, N5C, F4P, K0F, M8C, K7Q, N7F, T2R, H8W, W0I, Z0Z, P2H, J2D, E3I, C3L, B5N, Q4P, Z8T, I7N, B2A, E1E, H1P, E5T, Q6Z, R3Q, E5B, K4K, Z7G, I1C, X2R, I0K, C1K, B3K, F3Z, O6G, N4W, D5C, C5G, A1N, W4G, X2Y, Z4J, M7H, R2H, O3D, Z1F, I5Y, M9V, C8F, X4I, A4G, K0I, A5G, K0G, C7S, N7B, W5B, K8X, J2A, Q3U, V6U, J3A, Q0B, D6M, X2Z, N6T, K3F, G4E, P1K, Z4E, P6A, F8B, C3A, I8Z, X3L, I7W, U8X, D6H, N0M, X1L, Q4T, Q5G, N3A, V8A, F3C, Z0T, T1M, N1Z, K3K, L1I, W7Y, J1V, J6C, W0Q, W5C, W3K, E1H, N3K, D5B, P2D, O1U, O7V, W3Q, Z5G, Q1K, N3M, X1Q, K3U, R7B, E0Z, J2U, S8C, V7A, Z4Y, Y3E, K2J, X5G, Z2I, F2Z, D9X, F2U, Q4Z, K2P, R5Q, T1Y, V1C, W4H, P4A, C3S, Q7J, L2H, P9C, J3I, Q2N, V0X, V6B, N5V, E1O, D0K, A0D, Z3R, U0D, T1W, Q2S, F8Z, F1H, Z9K, O8L, I4K, E3E, Q3C, Q4I, B3G, R2S, C1Q, F4X, Q1N, Q7Y, Z5A, D2F, B9Y, X2M, E4G, F3K, R9Y, X1I, O2H, D4B, K7A, Q7H, C2R, Q8Y, D6Y, O7Y, O7E, N3T, F5F</t>
+          <t>Z5E, M3E, E1N, P4U, Z6M, A5J, F0K, D0V, P8Z, Z2O, D3Z, M8Q, N7G, L4B, K0V, A5D, A1L, F9C, I6D, F6L, C0F, O1X, C2O, Z5O, C2G, B5J, R4Z, D0R, J6Y, J9D, X3P, Z6I, E3S, W5Q, A6B, R1W, S8J, E2I, Z4R, D3B, O4A, K5E, Z7I, C9J, I1F, I2V, W9C, E5D, C0X, K5G, V7J, H6A, S5B, L9Y, J3K, W5N, K0W, Z3I, C2J, W9Q, K7R, E6H, N8K, K0P, G1E, D3F, F7X, B5K, P6Z, B2C, R5I, A4L, Z9V, Z4H, W6N, V7G, C3K, A2A, F4Y, J1O, K2K, N5C, F4P, K0F, M8C, K7Q, N7F, T2R, H8W, W0I, Z0Z, P2H, J2D, E3I, C3L, B5N, Q4P, Z8T, I7N, B2A, E1E, H1P, E5T, Q6Z, R3Q, E5B, K4K, Z7G, I1C, X2R, I0K, C1K, B3K, F3Z, O6G, N4W, D5C, C5G, A1N, W4G, X2Y, Z4J, M7H, R2H, O3D, Z1F, I5Y, M9V, C8F, X4I, A4G, K0I, A5G, K0G, C7S, N7B, W5B, K8X, J2A, Q3U, V6U, J3A, Q0B, D6M, X2Z, N6T, K3F, G4E, P1K, Z4E, P6A, F8B, C3A, I8Z, X3L, I7W, U8X, D6H, N0M, X1L, Q4T, Q5G, N3A, V8A, F3C, Z0T, T1M, N1Z, K3K, L1I, W7Y, J1V, J6C, W0Q, W5C, W3K, E1H, N3K, D5B, P2D, O1U, O7V, W3Q, Z5G, Q1K, N3M, X1Q, K3U, R7B, E0Z, J2U, S8C, V7A, Z4Y, Y3E, K2J, X5G, Z2I, F2Z, D9X, F2U, Q4Z, K2P, R5Q, T1Y, V1C, W4H, P4A, C3S, Q7J, L2H, P9C, J3I, Q2N, V0X, V6B, N5V, E1O, D0K, A0D, Z3R, U0D, T1W, Q2S, F8Z, F1H, Z9K, O8L, I4K, E3E, Q3C, Q4I, B3G, R2S, C1Q, F4X, Q1N, Q7Y, D2F, B9Y, X2M, E4G, F3K, R9Y, X1I, O2H, D4B, K7A, Q7H, C2R, Q8Y, D6Y, O7Y, O7E, N3T, F5F</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -930,7 +934,11 @@
           <t>W1T70075084730571</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1086,7 +1094,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Z5F, M3P, Q1L, U2L, O8T, D0U, U1U, E2T, N9V, L2B, J2A, S1S, D9H, M4D, N7O, N3J, W5C, N6J, N7I, K4K, A4A, C0Y, K7D, K7O, I2C, C9I, M5N, V1N, A6D, W2T, K8X, O5M, S5Q, P9E, W2Q, Z7G, E5F, K2P, E5Z, W5Y, N7A, C6Z, R2K, J3D, J9K, K7W, C3Q, P9X, W9I, F7E, D7V, Z1L, W1U, I6C, Q7Q, L2A, N2I, K1B, P9G, W4K, C1J, Z9M, P9C, K0T, J3S, A4B, O7C, P1N, I9I, K2C, F0L, X1E, Y6J, A4P, R1B, E1O, C8W, D3Z, F1A, T1U, U3D, S5I, R2E, T3C, B9V, M5Y, D4A, A1S, I4H, Z7I, D5L, E6K, D2C, Y1B, C6I, M9X, Q6T, Z3S, M0U, Q6L, F9M, E2F, P5N, T4U, W2K, V1Z, L1X, H2I, B2Z, I1I, M5T, E1P, N1Y, T1E, Q7D, E9J, Z3H, A2H, Y1A, Z5A, D0R, Q1C, F8M, A0D, I5H, R2W, C6W, T2D, K8Z, F3S, T1N, Q4P, W5V, R0S, K1Q, A1A, O4P, F8W, Q1H, I5B, X2I, O6Y, R0Z, C9P, R7E, W0L, L1S, Z1T, A5A, E6A, Z7A, A2O, A6B, D5C, M2H, E0Z, P5B, M1B, P4W, Q3Y, U0C, V7A, M0W, W7N, K0X, D7G, D7A, R6S, R8D, G5B, U2I, K0G, A5R, F9T, E0V, F6P, V1E, N1X, X1Z, W1J, Z9Y, V2L, D4I, M0T, Z7C, V3W, X2H, Q1I, Y3K, F5Y, Z3W, C5Y, K0N, N7P, A6K, B3K, W6V, G1I, D4W, N5C, O7G, D0J, R1D, T2C, C0S, O1T, U3Y, H8N, Q8M, D8Z, W7R, F7I, A4L, I6J, D2W, J3P, C9X, B9W, Y4W, O4B, C2H, O4L, C3H, K6N, J2C, B4Z, Z2Y, Q1Y, G2D, W2J, B5B, W4D, C9U, M0K, Q6G, O1O, F6F, C6Y, X1I, T0U, K3Z, F3W, F5U, X4C, V1U, Z1G, E3X, F7D, C7I, A1D, T1B, Z1E, Q8N</t>
+          <t>Z5F, M3P, Q1L, U2L, O8T, D0U, U1U, E2T, N9V, L2B, J2A, S1S, D9H, M4D, N7O, N3J, W5C, N6J, N7I, K4K, A4A, C0Y, K7D, K7O, I2C, C9I, M5N, V1N, A6D, W2T, K8X, O5M, S5Q, P9E, W2Q, Z7G, E5F, K2P, E5Z, W5Y, N7A, C6Z, R2K, J3D, J9K, K7W, C3Q, P9X, W9I, F7E, D7V, Z1L, W1U, I6C, Q7Q, L2A, N2I, K1B, P9G, W4K, C1J, Z9M, P9C, K0T, J3S, A4B, O7C, P1N, I9I, K2C, F0L, X1E, Y6J, A4P, R1B, E1O, C8W, D3Z, F1A, T1U, U3D, S5I, R2E, T3C, B9V, M5Y, D4A, A1S, I4H, Z7I, D5L, E6K, D2C, Y1B, C6I, M9X, Q6T, Z3S, M0U, Q6L, F9M, E2F, P5N, T4U, W2K, V1Z, L1X, H2I, B2Z, I1I, M5T, E1P, N1Y, T1E, Q7D, E9J, Z3H, A2H, Y1A, D0R, Q1C, F8M, A0D, I5H, R2W, C6W, T2D, K8Z, F3S, T1N, Q4P, W5V, R0S, K1Q, A1A, O4P, F8W, Q1H, I5B, X2I, O6Y, R0Z, C9P, R7E, W0L, L1S, Z1T, A5A, E6A, Z7A, A2O, A6B, D5C, M2H, E0Z, P5B, M1B, P4W, Q3Y, U0C, V7A, M0W, W7N, K0X, D7G, D7A, R6S, R8D, G5B, U2I, K0G, A5R, F9T, E0V, F6P, V1E, N1X, X1Z, W1J, Z9Y, V2L, D4I, M0T, Z7C, V3W, X2H, Q1I, Y3K, F5Y, Z3W, C5Y, K0N, N7P, A6K, B3K, W6V, G1I, D4W, N5C, O7G, D0J, R1D, T2C, C0S, O1T, U3Y, H8N, Q8M, D8Z, W7R, F7I, A4L, I6J, D2W, J3P, C9X, B9W, Y4W, O4B, C2H, O4L, C3H, K6N, J2C, B4Z, Z2Y, Q1Y, G2D, W2J, B5B, W4D, C9U, M0K, Q6G, O1O, F6F, C6Y, X1I, T0U, K3Z, F3W, F5U, X4C, V1U, Z1G, E3X, F7D, C7I, A1D, T1B, Z1E, Q8N</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1206,7 +1214,11 @@
           <t>WEB35019575171220</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1314,7 +1326,11 @@
           <t>WEB82176696345140</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1562,7 +1578,11 @@
           <t>W1T51066142888378</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1606,7 +1626,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Z5C, M2A, P8A, F7X, F3H, C9B, Q5Q, S8H, F6C, G3B, S1J, P7N, C3B, P9F, F3Y, Q3R, Z9Y, F0V, L2N, C0U, W7Z, P2H, Q7V, Z8E, W1S, V7T, W7V, N5K, Q4Q, O4D, V7H, O1N, E0F, A2M, L1Y, Z3P, K8Z, J9O, V1I, D3C, G0D, A5J, R6B, W9T, I9Y, V2G, K8Y, E6G, Q7M, K3O, W5M, A4U, Z8R, U3N, H1H, Z5H, X1V, V4S, O2F, N7C, D1I, Q4T, Z0C, H1W, G5A, X1Q, D8U, E6H, E0M, D2L, F7D, W8E, K3F, E7B, M5V, P6Y, Q2R, V8X, M5R, W4V, F0W, Q5K, J2H, N8H, D2P, O3C, R1B, K7P, D6F, P7Q, V7F, T0D, D2T, D7C, M6O, R5R, L1C, K9Z, G1H, Q0V, V2A, V5Z, C1Z, N3A, Z8B, K1U, O9H, I5B, F0Y, O6U, N5V, V7K, C5V, I1Y, P0R, R1H, A6D, I3L, T3Q, C6L, M6L, K1G, I9W, F7I, U6E, C6Q, I0K, S9Y, G1J, G3F, Y4D, U3H, D4M, K0Z, M0I, W3N, D5V, F1Y, A4B, K4C, Z2G, X1X, I5L, P6L, E5Z, Q7I, U3B, Z2N, J1P, N2I, J9D, F2O, D9G, T5B, P5Z, Y1O, L3E, W6S, N8K, I7Y, C6D, D0X, N1H, D4U, J2Y, I2R, N5F, N5H, A2N, K9V, U3M, Z0P, N7B, S9Z, W7J, K0V, W9C, Q8O, V7J, B5Z, M8P, Y1Y, Z8J, M6B, Z8Z, K3C, Z8Y, T0I, O4M, C8R, C7C, W8F, E0U, Z1I, J9C, M9S, W5L, P5P, X4E, K7V, V2I, Z7S, O1M, M5A, Z5U, M5S, C7P, M5U, W4N, K6W, I0A, E4T, Z1V, W0N, M7S, Z5X, K0X, T0S, N7Q, N7F, T1A, B4A, D2O, W8Z, X6A, D5Q, H2H, G5G, F4Z, Z8G, C3D, J2K, D2Z, C3F, K0S, F0L, X2X, F0Z, O7B, T3M, N3N</t>
+          <t>Z5C, M2A, P8A, F7X, F3H, C9B, Q5Q, S8H, F6C, G3B, S1J, P7N, C3B, P9F, F3Y, Q3R, Z9Y, F0V, L2N, C0U, W7Z, P2H, Q7V, Z8E, W1S, V7T, W7V, N5K, Q4Q, O4D, V7H, O1N, E0F, A2M, L1Y, Z3P, K8Z, J9O, V1I, D3C, G0D, A5J, R6B, W9T, I9Y, V2G, K8Y, E6G, Q7M, K3O, W5M, A4U, Z8R, U3N, H1H, Z5H, X1V, V4S, O2F, N7C, D1I, Q4T, Z0C, H1W, G5A, X1Q, D8U, E6H, E0M, D2L, F7D, W8E, K3F, E7B, M5V, P6Y, Q2R, V8X, M5R, W4V, F0W, Q5K, J2H, N8H, D2P, O3C, R1B, K7P, D6F, P7Q, V7F, T0D, D2T, D7C, M6O, R5R, L1C, K9Z, G1H, Q0V, V2A, V5Z, C1Z, N3A, Z8B, K1U, O9H, I5B, F0Y, O6U, N5V, V7K, C5V, I1Y, P0R, R1H, A6D, I3L, T3Q, C6L, M6L, K1G, I9W, F7I, U6E, C6Q, I0K, S9Y, G1J, G3F, Y4D, U3H, D4M, K0Z, W3N, D5V, F1Y, A4B, K4C, Z2G, X1X, I5L, P6L, E5Z, Q7I, U3B, Z2N, J1P, N2I, J9D, F2O, D9G, T5B, P5Z, Y1O, L3E, W6S, N8K, I7Y, C6D, D0X, N1H, D4U, J2Y, I2R, N5F, N5H, A2N, K9V, U3M, Z0P, N7B, S9Z, W7J, K0V, W9C, Q8O, V7J, B5Z, M8P, Y1Y, Z8J, M6B, Z8Z, K3C, Z8Y, T0I, O4M, C8R, C7C, W8F, E0U, Z1I, J9C, M9S, W5L, P5P, X4E, K7V, V2I, Z7S, O1M, M5A, Z5U, M5S, C7P, M5U, W4N, K6W, I0A, E4T, Z1V, W0N, M7S, Z5X, K0X, T0S, N7Q, N7F, T1A, B4A, D2O, W8Z, X6A, D5Q, H2H, G5G, F4Z, Z8G, C3D, J2K, D2Z, C3F, K0S, F0L, X2X, F0Z, O7B, T3M, N3N</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1754,7 +1774,11 @@
           <t>W1T42983246132574</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1834,7 +1858,11 @@
           <t>WDB97246638640936</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1934,7 +1962,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Z5E, M3C, M8D, S1M, J2X, M9V, W7E, Z8N, I5W, E0V, Z2U, K7B, F4Y, H2H, H2K, K5D, W0R, T1W, F6X, K7F, M7U, U2S, O6D, J1D, A6R, T4C, L9F, R8P, Z9V, O6N, S5R, K0X, O8A, O4M, V3F, I1I, P1E, I9Z, W5O, X4N, J1F, A2H, Z6I, D2C, D3L, K6L, X0Z, Q5K, Z3A, V6X, X2M, W0Q, Z5A, F6P, Q6N, I6J, Q3Y, M8C, R2T, Q1S, Y4D, A2X, F5C, O2A, V5V, K6W, C2C, D2P, H1Q, U1P, P9Z, D4Z, D1W, N7W, G1M, U6E, X3A, T0K, T5B, A4B, P8F, W2G, O8U, K7L, I7H, F5N, Z1U, W9H, Z7V, D1Q, E2T, E3H, K4V, E7E, W4J, J1E, W4P, Q2K, A1Q, C9W, P0R, I8Z, E9J, F1A, Q6X, K1C, O7D, K4K, B1E, W2L, F6L, A5E, K7V, W2M, M1C, O2E, O7C, W7V, I7G, D9Y, E1V, L1D, W5U, P9P, T0H, W8B, T2U, W1A, L9I, Q1P, O8O, A1Z, W4D, M6B, I6B, I8Y, X2R, W8M, F2A, P7T, P1M, D7C, K7S, A6S, J3G, Y1C, K7I, K6P, I4K, Z8M, J3Z, D3E, Q5Y, Z3D, J2U, F0S, B1I, T5A, W7T, Q2R, A5H, M5C, W5X, W4K, E6H, N0C, P8T, P2L, R3G, A4H, Z0I, W0W, E0M, X1T, W1G, P2B, W5S, D6W, O1H, C7L, V7O, W2D, N7M, Z4J, E7L, Z2J, E3Q, V3L, K1B, J9B, L9Y, W5C, D2W</t>
+          <t>Z5E, M3C, M8D, S1M, J2X, M9V, W7E, Z8N, I5W, E0V, Z2U, K7B, F4Y, H2H, H2K, K5D, W0R, T1W, F6X, K7F, M7U, U2S, O6D, J1D, A6R, T4C, L9F, R8P, Z9V, O6N, S5R, K0X, O8A, O4M, V3F, I1I, P1E, I9Z, W5O, X4N, J1F, A2H, Z6I, D2C, D3L, K6L, X0Z, Q5K, Z3A, V6X, X2M, W0Q, F6P, Q6N, I6J, Q3Y, M8C, R2T, Q1S, Y4D, A2X, F5C, O2A, V5V, K6W, C2C, D2P, H1Q, U1P, P9Z, D4Z, D1W, N7W, G1M, U6E, X3A, T0K, T5B, A4B, P8F, W2G, O8U, K7L, I7H, F5N, Z1U, W9H, Z7V, D1Q, E2T, E3H, K4V, E7E, W4J, J1E, W4P, Q2K, A1Q, C9W, P0R, I8Z, E9J, F1A, Q6X, K1C, O7D, K4K, B1E, W2L, F6L, A5E, K7V, W2M, M1C, O2E, O7C, W7V, I7G, D9Y, E1V, L1D, W5U, P9P, T0H, W8B, T2U, W1A, L9I, Q1P, O8O, A1Z, W4D, M6B, I6B, I8Y, X2R, W8M, F2A, P7T, P1M, D7C, K7S, A6S, J3G, Y1C, K7I, K6P, I4K, Z8M, J3Z, D3E, Q5Y, Z3D, J2U, F0S, B1I, T5A, W7T, Q2R, A5H, M5C, W5X, W4K, E6H, N0C, P8T, P2L, R3G, A4H, Z0I, W0W, E0M, X1T, W1G, P2B, W5S, D6W, O1H, C7L, V7O, W2D, N7M, Z4J, E7L, Z2J, E3Q, V3L, K1B, J9B, L9Y, W5C, D2W</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1970,7 +1998,11 @@
           <t>W1T84920730738326</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr"/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2014,7 +2046,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Z5L, M3G, B2E, G0C, S5S, C0Z, Y6J, W5M, D1I, I0U, L1Z, O7Z, P9F, R9Y, K0V, D2F, K5Q, X3Y, J3M, W0F, U2S, V7J, Y3I, K5N, W0O, N8Q, Z2M, F3C, Q1T, R0S, C4F, P9Y, N6E, M4D, X2Z, C3D, N2E, Q3Q, E1Q, G1C, J3T, B9Z, C3K, A1K, Q7D, F1J, O2R, K1I, V6U, Z1F, D6Y, D2H, E4Y, Q6G, Q0N, O5N, S5L, O2B, U3F, W9S, C8I, A1R, F6X, C1L, E1D, C6D, Q3C, E9K, W5U, T2Q, Z6M, F8Z, K0E, K7P, X1U, W9J, V1L, K8Z, D3T, Y4J, N7E, P9Z, H1Q, R8A, N7A, U1E, B5C, X3A, N3M, N6R, L1D, W0I, L4Z, D6W, M5F, O4H, V7R, K7Z, Z0C, T1N, C5W, E1V, P1C, Q3X, O7W, Q4A, E1L, J0Z, K0P, F2Y, V1X, Z6B, J2I, M5K, Z6F, C5U, E7C, A5H, V6S, C8Z, I6N, T2E, T3M, M5T, W4T, P2A, Z4B, Q2Y, E6G, V1J, N3A, F1I, W4D, O8B, S8F, D3N, P1F, M8Q, D5J, P5Z, O3D, Q8G, V7D, U1A, I0A, J2U, X1Z, N1I, Z8W, J3R, V6Q, F9Q, Q8L, D5Z, W2X, Q5S, W0N, Y4R, R4Z, C5O, R5H, W4Z, C9B, R1X, U3D, Z9D, C3S, Q4T, E4C, L9G, D3G, W8F, D5X, R2C, I2N, S1D, S1E, W3A, N7P, W3W, Q2H, F5U, K3C, Q2I, J3Q, E5V, F8V, Q2E, U0B, C3J, K0Q, R5P, P2C, F6K, L4A, E6Z, Y6D, E3F, Z2A, K1Y, Z3R, C4I, R8F, J3U, Z3C, L1X, I0F, V8A, E7B, P2J, O1F, I7V, Q3L, R3K, P0T, C9R, E9F, N8M, R9Z, G0W, Z4T, V5Y, A1O, W5R, D6J, R5W, M0I, S1S</t>
+          <t>Z5L, M3G, B2E, G0C, S5S, C0Z, Y6J, W5M, D1I, I0U, L1Z, O7Z, P9F, R9Y, K0V, D2F, K5Q, X3Y, J3M, W0F, U2S, V7J, Y3I, K5N, W0O, N8Q, Z2M, F3C, Q1T, R0S, C4F, P9Y, N6E, M4D, X2Z, C3D, N2E, Q3Q, E1Q, G1C, J3T, B9Z, C3K, A1K, Q7D, F1J, O2R, K1I, V6U, Z1F, D6Y, D2H, E4Y, Q6G, Q0N, O5N, S5L, O2B, U3F, W9S, C8I, A1R, F6X, C1L, E1D, C6D, Q3C, E9K, W5U, T2Q, Z6M, F8Z, K0E, K7P, X1U, W9J, V1L, K8Z, D3T, Y4J, N7E, P9Z, H1Q, R8A, N7A, U1E, B5C, X3A, N3M, N6R, L1D, W0I, L4Z, D6W, M5F, O4H, V7R, K7Z, Z0C, T1N, C5W, E1V, P1C, Q3X, O7W, Q4A, E1L, J0Z, K0P, F2Y, V1X, Z6B, J2I, M5K, Z6F, C5U, E7C, A5H, V6S, C8Z, I6N, T2E, T3M, M5T, W4T, P2A, Z4B, Q2Y, E6G, V1J, N3A, F1I, W4D, O8B, S8F, D3N, P1F, M8Q, D5J, P5Z, O3D, Q8G, V7D, U1A, I0A, J2U, X1Z, N1I, Z8W, J3R, V6Q, F9Q, Q8L, D5Z, W2X, Q5S, W0N, Y4R, R4Z, C5O, R5H, W4Z, C9B, R1X, U3D, Z9D, C3S, Q4T, E4C, L9G, D3G, W8F, D5X, R2C, I2N, S1D, S1E, W3A, N7P, W3W, Q2H, F5U, K3C, Q2I, J3Q, E5V, F8V, Q2E, U0B, C3J, K0Q, R5P, P2C, F6K, L4A, E6Z, Y6D, E3F, Z2A, K1Y, Z3R, C4I, R8F, J3U, Z3C, L1X, I0F, V8A, E7B, P2J, O1F, I7V, Q3L, R3K, P0T, C9R, E9F, N8M, R9Z, G0W, Z4T, V5Y, A1O, W5R, D6J, R5W, S1S</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2022,7 +2054,11 @@
           <t>W1T39073570795970</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2038,7 +2074,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Z5C, M2E, M0I, C9V, V5V, Z1C, K1W, B9V, V2J, R1L, Y1W, B5L, T2L, E1B, X1V, Q1G, D1N, I4J, K8A, G0Z, U1E, Z4D, E0W, M0J, Y4R, U1P, Q4J, F0I, M5B, F1R, C1P, E5B, D4Q, C4G, K2Z, Q2O, W1R, S3A, Q1Z, I7M, E9F, S9B, E2R, E1H, L2P, U3L, E0F, K5J, T2Z, C5Z, J4A, J3Z, W6V, B4K, D1I, E1T, F9W, D4L, Q5Q, L2Q, T2Q, Z7G, A1L, K0G, R1R, Z8R, Z1I, R0Z, M9O, M5Z, P6B, H1M, Q5O, Q4K, X2E, I6P, D6W, Q0H, C7C, W4P, W6P, O3B, D7C, P9S, T1J, Q3X, Q7U, F3G, Y1O, C6O, F0F, I2I, W1X, J3J, E6L, M5M, X2H, R1T, N5L, O7M, N2E, L0A, E0K, W6S, O7Z, W3Y, R8N, J9O, P5X, D9Y, O3C, W6C, F6L, R5I, F8V, T1N, C9Q, F2F, D1A, V8O, X6F, F5C, N5N, V6E, H2C, O0H, E7A, S5S, A0H, C0Q, D0Q, V4D, F0S, K1X, I0Y, Y1T, E9E, N5I, W6F, X6A, I3D, Q4D, P6J, Q1N, E4F, T1X, I1K, G0Q, C4E, Q2S, I5S, N3N, Q7B, Z3B, R6U, D2Y, Q2P, T0U, T1T, A4F, O6Y, Y6D, P2B</t>
+          <t>Z5C, M2E, C9V, V5V, Z1C, K1W, B9V, V2J, R1L, Y1W, B5L, T2L, E1B, X1V, Q1G, D1N, I4J, K8A, G0Z, U1E, Z4D, E0W, Y4R, U1P, Q4J, F0I, M5B, F1R, C1P, E5B, D4Q, C4G, K2Z, Q2O, W1R, S3A, Q1Z, I7M, E9F, S9B, E2R, E1H, L2P, U3L, E0F, K5J, T2Z, C5Z, J4A, J3Z, W6V, B4K, D1I, E1T, F9W, D4L, Q5Q, L2Q, T2Q, Z7G, A1L, K0G, R1R, Z8R, Z1I, R0Z, M9O, M5Z, P6B, H1M, Q5O, Q4K, X2E, I6P, D6W, Q0H, C7C, W4P, W6P, O3B, D7C, P9S, T1J, Q3X, Q7U, F3G, Y1O, C6O, F0F, I2I, W1X, J3J, E6L, M5M, X2H, R1T, N5L, O7M, N2E, L0A, E0K, W6S, O7Z, W3Y, R8N, J9O, P5X, D9Y, O3C, W6C, F6L, R5I, F8V, T1N, C9Q, F2F, D1A, V8O, X6F, F5C, N5N, V6E, H2C, O0H, E7A, S5S, A0H, C0Q, D0Q, V4D, F0S, K1X, I0Y, Y1T, E9E, N5I, W6F, X6A, I3D, Q4D, P6J, Q1N, E4F, T1X, I1K, G0Q, C4E, Q2S, I5S, N3N, Q7B, Z3B, R6U, D2Y, Q2P, T0U, T1T, A4F, O6Y, Y6D, P2B</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2130,7 +2166,11 @@
           <t>NMB85011258328792</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2482,7 +2522,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Z5E, M3D, Z8K, U0C, T4C, E1L, R4Z, K3E, Z0V, T3K, X1U, E3B, Z0D, M7R, D0L, K1L, Y4X, O1N, F4I, Z1J, P6L, Y9W, D3D, D9Q, C8L, E2N, K4Z, N4B, D3H, D7G, P1I, W3Y, R2E, E0X, R2H, C7G, P9S, I7V, B1H, N8N, Q8T, F1S, Q4M, Q4F, E9W, R5R, F6E, P7Q, T1M, R1J, O8B, Q9A, O6S, M0E, V5O, Z5O, C3A, U3Q, V1M, Q3Y, R2S, S5K, F0L, L2I, N1G, D5L, I7N, V2B, X2T, L1P, U8C, T1V, Z1G, K1N, D5E, D3E, Z3I, R7K, S1R, L2P, K6D, N9S, O1C, G3H, C5I, R1G, Q7F, E4S, I4J, K1W, K7I, V3K, R0Z, K2L, Q4S, D4C, W5N, T2Q, F3G, P5H, C5A, X2P, Y1I, E2I, Z2O, K6G, V0Z, K7A, V1B, K1C, Q2T, Y2A, R2J, R8F, W0T, D3C, A5P, B5C, Z8Y, M6D, Z8C, W0G, U7L, P8A, O7W, F4G, M0T, E3J, E4Z, O8A, Z3Z, Z8B, L1I, J9Q, O4I, Q8U, C3T, Q4T, I4D, K6V, M4Y, Z8H, P7R, O4S, Z4O, Z0C, Z0O, P5Y, I6D, V5Q, E2T, E9H, C6K, Y4B, A1N, F3C, E4C, C5F, R4P, I6A, G1J, M5P, T1U, N1N, M4D, F3S, K3F, F1M, B1Z, W8C, C8H, M5X, C3P, J2M, Q3U, T8A, D9L, M5G, V7A, D7A, O2H, Q5Z, P2R, W7T, C6C, J1E, E4B, T3L, K3Z, K0Z, R5O, E1P, V1Z, X1X, E3Q, N5N, E9Z, K1H, I0F, Q8Y, W0Y, D5Z, V1K, F6B, K2X, Q1A, D8L, E0Z, J0Z, P2C, E6L, X3V, F3V, N4D, M7F, W4N, Z4U, U0Q, Q7Y, A0H, I6B, I7M, Q1W, G0Q, E0D, A2K, F9X, P6Q, C3L, G3A, I8X, P0L, X2V, C7T, T0X, L3Z, C2H, F4Y, K0D, U1F, H1N, K1F, E0R, C0W, O6E, N5X, I1T, Z5A, M0J, P1N, V5Y, P8Y, W3H, W8E, C2A, R2P, W2M, U3V, D1L, J6A, G5G, V5T, K7N</t>
+          <t>Z5E, M3D, Z8K, U0C, T4C, E1L, R4Z, K3E, Z0V, T3K, X1U, E3B, Z0D, M7R, D0L, K1L, Y4X, O1N, F4I, Z1J, P6L, Y9W, D3D, D9Q, C8L, E2N, K4Z, N4B, D3H, D7G, P1I, W3Y, R2E, E0X, R2H, C7G, P9S, I7V, B1H, N8N, Q8T, F1S, Q4M, Q4F, E9W, R5R, F6E, P7Q, T1M, R1J, O8B, Q9A, O6S, M0E, V5O, Z5O, C3A, U3Q, V1M, Q3Y, R2S, S5K, F0L, L2I, N1G, D5L, I7N, V2B, X2T, L1P, U8C, T1V, Z1G, K1N, D5E, D3E, Z3I, R7K, S1R, L2P, K6D, N9S, O1C, G3H, C5I, R1G, Q7F, E4S, I4J, K1W, K7I, V3K, R0Z, K2L, Q4S, D4C, W5N, T2Q, F3G, P5H, C5A, X2P, Y1I, E2I, Z2O, K6G, V0Z, K7A, V1B, K1C, Q2T, Y2A, R2J, R8F, W0T, D3C, A5P, B5C, Z8Y, M6D, Z8C, W0G, U7L, P8A, O7W, F4G, M0T, E3J, E4Z, O8A, Z3Z, Z8B, L1I, J9Q, O4I, Q8U, C3T, Q4T, I4D, K6V, M4Y, Z8H, P7R, O4S, Z4O, Z0C, Z0O, P5Y, I6D, V5Q, E2T, E9H, C6K, Y4B, A1N, F3C, E4C, C5F, R4P, I6A, G1J, M5P, T1U, N1N, M4D, F3S, K3F, F1M, B1Z, W8C, C8H, M5X, C3P, J2M, Q3U, T8A, D9L, M5G, V7A, D7A, O2H, Q5Z, P2R, W7T, C6C, J1E, E4B, T3L, K3Z, K0Z, R5O, E1P, V1Z, X1X, E3Q, N5N, E9Z, K1H, I0F, Q8Y, W0Y, D5Z, V1K, F6B, K2X, Q1A, D8L, E0Z, J0Z, P2C, E6L, X3V, F3V, N4D, M7F, W4N, Z4U, U0Q, Q7Y, A0H, I6B, I7M, Q1W, G0Q, E0D, A2K, F9X, P6Q, C3L, G3A, I8X, P0L, X2V, C7T, T0X, L3Z, C2H, F4Y, K0D, U1F, H1N, K1F, E0R, C0W, O6E, N5X, I1T, P1N, V5Y, P8Y, W3H, W8E, C2A, R2P, W2M, U3V, D1L, J6A, G5G, V5T, K7N</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2538,7 +2578,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Z5B, M1K, I5X, J3G, X1B, A4Z, O8A, N8I, D5U, S1G, E3A, Y4H, R2G, O7D, Z9B, V9Q, D4H, S5I, N2F, R6M, A6L, Z4O, E5J, I1T, O1D, K7N, D6Y, Z6E, V1S, J3E, I6J, W2I, U3M, N8N, O7B, C5G, K6I, N4E, W3Z, Z5G, K7K, A6P, P2E, L3E, N5D, V5T, D0K, J3U, I1V, C9Y, Z0S, R2J, N2S, U3H, X4N, Z1A, K7O, V4S, Y4J, K3Q, W5K, X2F, S1J, C1L, V1Y, I5E, D9M, M5O, O4B, Q4C, Q2H, Z9I, Z5A, P1L, I7Y, E3V, V7B, I1H, N4M, Z0D, I0U, J1T, X1H, K0P, N7Q, W9R, M5Z, E1M, C7Q, C6S, B5L, N5Z, Y1F, M5M, N5F, Q3D, X1Z, X4E, Q0H, S1M, B3H, W2B, L1Z, V1J, K1U, X3F, C3U, V2V, N0C, C5Z, A1K, C9A, F1O, Y9Y, C8D, H1X, W7R, A4R, Q0X, D2F, C4B, W9P, P9A, Z6M, C3M, Q6A, O0C, K1J, P6D, B5Z, K6C, O8C, V9B, O4A, T1M, E3S, I8Z, U1E, T0F, X2M, Z2R, I4H, M6L, L3C, Q7U, I5R, M0Z, P8M, K1A, M7R, Z6A, E0E, E5L, E5C, R7L, O0G, Z9M, N8K, K0L, I6N, V2J, I5T, J2J, V7Q, V1G, W1M, O6N, I0A, S5P, H2J, Q3R, I2F, V2L, S9X, O6H, R1T, F6V, J4Z, U2F, K6K, B5E, N5M, K2A, P0U, O2R, A2P, Y6D, K9V, F8C, K5L, F0P, E0W, W5G, W9J, K6F, Z7Q, X2A, M0S, T3B, N1Z, Q2O, J1G, I5Z, W2M, J1F, Z0X, W8P, Q5S, X1E, Q2G, D6I, O1V, E5I, A1R, G0S, Z4I, U8D, H8Y, N7K, A5A, F0L, P8E, I6C, C1V, K3U, H8X, L9W, Q4F, E9I, M5F, V6E, W5J, W5N</t>
+          <t>Z5B, M1K, I5X, J3G, X1B, A4Z, O8A, N8I, D5U, S1G, E3A, Y4H, R2G, O7D, Z9B, V9Q, D4H, S5I, N2F, R6M, A6L, Z4O, E5J, I1T, O1D, K7N, D6Y, Z6E, V1S, J3E, I6J, W2I, U3M, N8N, O7B, C5G, K6I, N4E, W3Z, Z5G, K7K, A6P, P2E, L3E, N5D, V5T, D0K, J3U, I1V, C9Y, Z0S, R2J, N2S, U3H, X4N, Z1A, K7O, V4S, Y4J, K3Q, W5K, X2F, S1J, C1L, V1Y, I5E, D9M, M5O, O4B, Q4C, Q2H, Z9I, P1L, I7Y, E3V, V7B, I1H, N4M, Z0D, I0U, J1T, X1H, K0P, N7Q, W9R, M5Z, E1M, C7Q, C6S, B5L, N5Z, Y1F, M5M, N5F, Q3D, X1Z, X4E, Q0H, S1M, B3H, W2B, L1Z, V1J, K1U, X3F, C3U, V2V, N0C, C5Z, A1K, C9A, F1O, Y9Y, C8D, H1X, W7R, A4R, Q0X, D2F, C4B, W9P, P9A, Z6M, C3M, Q6A, O0C, K1J, P6D, B5Z, K6C, O8C, V9B, O4A, T1M, E3S, I8Z, U1E, T0F, X2M, Z2R, I4H, M6L, L3C, Q7U, I5R, M0Z, P8M, K1A, M7R, Z6A, E0E, E5L, E5C, R7L, O0G, Z9M, N8K, K0L, I6N, V2J, I5T, J2J, V7Q, V1G, W1M, O6N, I0A, S5P, H2J, Q3R, I2F, V2L, S9X, O6H, R1T, F6V, J4Z, U2F, K6K, B5E, N5M, K2A, P0U, O2R, A2P, Y6D, K9V, F8C, K5L, F0P, E0W, W5G, W9J, K6F, Z7Q, X2A, M0S, T3B, N1Z, Q2O, J1G, I5Z, W2M, J1F, Z0X, W8P, Q5S, X1E, Q2G, D6I, O1V, E5I, A1R, G0S, Z4I, U8D, H8Y, N7K, A5A, F0L, P8E, I6C, C1V, K3U, H8X, L9W, Q4F, E9I, M5F, V6E, W5J, W5N</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2594,7 +2634,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Z5B, M1K, P9S, F5T, C5P, F0L, K5J, N1N, E7L, V7N, I6H, A4P, R1C, I3L, W2L, M0S, C8I, S9Y, N1J, M0J, C6J, L9Y, G3G, H2G, A6N, R5O, I2N, K8A, U2P, Q6I, V0V, J3N, K2B, N8I, C6P, F5F, Q7U, J3F, L1P, X4A, O7T, V5R, F0P, X1W, F9P, R4W, F0O, W3Y, A5C, W6N, D2A, Q1X, D7X, K6D, E1A, C4P, E2F, C4M, M0C, R2T, R1Y, S1U, K7Y, J1F, Y4Y, I2P, T1Y, K6M, A6J, K5Y, P2H, Q3B, W4H, L1L, O0B, T0R, R1T, D4H, C0L, A4G, Q2H, Y1H, E5V, Z2Z, C2Q, N3H, N4B, D6G, C6D, F1P, E9E, D5E, I6Y, J6C, Z4V, Z0R, H8Z, E1S, I7G, L1C, I1M, Z2H, L1A, M8C, V2L, W7K, D1S, P0X, S5Z, C0U, O2H, V9B, A6K, T1V, T0H, K1W, A9Z, R4X, V7R, A6D, C3E, P2N, X2N, O1V, Q3U, X1U, O7P, U2Y, C4X, R6Y, Q2S, D4X, C7M, E5M, Z9X, J1W, T2V, Z1V, Z2M, F0G, Z8I, Z5N, Z0J, C8V, B9Y, Q8M, B2D, Q1B, O8J, Z9E, R7J, O4B, Q7T, I0A, F9R, O2E, Z4P, A5P, E7A, Q6H, G3L, U1E, F3H, X1G, L0Y, D2T, E6M, P2Q, W5H, N5N, O0F, Q1Z, Z4I, W4E, Y1T, P1J, A3D, Z7Y, V1D, Q5D, B5L, V6H, G1D, C2S, D0Z, T3R, F1T</t>
+          <t>Z5B, M1K, P9S, F5T, C5P, F0L, K5J, N1N, E7L, V7N, I6H, A4P, R1C, I3L, W2L, M0S, C8I, S9Y, N1J, C6J, L9Y, G3G, H2G, A6N, R5O, I2N, K8A, U2P, Q6I, V0V, J3N, K2B, N8I, C6P, F5F, Q7U, J3F, L1P, X4A, O7T, V5R, F0P, X1W, F9P, R4W, F0O, W3Y, A5C, W6N, D2A, Q1X, D7X, K6D, E1A, C4P, E2F, C4M, M0C, R2T, R1Y, S1U, K7Y, J1F, Y4Y, I2P, T1Y, K6M, A6J, K5Y, P2H, Q3B, W4H, L1L, O0B, T0R, R1T, D4H, C0L, A4G, Q2H, Y1H, E5V, Z2Z, C2Q, N3H, N4B, D6G, C6D, F1P, E9E, D5E, I6Y, J6C, Z4V, Z0R, H8Z, E1S, I7G, L1C, I1M, Z2H, L1A, M8C, V2L, W7K, D1S, P0X, S5Z, C0U, O2H, V9B, A6K, T1V, T0H, K1W, A9Z, R4X, V7R, A6D, C3E, P2N, X2N, O1V, Q3U, X1U, O7P, U2Y, C4X, R6Y, Q2S, D4X, C7M, E5M, Z9X, J1W, T2V, Z1V, Z2M, F0G, Z8I, Z5N, Z0J, C8V, B9Y, Q8M, B2D, Q1B, O8J, Z9E, R7J, O4B, Q7T, I0A, F9R, O2E, Z4P, A5P, E7A, Q6H, G3L, U1E, F3H, X1G, L0Y, D2T, E6M, P2Q, W5H, N5N, O0F, Q1Z, Z4I, W4E, Y1T, P1J, A3D, Z7Y, V1D, Q5D, B5L, V6H, G1D, C2S, D0Z, T3R, F1T</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2658,7 +2698,11 @@
           <t>NMB76915082126852</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2814,7 +2858,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Z5F, M3V, G5G, L2A, A5P, F9M, D6N, E9F, W3R, P7A, Q3B, W4U, K6D, M0D, Z1F, V6I, Q6N, S3A, O0F, Z9F, D2F, D0Z, Q9C, O4O, G1J, L1I, A2X, P9R, E8A, B2G, V4T, A2V, V2I, E3X, J0Z, O1T, Y1F, P6E, D9N, E3S, W1B, K3S, C9E, T4C, Q5N, Z9C, A2M, S5A, V7Z, E4C, W1O, D6R, Q4F, C3E, R6U, D8M, Z1L, L2I, D3K, D8A, W3Q, O2L, T0F, D7Y, X1T, A4K, Q1V, W8Z, A6S, O7F, V0V, Q1K, U2P, N1V, Q8G, L9Y, C2C, B2A, N6E, A6K, S1S, Z7G, D0B, Y9W, K5U, A1X, L3A, K1B, L0U, V1K, M5L, F1W, Z3Q, Z5I, M0I, Z4L, X3Y, O9G, R2Y, Z9I, K5G, N6J, D2B, E1T, P5H, W3L, X2X, D3N, R2J, P2B, X3D, G0O, W0F, D2V, J9Q, E2R, Z4Q, K1R, T0Z, A4H, X3V, R5O, P8D, W7F, O7C, U0D, F7S, P2S, K1M, D2Q, D5L, Q9A, J8Z, R2Z, U3S, K3E, A2J, A1J, N4D, K6G, Z4I, J1V, V4N, K0F, K5C, T1Z, C6T, C3S, D2U, T1Y, Q7S, F6X, C6P, R2R, J8W, E5J, V3K, N1Z, F8F, Q3X, V1M, J2E, Q5Z, D9A, F3W, M8P, V7P, R5M, Y4H, K3K, D2L, D3H, K2K, Q7D, C5F, W0Y, K8Z, R7H, Z9V, D1V, B4A, P2D, O4S, K3J, D4C, P6C, O6E, C3T, C7E, O6J, B9Z, E9Z, J9R, K0L, W1Z, M5B, C7B, W2F, I5X, O1H, V1B, K7C, N5U, S5C, Z4O, W5K, V5T, V1P, E2L, V8N, T1M, D6J, O7Y, Z8U, Q5L, X1J, M6L, F9W, T3N, D3O, R1N, Z1U, D4Q, V7Q, Y3F, J3P, S9Y, V7O, T5B, A4S, P4W, G3Y, G0N, T0G, W5D, D7F, E9E, F6B, P7N, T1C, U2Q, C1R, Z9H, Q8B, D7J, V2E, O6B, M8B, T2B, M5M, Q1I, R8A, O7W, V1X, Z2I, Q4Z, J1A, B2C</t>
+          <t>Z5F, M3V, G5G, L2A, A5P, F9M, D6N, E9F, W3R, P7A, Q3B, W4U, K6D, M0D, Z1F, V6I, Q6N, S3A, O0F, Z9F, D2F, D0Z, Q9C, O4O, G1J, L1I, A2X, P9R, E8A, B2G, V4T, A2V, V2I, E3X, J0Z, O1T, Y1F, P6E, D9N, E3S, W1B, K3S, C9E, T4C, Q5N, Z9C, A2M, S5A, V7Z, E4C, W1O, D6R, Q4F, C3E, R6U, D8M, Z1L, L2I, D3K, D8A, W3Q, O2L, T0F, D7Y, X1T, A4K, Q1V, W8Z, A6S, O7F, V0V, Q1K, U2P, N1V, Q8G, L9Y, C2C, B2A, N6E, A6K, S1S, Z7G, D0B, Y9W, K5U, A1X, L3A, K1B, L0U, V1K, M5L, F1W, Z3Q, Z5I, Z4L, X3Y, O9G, R2Y, Z9I, K5G, N6J, D2B, E1T, P5H, W3L, X2X, D3N, R2J, P2B, X3D, G0O, W0F, D2V, J9Q, E2R, Z4Q, K1R, T0Z, A4H, X3V, R5O, P8D, W7F, O7C, U0D, F7S, P2S, K1M, D2Q, D5L, Q9A, J8Z, R2Z, U3S, K3E, A2J, A1J, N4D, K6G, Z4I, J1V, V4N, K0F, K5C, T1Z, C6T, C3S, D2U, T1Y, Q7S, F6X, C6P, R2R, J8W, E5J, V3K, N1Z, F8F, Q3X, V1M, J2E, Q5Z, D9A, F3W, M8P, V7P, R5M, Y4H, K3K, D2L, D3H, K2K, Q7D, C5F, W0Y, K8Z, R7H, Z9V, D1V, B4A, P2D, O4S, K3J, D4C, P6C, O6E, C3T, C7E, O6J, B9Z, E9Z, J9R, K0L, W1Z, M5B, C7B, W2F, I5X, O1H, V1B, K7C, N5U, S5C, Z4O, W5K, V5T, V1P, E2L, V8N, T1M, D6J, O7Y, Z8U, Q5L, X1J, M6L, F9W, T3N, D3O, R1N, Z1U, D4Q, V7Q, Y3F, J3P, S9Y, V7O, T5B, A4S, P4W, G3Y, G0N, T0G, W5D, D7F, E9E, F6B, P7N, T1C, U2Q, C1R, Z9H, Q8B, D7J, V2E, O6B, M8B, T2B, M5M, Q1I, R8A, O7W, V1X, Z2I, Q4Z, J1A, B2C</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2898,7 +2942,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Z5L, M3I, F7E, O6G, Q7P, R8B, F1Y, C2P, C6G, D2V, V4A, D0Y, W8B, V7N, N5E, K1P, D1W, M9U, W5R, L1X, J1O, T0Q, X6A, Z8S, I1C, W2L, Q9A, C8T, W2S, T2L, V2P, Z0P, W5X, X4L, P7N, V7S, F0S, P6D, W9Q, U3A, C2Q, T3L, F6X, E1C, F6H, U2V, W5L, W7D, Y6E, Z9B, R8K, H8X, V5R, I4C, Q6E, F8H, P5Z, B5C, F9X, M7T, C0Y, B9X, J3H, W1N, W6V, O2O, F0N, R5Z, R1V, K2A, M0I, L0V, K0V, Q2O, V2D, W9F, Q4K, M6P, R5P, V6C, A1G, R1U, K6K, E9F, U8D, O7P, W0Z, E4W, D7I, N6R, K8A, P6I, I6K, Y4U, Z0R, W0H, R6B, J9Z, P2P, A4G, E5E, C5H, W8U, U1P, D1K, N8M, E1M, D2C, Z6K, P0D, W1B, G0U, K6W, I0Y, E7T, A1S, K1F, F0Z, Z9D, D9Q, A2I, F3P, N4W, D2B, T2Z, I4U, T1H, E3C, G4B, C8B, P4Y, I1F, C9E, F5U, E4T, O6J, S5R, P7P, T0P, D3A, D0E, T0F, F4X, Q8V, K4N, X1S, E2F, P1F, C7K, Y1D, O2E, K1T, E2I, V3F, D3E, Q8C, N1I, I6F, Q6H, L2K, F6B, G5A, V7L, M0L, I2R, U3V, D2F, Q7S, V6E, A2T, S3A, Z1U, V7W, W8E, C6H, A4R, N4G, V5S, H1Y, T5A, O5M, C9C, R2R, Z0C, A0D, T0J, N0M, Q8F, E9H, W8M, A6K, C3M, N1M, Z1M, K0G, T8A, V8B, I4A, V6D, X2R, F6Q, J8Z, F9A, F8C, O2C, N9Y, N4F, M4Y, L2A, E1I, K1W, P9B, Y1Y, R6Z, S5A, W6C, A2H, I5M, H2A, Z7Y, O1H, B2B</t>
+          <t>Z5L, M3I, F7E, O6G, Q7P, R8B, F1Y, C2P, C6G, D2V, V4A, D0Y, W8B, V7N, N5E, K1P, D1W, M9U, W5R, L1X, J1O, T0Q, X6A, Z8S, I1C, W2L, Q9A, C8T, W2S, T2L, V2P, Z0P, W5X, X4L, P7N, V7S, F0S, P6D, W9Q, U3A, C2Q, T3L, F6X, E1C, F6H, U2V, W5L, W7D, Y6E, Z9B, R8K, H8X, V5R, I4C, Q6E, F8H, P5Z, B5C, F9X, M7T, C0Y, B9X, J3H, W1N, W6V, O2O, F0N, R5Z, R1V, K2A, L0V, K0V, Q2O, V2D, W9F, Q4K, M6P, R5P, V6C, A1G, R1U, K6K, E9F, U8D, O7P, W0Z, E4W, D7I, N6R, K8A, P6I, I6K, Y4U, Z0R, W0H, R6B, J9Z, P2P, A4G, E5E, C5H, W8U, U1P, D1K, N8M, E1M, D2C, Z6K, P0D, W1B, G0U, K6W, I0Y, E7T, A1S, K1F, F0Z, Z9D, D9Q, A2I, F3P, N4W, D2B, T2Z, I4U, T1H, E3C, G4B, C8B, P4Y, I1F, C9E, F5U, E4T, O6J, S5R, P7P, T0P, D3A, D0E, T0F, F4X, Q8V, K4N, X1S, E2F, P1F, C7K, Y1D, O2E, K1T, E2I, V3F, D3E, Q8C, N1I, I6F, Q6H, L2K, F6B, G5A, V7L, M0L, I2R, U3V, D2F, Q7S, V6E, A2T, S3A, Z1U, V7W, W8E, C6H, A4R, N4G, V5S, H1Y, T5A, O5M, C9C, R2R, Z0C, A0D, T0J, N0M, Q8F, E9H, W8M, A6K, C3M, N1M, Z1M, K0G, T8A, V8B, I4A, V6D, X2R, F6Q, J8Z, F9A, F8C, O2C, N9Y, N4F, M4Y, L2A, E1I, K1W, P9B, Y1Y, R6Z, S5A, W6C, A2H, I5M, H2A, Z7Y, O1H, B2B</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2906,7 +2950,11 @@
           <t>W1T95977627054218</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2950,7 +2998,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Z5F, M3N, R2L, R1H, I8Y, Z4G, D1L, B1I, F3F, C8I, G2D, Q1A, B5Z, D4Z, W3N, Q2X, N5M, E6C, Y1G, C5M, C0A, B0A, Q1H, I6X, C0M, G3B, N7Q, F9R, K6H, A2L, G0N, Z8Q, Q7Z, P6Z, E0M, P2C, I5A, S1I, R6S, Q4B, A0D, K3R, I4F, J9N, W7Y, I7X, D4S, Z1W, B5D, Z7C, F5E, W5W, R7K, Z2K, B2F, A4D, M0I, R3H, N3H, W4B, K6S, W3Z, K2K, L1Y, W2A, C1S, A2M, E0Z, K4N, M5Y, K0E, O5X, A5L, Z0K, Q7C, I1A, J9F, F0I, M8Z, N2G, N0C, O5T, E6H, X1V, S8F, U1E, W8E, M8P, T1L, E2R, D8U, C2Q, J3O, V6W, A3C, P9R, N5K, Z1A, Q8D, I5E, A4L, W7N, M5V, I6Y, G0C, U8B, F3Z, C1M, Q8L, B1U, N7B, T3C, V7O, D8A, M0A, W6C, B5E, X6F, W9R, O6R, Z4M, I4I, P2A, Q7O, D4H, A2E, Z2Y, K5C, D0I, I4D, E3G, Q1D, N0D, M7F, D4C, K7B, V1G, C1P, C4I, V1S, Z5I, X2V, E5X, K4L, W7R, Q1Q, V7N, K6U, W2Y, K4Z, Q7E, N3N, D2F, J3H, G0U, C3H, Q2A, T2J, U2S, U0O, W0T, Z4S, P9S, Z5Z, K7P, D0D, P1M, E0Y, Z7Z, V7R, K1D, T1J, F7A, K1H, J3Y, Z7U, E6D, W6R, J2W, I6I, K2E, W5N, D0K, E2A, F9Z, O1X, I0F, R5M, I4U, Q9Y, A2B, T1N, D3X, D3N, E1A, E9C, E8A, Z8I, C7U, Z4W, Z4X, R7H, D6Y, O3B, Z7N, C6P, D5O, U2R, A5Q, M0X, F0A, M5B, B1D, L1I, K7F, E3V, F0T, X4M, O0I, V6V, P5Y, W6P, O9H, T4A, F3S, C3S, Q1U, C0E, J3Q, K5P, P5A, N5F, X3V</t>
+          <t>Z5F, M3N, R2L, R1H, I8Y, Z4G, D1L, B1I, F3F, C8I, G2D, Q1A, B5Z, D4Z, W3N, Q2X, N5M, E6C, Y1G, C5M, C0A, B0A, Q1H, I6X, C0M, G3B, N7Q, F9R, K6H, A2L, G0N, Z8Q, Q7Z, P6Z, E0M, P2C, I5A, S1I, R6S, Q4B, A0D, K3R, I4F, J9N, W7Y, I7X, D4S, Z1W, B5D, Z7C, F5E, W5W, R7K, Z2K, B2F, A4D, R3H, N3H, W4B, K6S, W3Z, K2K, L1Y, W2A, C1S, A2M, E0Z, K4N, M5Y, K0E, O5X, A5L, Z0K, Q7C, I1A, J9F, F0I, M8Z, N2G, N0C, O5T, E6H, X1V, S8F, U1E, W8E, M8P, T1L, E2R, D8U, C2Q, J3O, V6W, A3C, P9R, N5K, Z1A, Q8D, I5E, A4L, W7N, M5V, I6Y, G0C, U8B, F3Z, C1M, Q8L, B1U, N7B, T3C, V7O, D8A, M0A, W6C, B5E, X6F, W9R, O6R, Z4M, I4I, P2A, Q7O, D4H, A2E, Z2Y, K5C, D0I, I4D, E3G, Q1D, N0D, M7F, D4C, K7B, V1G, C1P, C4I, V1S, Z5I, X2V, E5X, K4L, W7R, Q1Q, V7N, K6U, W2Y, K4Z, Q7E, N3N, D2F, J3H, G0U, C3H, Q2A, T2J, U2S, U0O, W0T, Z4S, P9S, Z5Z, K7P, D0D, P1M, E0Y, Z7Z, V7R, K1D, T1J, F7A, K1H, J3Y, Z7U, E6D, W6R, J2W, I6I, K2E, W5N, D0K, E2A, F9Z, O1X, I0F, R5M, I4U, Q9Y, A2B, T1N, D3X, D3N, E1A, E9C, E8A, Z8I, C7U, Z4W, Z4X, R7H, D6Y, O3B, Z7N, C6P, D5O, U2R, A5Q, M0X, F0A, M5B, B1D, L1I, K7F, E3V, F0T, X4M, O0I, V6V, P5Y, W6P, O9H, T4A, F3S, C3S, Q1U, C0E, J3Q, K5P, P5A, N5F, X3V</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3034,7 +3082,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Z5L, M3L, C0J, Q8T, V2U, J1K, E5M, K6F, C4L, U2I, M2H, D3D, V2K, T1E, C5M, Z5A, P2D, J9Z, A4K, F9A, K3A, Q4Z, X2J, C2Q, C8D, Q9W, V2I, P2L, F3H, U3O, F2C, Z8L, Q5K, Y4X, N5K, W3R, N3E, I7V, I2U, O8I, A5X, R1V, L9H, F2G, O9G, J3Z, Q2R, D2U, P8A, Z1S, Q4T, N0C, F0P, B1X, Z9J, E0D, C1S, M0Z, V0V, A1S, Q2U, L1P, N7K, P9H, P1B, R8A, J9J, J4X, V7F, V1F, U0E, I5R, C9M, C1C, C9H, E7L, E7C, A1J, D2W, W1Q, W4L, Q8Y, U2P, Y9A, Z9E, C8G, O1V, K6X, Q8R, D2K, X2K, C4G, E5H, X9W, K1P, F6V, K7Y, Q5D, E1E, M0F, K4N, Z1F, F4G, S8E, M7K, E4C, W7L, I5X, N6R, I2M, F8M, W2P, O8U, X1Y, V1U, F3C, N8P, J3T, J3M, C1P, O8O, C3S, D6E, V7I, E4X, Z7T, I5W, X4N, F8E, D5O, F5A, N5V, D0Y, R9X, D1Z, I7W, C4E, A3C, C0Q, J1O, I7X, N9V, U2Q, W6U, S5D, D3H, M7Q, F5L, D3I, D7D, D8L, Z0K, Q1U, W7G, Z0T, S8F, X2Y, I2Q, I0U, P4A, N4B, G2B, R1D, X4C, N7E, I4E, D7J, Y1X, R5P, R6Z, Q8W, I4Y, V5Z, C6C, L2K, O1T, W5M, C7L, A5K, V1J, I4F, Q2S, K5G, D1G, N9W, W5R, J1Z, Q6X, V6Y, W4K, V5Q, A0D, V9B, V2A, G2H, K2W, P6H, J1D, X3F, D4M, A4T, Z2N, K3F, Q6R, M0L, G0Y, Z2P, W3D, O7J, Z4I, K8Z, X1P, F5N, R3Y, U8D, W0U, O4O, K5L, E0R, P5N, B4M, F2F, W2C, Y1O, E4B, R4Z, O6G, V7T, V4S, Z6A, Z3D, Q5X, N2R, P6D, J6A, R5O, R1J, A4V, I2I, W5L, E5T, G4I, Q1L, T1D, M9E, D0P, X1V, Q4L, J1T, M0T, N3C, F6D, R1B, Z4A, M9Z</t>
+          <t>Z5L, M3L, C0J, Q8T, V2U, J1K, E5M, K6F, C4L, U2I, M2H, D3D, V2K, T1E, C5M, P2D, J9Z, A4K, F9A, K3A, Q4Z, X2J, C2Q, C8D, Q9W, V2I, P2L, F3H, U3O, F2C, Z8L, Q5K, Y4X, N5K, W3R, N3E, I7V, I2U, O8I, A5X, R1V, L9H, F2G, O9G, J3Z, Q2R, D2U, P8A, Z1S, Q4T, N0C, F0P, B1X, Z9J, E0D, C1S, M0Z, V0V, A1S, Q2U, L1P, N7K, P9H, P1B, R8A, J9J, J4X, V7F, V1F, U0E, I5R, C9M, C1C, C9H, E7L, E7C, A1J, D2W, W1Q, W4L, Q8Y, U2P, Y9A, Z9E, C8G, O1V, K6X, Q8R, D2K, X2K, C4G, E5H, X9W, K1P, F6V, K7Y, Q5D, E1E, M0F, K4N, Z1F, F4G, S8E, M7K, E4C, W7L, I5X, N6R, I2M, F8M, W2P, O8U, X1Y, V1U, F3C, N8P, J3T, J3M, C1P, O8O, C3S, D6E, V7I, E4X, Z7T, I5W, X4N, F8E, D5O, F5A, N5V, D0Y, R9X, D1Z, I7W, C4E, A3C, C0Q, J1O, I7X, N9V, U2Q, W6U, S5D, D3H, M7Q, F5L, D3I, D7D, D8L, Z0K, Q1U, W7G, Z0T, S8F, X2Y, I2Q, I0U, P4A, N4B, G2B, R1D, X4C, N7E, I4E, D7J, Y1X, R5P, R6Z, Q8W, I4Y, V5Z, C6C, L2K, O1T, W5M, C7L, A5K, V1J, I4F, Q2S, K5G, D1G, N9W, W5R, J1Z, Q6X, V6Y, W4K, V5Q, A0D, V9B, V2A, G2H, K2W, P6H, J1D, X3F, D4M, A4T, Z2N, K3F, Q6R, M0L, G0Y, Z2P, W3D, O7J, Z4I, K8Z, X1P, F5N, R3Y, U8D, W0U, O4O, K5L, E0R, P5N, B4M, F2F, W2C, Y1O, E4B, R4Z, O6G, V7T, V4S, Z6A, Z3D, Q5X, N2R, P6D, J6A, R5O, R1J, A4V, I2I, W5L, E5T, G4I, Q1L, T1D, M9E, D0P, X1V, Q4L, J1T, M0T, N3C, F6D, R1B, Z4A, M9Z</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3042,7 +3090,11 @@
           <t>WDB55210210126674</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3170,7 +3222,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Z5F, M3N, A2F, V5P, V2L, B5Z, B1I, E3C, W3M, F0C, L1T, M0I, C5C, E5Z, R0R, Z2Z, L2U, I5J, F7Q, W0H, B2E, G0X, M5V, S1S, F1H, P9D, F3E, E5L, E4S, J2D, C0O, F2B, O9G, Q5Q, D2P, V3K, Q0A, Q4E, D7P, W7U, C7M, C8A, S1V, G3N, P6J, F4H, J4X, F5P, D0E, F4Z, B2A, N3K, X2H, M5A, J3S, W9Z, T2D, K6T, N8K, Z5Y, U0D, Z8U, A5I, K7E, I6J, H2H, M1B, A6N, Z4C, R2G, W7Z, Q6V, D5C, J2X, V8O, D2A, R7K, V8W, F7D, P9R, M5L, O9I, M6D, Q7U, D9C, C9U, K0D, F5Y, N0N, G3L, W7T, V3F, Q5O, F8F, P9H, B5J, E5J, O4R, Q3Y, J1G, Q2H, Z8Y, C2C, I6F, Z7Y, E5B, T0I, O5N, P8U, M9S, Y1W, Z3B, W1R, R1S, L3Z, H1M, P4Y, Q8U, O2I, E1D, F1Z, D3Q, M8U, I5Z, W2D, B2D, K5K, Q5U, V5Q, M5B, I5W, U0A, D3H, S8E, D7C, U6C, Q6Y, G0B, D1S, I4U, V1L, K5A, K3Q, D3F, Q3F, W5N, M5H, I0S, O1Q, C2R, G0K, F6C, Q6C, A5S, C4Y, J3M, Z8F, P0F, V6P, F0P, I6M, U3B, R0E, Z0R, F6X, Q4W, W5G, K7W, Z9B, W8P, P7A, C2F, P4U, U2G, Z2R, W5M, F1S, F1N, J6Y, I0C, F5T, I4M, G0A, H2G, G3X, J3T, Q1G, Q6L, O4O, K1J, W2M, W4L, D0B, Z2X, V7H, R0S, F7W, Q7I, Z0E, L2Q, W7V, C3F, W9R, K6O, B1V</t>
+          <t>Z5F, M3N, A2F, V5P, V2L, B5Z, B1I, E3C, W3M, F0C, L1T, C5C, E5Z, R0R, Z2Z, L2U, I5J, F7Q, W0H, B2E, G0X, M5V, S1S, F1H, P9D, F3E, E5L, E4S, J2D, C0O, F2B, O9G, Q5Q, D2P, V3K, Q0A, Q4E, D7P, W7U, C7M, C8A, S1V, G3N, P6J, F4H, J4X, F5P, D0E, F4Z, B2A, N3K, X2H, M5A, J3S, W9Z, T2D, K6T, N8K, Z5Y, U0D, Z8U, A5I, K7E, I6J, H2H, M1B, A6N, Z4C, R2G, W7Z, Q6V, D5C, J2X, V8O, D2A, R7K, V8W, F7D, P9R, M5L, O9I, M6D, Q7U, D9C, C9U, K0D, F5Y, N0N, G3L, W7T, V3F, Q5O, F8F, P9H, B5J, E5J, O4R, Q3Y, J1G, Q2H, Z8Y, C2C, I6F, Z7Y, E5B, T0I, O5N, P8U, M9S, Y1W, Z3B, W1R, R1S, L3Z, H1M, P4Y, Q8U, O2I, E1D, F1Z, D3Q, M8U, I5Z, W2D, B2D, K5K, Q5U, V5Q, M5B, I5W, U0A, D3H, S8E, D7C, U6C, Q6Y, G0B, D1S, I4U, V1L, K5A, K3Q, D3F, Q3F, W5N, M5H, I0S, O1Q, C2R, G0K, F6C, Q6C, A5S, C4Y, J3M, Z8F, P0F, V6P, F0P, I6M, U3B, R0E, Z0R, F6X, Q4W, W5G, K7W, Z9B, W8P, P7A, C2F, P4U, U2G, Z2R, W5M, F1S, F1N, J6Y, I0C, F5T, I4M, G0A, H2G, G3X, J3T, Q1G, Q6L, O4O, K1J, W2M, W4L, D0B, Z2X, V7H, R0S, F7W, Q7I, Z0E, L2Q, W7V, C3F, W9R, K6O, B1V</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3226,7 +3278,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Z5L, M3I, I6M, O6P, T5V, G1C, A4K, Q4T, E1U, A5I, A5W, V5P, P0E, R8D, R9A, E3F, Q4R, V2P, L1S, F6P, C0A, O7J, S5G, M7S, W6F, I3L, J3Q, Z7U, L2I, T0W, C6Q, K0P, W0U, R1I, A3D, O7E, W7J, Q1U, Q7G, R1O, D3K, L1H, Z5A, B2B, V1U, L9Y, G0D, O6R, K5U, K3Z, W3Q, Z7B, U3Y, N7O, F0M, U3V, T1R, Z3Z, W3E, K0U, W2P, M8S, N4E, W7H, V9B, J3K, I6D, U2P, W4L, B1B, J1W, J3S, M9E, F3F, J2Y, D9X, S9Y, Z2M, O3B, K7B, B5N, D4Y, V9A, N2I, D6W, L2U, F9B, I1N, E1R, I5C, E1K, R7E, D7N, P9A, F7X, K1V, Z9E, C9N, E9E, Z0D, C4F, Y1B, A4R, O1M, Z0K, Q8O, D2C, E6J, N5U, E0W, M5G, E3J, O2G, B9V, F3C, Z8F, F1R, W6O, Y1F, W4N, R2K, J2G, V2H, D4W, W6N, L2A, K1T, T5B, Z4L, C6S, A2A, W8Z, I1M, B1X, A6L, C8X, D2O, X1T, E4D, U1F, W1Z, C3S, O2P, X3G, Q4E, Q2T, I5W, V6A, B4L, Z8G, R1N, E7L, K5Y, K5V, C8V, F9C, G4C, W7A, E3B, Y1V, A4X, O7P, F6O, F3B, Q9W, S6F, D2V, G3X, J8X, Z5Q, M5N, W1S, X1M, T4A, L2K, Z2J, R6V, F9X, W3D, E1B, H1Y, Z4K, B5F, S9X, F2B, T3M, R7L, K0F, U2S, V4D, C7Q, G1H, I8Y, S5Q, Z9H, M6P, I1W, W2Q, B5C, A5B, W4C, C1Y, F7V, N0I, U1P, Z7T, P6C, A2F, D1W, Q6N, I0M, J3O, F3A, R6C, X1C, X1U, D3Y, N7F, J3Z, D5N, U3H, A4U, X1Z, P9F, N8Q, Z6E, N3B, P7Y, T1K, C2P, N4G, V3K, C5R, J5S, C6A, Q7Z, W4U, Z4Q, W2Y, P5E, P0R, C1N, Z1W, O1X, P2I, C9M, N1G, E1D, N1Y, D5J, X1Q, W1Q, F1E, Q7H, W8Y, C5J, R2P, J3A, I9H, X2H, J8Y, D9N, V7G, W4S, V7W, V7B, U2M, F9L, J1K, T2A, R2R, A5F, M0H, O7D, V0Z, C1K</t>
+          <t>Z5L, M3I, I6M, O6P, T5V, G1C, A4K, Q4T, E1U, A5I, A5W, V5P, P0E, R8D, R9A, E3F, Q4R, V2P, L1S, F6P, C0A, O7J, S5G, M7S, W6F, I3L, J3Q, Z7U, L2I, T0W, C6Q, K0P, W0U, R1I, A3D, O7E, W7J, Q1U, Q7G, R1O, D3K, L1H, B2B, V1U, L9Y, G0D, O6R, K5U, K3Z, W3Q, Z7B, U3Y, N7O, F0M, U3V, T1R, Z3Z, W3E, K0U, W2P, M8S, N4E, W7H, V9B, J3K, I6D, U2P, W4L, B1B, J1W, J3S, M9E, F3F, J2Y, D9X, S9Y, Z2M, O3B, K7B, B5N, D4Y, V9A, N2I, D6W, L2U, F9B, I1N, E1R, I5C, E1K, R7E, D7N, P9A, F7X, K1V, Z9E, C9N, E9E, Z0D, C4F, Y1B, A4R, O1M, Z0K, Q8O, D2C, E6J, N5U, E0W, M5G, E3J, O2G, B9V, F3C, Z8F, F1R, W6O, Y1F, W4N, R2K, J2G, V2H, D4W, W6N, L2A, K1T, T5B, Z4L, C6S, A2A, W8Z, I1M, B1X, A6L, C8X, D2O, X1T, E4D, U1F, W1Z, C3S, O2P, X3G, Q4E, Q2T, I5W, V6A, B4L, Z8G, R1N, E7L, K5Y, K5V, C8V, F9C, G4C, W7A, E3B, Y1V, A4X, O7P, F6O, F3B, Q9W, S6F, D2V, G3X, J8X, Z5Q, M5N, W1S, X1M, T4A, L2K, Z2J, R6V, F9X, W3D, E1B, H1Y, Z4K, B5F, S9X, F2B, T3M, R7L, K0F, U2S, V4D, C7Q, G1H, I8Y, S5Q, Z9H, M6P, I1W, W2Q, B5C, A5B, W4C, C1Y, F7V, N0I, U1P, Z7T, P6C, A2F, D1W, Q6N, I0M, J3O, F3A, R6C, X1C, X1U, D3Y, N7F, J3Z, D5N, U3H, A4U, X1Z, P9F, N8Q, Z6E, N3B, P7Y, T1K, C2P, N4G, V3K, C5R, J5S, C6A, Q7Z, W4U, Z4Q, W2Y, P5E, P0R, C1N, Z1W, O1X, P2I, C9M, N1G, E1D, N1Y, D5J, X1Q, W1Q, F1E, Q7H, W8Y, C5J, R2P, J3A, I9H, X2H, J8Y, D9N, V7G, W4S, V7W, V7B, U2M, F9L, J1K, T2A, R2R, A5F, M0H, O7D, V0Z, C1K</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3234,7 +3286,11 @@
           <t>NMB19508764326332</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3306,7 +3362,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Z5D, M2Q, W4I, Z0G, R6S, Y4W, O8L, Q8T, Q4L, C5G, Z6M, N8I, P4A, E3A, N5U, G0N, Z2Q, Z5T, K3A, P1K, C4G, Q2X, V6X, Q4G, N2R, J5S, Z0U, G4C, H2B, P2G, I5B, I0C, Y9W, P5A, Z4Y, P9K, Q7W, N8D, N7G, D6I, B5J, B5F, P8T, W6V, K7Q, N5Y, W3W, N3S, E0U, U3Y, K6V, P5Y, M6M, A9Y, Q7C, Q1D, D6Z, F8I, D4X, Z2H, L9I, Y3K, J4A, V5V, Z3Z, V2S, Z2U, R2J, D3A, I9J, F2U, C5H, Z7N, V9B, F2W, L9H, Q7V, I1Y, J2Z, G3H, I5T, C2F, W5G, Z8I, E2L, K7D, O4A, W3P, X9V, R1S, N9V, J9Y, W7L, W9P, E0Y, F7A, U2P, E5C, Y4G, F4H, R8H, M0X, E0X, O1S, Y9V, I6F, F3P, D4L, Z5A, Q5A, R5Y, E0K, I2C, N4Y, M9V, I4F, I2D, K7J, V1O, C5B, I1T, W7N, F2B, I0M, A1C, Y4X, J2H, B2C, F3E, F8B, Q6A, Z3P, Z8Y, Y1D, X6A, B2E, R0V, N3G, F8A, W1E, K5N, O6N, P6M, W2C, R2E, F9R, F7E, Z5K, Z6N, B1E, Q2J, D3I, V1U, A5N, Z8G, C0O, P8B, S1I, Q4H, J1C, W0G, C3M, X3Z, W7Y, E0Z, F6P, H2I, Z2F, X2P, R1Y, R5S, J8W, E6M, A4U, C7G, J2D, N0X, N3T, Z0M, Z9W, J1Z, N6U, J3M, H8N, C5C, W0Y, A4A, K7Z, T1T, R7D, R1P, U1A, D3T, O2K, A6A, D9G, Z4V, D6X, O8A, V1D, Z8C, O1Y, R0T, K5R, P9P, O7E, D0D, O4H, T0Z, J4V, D0Y, F0O, T0K, Q1O, X2Z, E1I, F6A, Q4W, F0B, V8A, Y6J, V8Y, K2E, Z9A, M5H, O8M, L9V, D0E, W3T, K6H, R6C, J3V, W3G, M0J, V7W, C6G, D0K, Q3B, P2M, O1D, Q7O, N1A, F5Y, R4W, V6H, I6T, X1N, D1X, D9T, D6C, K7L, D5U, X1L, A5R, M4Y, X2C, D7Z, F9A, Y4P, F1V, T5A, Z4X, X3X, C2V, O6B, C6O, U5B, D7K, I5C, W9Q, W2H, Z4K, K6R, F0A, C1Y, A5S, U3E, G4Z, Z4E, V6Z, E4Z</t>
+          <t>Z5D, M2Q, W4I, Z0G, R6S, Y4W, O8L, Q8T, Q4L, C5G, Z6M, N8I, P4A, E3A, N5U, G0N, Z2Q, Z5T, K3A, P1K, C4G, Q2X, V6X, Q4G, N2R, J5S, Z0U, G4C, H2B, P2G, I5B, I0C, Y9W, P5A, Z4Y, P9K, Q7W, N8D, N7G, D6I, B5J, B5F, P8T, W6V, K7Q, N5Y, W3W, N3S, E0U, U3Y, K6V, P5Y, M6M, A9Y, Q7C, Q1D, D6Z, F8I, D4X, Z2H, L9I, Y3K, J4A, V5V, Z3Z, V2S, Z2U, R2J, D3A, I9J, F2U, C5H, Z7N, V9B, F2W, L9H, Q7V, I1Y, J2Z, G3H, I5T, C2F, W5G, Z8I, E2L, K7D, O4A, W3P, X9V, R1S, N9V, J9Y, W7L, W9P, E0Y, F7A, U2P, E5C, Y4G, F4H, R8H, M0X, E0X, O1S, Y9V, I6F, F3P, D4L, Q5A, R5Y, E0K, I2C, N4Y, M9V, I4F, I2D, K7J, V1O, C5B, I1T, W7N, F2B, I0M, A1C, Y4X, J2H, B2C, F3E, F8B, Q6A, Z3P, Z8Y, Y1D, X6A, B2E, R0V, N3G, F8A, W1E, K5N, O6N, P6M, W2C, R2E, F9R, F7E, Z5K, Z6N, B1E, Q2J, D3I, V1U, A5N, Z8G, C0O, P8B, S1I, Q4H, J1C, W0G, C3M, X3Z, W7Y, E0Z, F6P, H2I, Z2F, X2P, R1Y, R5S, J8W, E6M, A4U, C7G, J2D, N0X, N3T, Z0M, Z9W, J1Z, N6U, J3M, H8N, C5C, W0Y, A4A, K7Z, T1T, R7D, R1P, U1A, D3T, O2K, A6A, D9G, Z4V, D6X, O8A, V1D, Z8C, O1Y, R0T, K5R, P9P, O7E, D0D, O4H, T0Z, J4V, D0Y, F0O, T0K, Q1O, X2Z, E1I, F6A, Q4W, F0B, V8A, Y6J, V8Y, K2E, Z9A, M5H, O8M, L9V, D0E, W3T, K6H, R6C, J3V, W3G, V7W, C6G, D0K, Q3B, P2M, O1D, Q7O, N1A, F5Y, R4W, V6H, I6T, X1N, D1X, D9T, D6C, K7L, D5U, X1L, A5R, M4Y, X2C, D7Z, F9A, Y4P, F1V, T5A, Z4X, X3X, C2V, O6B, C6O, U5B, D7K, I5C, W9Q, W2H, Z4K, K6R, F0A, C1Y, A5S, U3E, G4Z, Z4E, V6Z, E4Z</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3454,7 +3510,11 @@
           <t>WDB15074727389501</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3478,7 +3538,11 @@
           <t>NMB91532838482279</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr"/>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3502,7 +3566,11 @@
           <t>WDB82620166664538</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3546,7 +3614,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Z5F, M3V, K5J, E3S, N5U, F7Z, D5P, K2A, L1S, C2H, D0P, A5M, D7M, E3Q, Z4O, Q8Q, N0S, B1C, M0J, U2I, C5H, G4H, R0T, X1K, A5K, W5R, C9V, V6A, K0B, Q1B, C4C, R2M, U3G, K1N, U7L, Q2M, D6Z, E4S, R2W, A4W, G0D, C2R, A2I, Z0G, T2K, X3Z, A6F, E4Z, J9I, W7I, Q5T, M0L, K7E, G1I, E7L, C1N, Q3F, S9X, X3P, Q7C, R5I, E7C, U5A, F3B, Z8W, W0R, Q6R, Z3X, E9H, J2B, E1J, N1J, R5Q, L3C, G0B, B2D, Z3F, C3Q, W8F, D4T, D8U, W1U, Z2U, Q1H, Q5N, F1N, O2S, E5L, C0W, K5Y, C0M, K7N, C6Y, W0F, V7S, I4U, N1T, D8N, N7M, P5Y, Y9Z, V7P, R7L, R1J, E3K, D9X, Z3Y, Z7O, K0I, Z1P, A6L, C0S, C5O, C7I, Q7B, O8U, F2Z, V3A, E1K, E2M, G4D, B1H, M5V, W6Y, I9I, C2Y, Z5G, Q2K, Z8V, I2P, X3V, O1E, S9Z, T2B, P9D, P2W, P8E, N4W, A2Z, I9H, N1U, J8Y, D5W, W5Q, M5S, F1F, A1L, F0G, O3A, R5O, U3I, O6Y, D1K, W2Y, O4C, F9Y, H2G, U0D, B5K, Z4L, G2G, F3P, C5Q, J9H, H2D, T2C, Z2Z, K0S, K1I, Z8I, M7Q, O1H, O9G, I6J, O8N, O9I, V2S, Q7R, D7V, C6T, L2A, W7A, N9V, I2N, M7V, O7Q, X4H, J2E, I3O, O7B, D8M, Q0H, Z0P, O2Q, Z7Q, Y1B, K2X, Z9I, Q2J, R1W, J9C, H8T, G3N, C2F, U6D, B4M, C2I, P9T, X1J, Z4T, E3V, O1T, F9Q, K2P, B1G, Z8K, J1D, K1A, Z0M, D1U, O1V, I1F, Q3E, F5Z, V5Q, N6R, Q5X, Y1K, C2A, P2J, M6B, M5L, R6Z, F8D, F2G, D0R, D2U, I1V, L4B, O2F, T1X, Z4U, E2A, P6M, N8M, E6Y, P8Z, F8W, C6U, F2V, W0Y, E5A, G4E</t>
+          <t>Z5F, M3V, K5J, E3S, N5U, F7Z, D5P, K2A, L1S, C2H, D0P, A5M, D7M, E3Q, Z4O, Q8Q, N0S, B1C, U2I, C5H, G4H, R0T, X1K, A5K, W5R, C9V, V6A, K0B, Q1B, C4C, R2M, U3G, K1N, U7L, Q2M, D6Z, E4S, R2W, A4W, G0D, C2R, A2I, Z0G, T2K, X3Z, A6F, E4Z, J9I, W7I, Q5T, M0L, K7E, G1I, E7L, C1N, Q3F, S9X, X3P, Q7C, R5I, E7C, U5A, F3B, Z8W, W0R, Q6R, Z3X, E9H, J2B, E1J, N1J, R5Q, L3C, G0B, B2D, Z3F, C3Q, W8F, D4T, D8U, W1U, Z2U, Q1H, Q5N, F1N, O2S, E5L, C0W, K5Y, C0M, K7N, C6Y, W0F, V7S, I4U, N1T, D8N, N7M, P5Y, Y9Z, V7P, R7L, R1J, E3K, D9X, Z3Y, Z7O, K0I, Z1P, A6L, C0S, C5O, C7I, Q7B, O8U, F2Z, V3A, E1K, E2M, G4D, B1H, M5V, W6Y, I9I, C2Y, Z5G, Q2K, Z8V, I2P, X3V, O1E, S9Z, T2B, P9D, P2W, P8E, N4W, A2Z, I9H, N1U, J8Y, D5W, W5Q, M5S, F1F, A1L, F0G, O3A, R5O, U3I, O6Y, D1K, W2Y, O4C, F9Y, H2G, U0D, B5K, Z4L, G2G, F3P, C5Q, J9H, H2D, T2C, Z2Z, K0S, K1I, Z8I, M7Q, O1H, O9G, I6J, O8N, O9I, V2S, Q7R, D7V, C6T, L2A, W7A, N9V, I2N, M7V, O7Q, X4H, J2E, I3O, O7B, D8M, Q0H, Z0P, O2Q, Z7Q, Y1B, K2X, Z9I, Q2J, R1W, J9C, H8T, G3N, C2F, U6D, B4M, C2I, P9T, X1J, Z4T, E3V, O1T, F9Q, K2P, B1G, Z8K, J1D, K1A, Z0M, D1U, O1V, I1F, Q3E, F5Z, V5Q, N6R, Q5X, Y1K, C2A, P2J, M6B, M5L, R6Z, F8D, F2G, D0R, D2U, I1V, L4B, O2F, T1X, Z4U, E2A, P6M, N8M, E6Y, P8Z, F8W, C6U, F2V, W0Y, E5A, G4E</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3582,7 +3650,11 @@
           <t>W1T65408549768006</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -3598,7 +3670,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Z5E, M3D, A5D, H1M, O1N, D2O, K8Y, K7I, J2G, W0H, I6I, R3Q, P1N, W2L, C0B, R7D, P9E, T0N, K4Z, K5P, U7G, V3K, P6L, Z0D, X3Q, K0N, A1F, L4C, R1C, Z2C, Q6L, U8D, U6A, Y1T, O7A, T1E, L0U, C6E, N8K, M0S, D7V, F7S, Z9K, F6Y, B1C, W5V, E5M, K6N, I4K, W3G, Z7B, N8P, U6E, G3Y, K1O, R8B, C2H, C4P, Y6D, P9A, L9G, J1D, P2T, Z9G, L1T, E4I, Q1J, T4A, T0Q, V2V, H8T, L9W, Q3D, P7U, E9L, C9N, D3W, K2J, Q8U, L4B, C4I, C8R, N8B, Z3D, U2L, F0S, W6R, Y1R, W7D, E9D, I4I, Z3N, C5U, B3K, V7Q, V7V, V7B, C5D, F0P, R1B, M0D, R2J, C9H, E3M, I5S, S5G, M1A, C3J, E3Z, X1E, G5Z, A6R, N4E, J6A, E2J, C8F, F2E, I2F, D7R, Q5V, Z5A, J9Y, E1W, Y1H, J9A, M5B, E1E, C0Z, W9G, I6Y, Z9B, K6L, P8F, T3N, V1W, N3U, H8W, A4U, F8V, P6G, Z2K, Q7H, Y3M, N4A, K6R, N6I, K6O, T0F, N5D, T1W, Z5N, P9R, D5Z, U8C, X1F, C8E, X3Z, C2T, W2T, J1X, D2W, T0J, M9Y, R5O, J3C, D6J, C7N, D4T, K3R, M5O, Z0J, F7E, A5F, V2B, Z1P, C6K, K0W, Z6M, O6R, Q8E, J9S, X3F, E1P, P6M, D9W, F1P, V6W, C6T, W1N, F7T, S1M, D3D, Q2O, E7B, B2D, J3I, Z1S, Z0P, G3B, B1I, Z9W, Q5T, M8Z, K1T, Q5R, Q7U, T1B, K6X, A2P, N9V, Y1Y, I9I, U0D, Q6Q, B4L, K3Q, N1A, B5F, E1J, Z3K, N2I, R4Y, R6M, L2N, E6E, F0E, U8A, J1E, G1E, A4Q, N4L, N3A, F0W, G4D, Z8K, Z4N, D1V, L1B, O2Q, Z3A, R1D, H1Q, R2K, O4C, C7C, H1H, E5F, Z7S, X0Z</t>
+          <t>Z5E, M3D, A5D, H1M, O1N, D2O, K8Y, K7I, J2G, W0H, I6I, R3Q, P1N, W2L, C0B, R7D, P9E, T0N, K4Z, K5P, U7G, V3K, P6L, Z0D, X3Q, K0N, A1F, L4C, R1C, Z2C, Q6L, U8D, U6A, Y1T, O7A, T1E, L0U, C6E, N8K, M0S, D7V, F7S, Z9K, F6Y, B1C, W5V, E5M, K6N, I4K, W3G, Z7B, N8P, U6E, G3Y, K1O, R8B, C2H, C4P, Y6D, P9A, L9G, J1D, P2T, Z9G, L1T, E4I, Q1J, T4A, T0Q, V2V, H8T, L9W, Q3D, P7U, E9L, C9N, D3W, K2J, Q8U, L4B, C4I, C8R, N8B, Z3D, U2L, F0S, W6R, Y1R, W7D, E9D, I4I, Z3N, C5U, B3K, V7Q, V7V, V7B, C5D, F0P, R1B, M0D, R2J, C9H, E3M, I5S, S5G, M1A, C3J, E3Z, X1E, G5Z, A6R, N4E, J6A, E2J, C8F, F2E, I2F, D7R, Q5V, J9Y, E1W, Y1H, J9A, M5B, E1E, C0Z, W9G, I6Y, Z9B, K6L, P8F, T3N, V1W, N3U, H8W, A4U, F8V, P6G, Z2K, Q7H, Y3M, N4A, K6R, N6I, K6O, T0F, N5D, T1W, Z5N, P9R, D5Z, U8C, X1F, C8E, X3Z, C2T, W2T, J1X, D2W, T0J, M9Y, R5O, J3C, D6J, C7N, D4T, K3R, M5O, Z0J, F7E, A5F, V2B, Z1P, C6K, K0W, Z6M, O6R, Q8E, J9S, X3F, E1P, P6M, D9W, F1P, V6W, C6T, W1N, F7T, S1M, D3D, Q2O, E7B, B2D, J3I, Z1S, Z0P, G3B, B1I, Z9W, Q5T, M8Z, K1T, Q5R, Q7U, T1B, K6X, A2P, N9V, Y1Y, I9I, U0D, Q6Q, B4L, K3Q, N1A, B5F, E1J, Z3K, N2I, R4Y, R6M, L2N, E6E, F0E, U8A, J1E, G1E, A4Q, N4L, N3A, F0W, G4D, Z8K, Z4N, D1V, L1B, O2Q, Z3A, R1D, H1Q, R2K, O4C, C7C, H1H, E5F, Z7S, X0Z</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3682,7 +3754,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Z5D, M2Q, F9A, C2Z, V7K, K9Z, R5P, C3L, F8A, A0H, E5D, W1Q, V2T, T2C, I6J, I2V, U3L, Z8K, K5M, A2T, W4H, K0Q, D4Q, N3L, V8R, Q4N, P6Y, F9W, Q3C, X2J, H2F, A6M, M9T, V2F, F9L, K1A, Q8G, M7T, E0D, T2S, N4G, C1M, E2T, F3W, R8N, F8Z, Q4P, E6H, Q2N, D6G, E3R, D9T, E1T, V6H, D3T, V1M, D5C, F6I, L2L, W9F, G2H, K1D, S1I, S8E, X1W, M7J, X2V, K4L, O4H, A1P, Z8A, Z2Y, N7C, D5B, N2G, X3U, F1O, K3E, D5Z, C9L, L2Q, U3A, K4V, R3K, Z0H, F1F, O1C, X3I, Z0F, A5P, O8K, Q6M, P8Z, Z8O, Z1W, A4V, G4B, Q8Z, T2F, T2R, O7B, F6Y, Q8M, C5F, Q2S, Z3X, U3H, D3O, Q7L, F2N, B4L, K1X, U2I, F9Z, F0B, J3K, N5H, Z4W, M0C, V1D, O2Q, C9H, V6C, A2Z, R1H, Q1X, Q0X, M5M, Q6J, K5E, T1C, C5C, E7B, C7G, X2Z, C6B, P6C, E5W, T1Q, E1I, F2Q, C8W, O8O, P9P, L9V, E9D, D9R, I6Z, A1M, K2E, F2W, S9X, V6P, A4X, X2K, R9Y, V7S, E2M, A2G, D0Q, U3O, D7N, Z2Q, F0G, J3A, G1H, T1D, F0I, H2H, R6C, K5O, D4Y, C6A, A5W, O3A, U8D, O7R, N0E, C3G, W3Z, F5E, P7S, A4P, Z2F, Q6G, G1C, Y1C, Y3I, P8E, A5F, W9H, D3F, Z5O, O1E, Q5R, E9F, Y1B, A2J, F5Q, O8D, Z7I, W0K, A4R, F0S, I7T, J9I, P5A, P0R, Z4P, T3Q, I4R, N7A, C4E, D7K, M1B, K5J, J1P, K0I, C5D, D7F, A2M, D4S, J1K, N0M, D0P, M5Y, D6Z, N8H, Q2B, P5Z, L9G, U1P, C4M, C7D, D1G, R1V, M7R, Z6S, R4Y, D5W, P0X, C5T, D7G, B2B, E0F, M8T, J8Y, E4F, I4G, M7F, O1X, N3N, I1P, W5I, Y3E, G5Y, F8D, W5Q, R1O, C1Z, W2B, I4I, W3C, W7G, J9C, K2B, Z4H, K3V, I2Q, C8R, L2J, O8T, J4A, W1P, A6S, B5I, M0I</t>
+          <t>Z5D, M2Q, F9A, C2Z, V7K, K9Z, R5P, C3L, F8A, A0H, E5D, W1Q, V2T, T2C, I6J, I2V, U3L, Z8K, K5M, A2T, W4H, K0Q, D4Q, N3L, V8R, Q4N, P6Y, F9W, Q3C, X2J, H2F, A6M, M9T, V2F, F9L, K1A, Q8G, M7T, E0D, T2S, N4G, C1M, E2T, F3W, R8N, F8Z, Q4P, E6H, Q2N, D6G, E3R, D9T, E1T, V6H, D3T, V1M, D5C, F6I, L2L, W9F, G2H, K1D, S1I, S8E, X1W, M7J, X2V, K4L, O4H, A1P, Z8A, Z2Y, N7C, D5B, N2G, X3U, F1O, K3E, D5Z, C9L, L2Q, U3A, K4V, R3K, Z0H, F1F, O1C, X3I, Z0F, A5P, O8K, Q6M, P8Z, Z8O, Z1W, A4V, G4B, Q8Z, T2F, T2R, O7B, F6Y, Q8M, C5F, Q2S, Z3X, U3H, D3O, Q7L, F2N, B4L, K1X, U2I, F9Z, F0B, J3K, N5H, Z4W, M0C, V1D, O2Q, C9H, V6C, A2Z, R1H, Q1X, Q0X, M5M, Q6J, K5E, T1C, C5C, E7B, C7G, X2Z, C6B, P6C, E5W, T1Q, E1I, F2Q, C8W, O8O, P9P, L9V, E9D, D9R, I6Z, A1M, K2E, F2W, S9X, V6P, A4X, X2K, R9Y, V7S, E2M, A2G, D0Q, U3O, D7N, Z2Q, F0G, J3A, G1H, T1D, F0I, H2H, R6C, K5O, D4Y, C6A, A5W, O3A, U8D, O7R, N0E, C3G, W3Z, F5E, P7S, A4P, Z2F, Q6G, G1C, Y1C, Y3I, P8E, A5F, W9H, D3F, Z5O, O1E, Q5R, E9F, Y1B, A2J, F5Q, O8D, Z7I, W0K, A4R, F0S, I7T, J9I, P5A, P0R, Z4P, T3Q, I4R, N7A, C4E, D7K, M1B, K5J, J1P, K0I, C5D, D7F, A2M, D4S, J1K, N0M, D0P, M5Y, D6Z, N8H, Q2B, P5Z, L9G, U1P, C4M, C7D, D1G, R1V, M7R, Z6S, R4Y, D5W, P0X, C5T, D7G, B2B, E0F, M8T, J8Y, E4F, I4G, M7F, O1X, N3N, I1P, W5I, Y3E, G5Y, F8D, W5Q, R1O, C1Z, W2B, I4I, W3C, W7G, J9C, K2B, Z4H, K3V, I2Q, C8R, L2J, O8T, J4A, W1P, A6S, B5I</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3746,7 +3818,11 @@
           <t>W1T14104931218774</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr"/>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -3798,7 +3874,11 @@
           <t>W1T59495989046715</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr"/>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -3962,7 +4042,11 @@
           <t>NMB97518139456297</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr"/>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3978,7 +4062,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Z5C, M2E, I0K, W5X, V7I, Q2P, Q6J, U1W, E1C, Y2A, S8H, D7E, Q3A, Q1Y, P8A, Z0E, K7Y, P0T, U8X, D1C, K1M, D6J, Z0D, Z3O, N5Z, W6X, V2B, S5I, D6Z, N5I, W1E, E9G, Z5W, E4C, G5H, X9V, A2Z, A5M, E6A, K4N, X2K, W2B, Z5P, X2M, Z1S, P1B, Y4F, P0D, Y1A, F5N, F8I, X4M, K7Z, A1W, Q0B, V7K, D6R, C2Q, C6T, E6K, R2Y, W6M, J1V, F3C, M7S, Y4D, F6G, K3C, R7K, Q5R, P6R, M5K, F9Y, Y1B, S1H, D3F, H2H, G9B, Q8B, D6I, I8H, A1K, R5Z, I5R, X4L, K6D, R5W, H1P, M5B, R6V, D3W, D3Q, D3Y, I6H, C7J, C0Q, P5G, W3P, G2G, T2K, V3K, C4K, X3A, C5U, R5I, M8Y, V4Y, X1T, L2I, E2R, Y9C, Y1V, T3Q, C3J, M0J, F8X, U3F, R2D, O3C, F1H, T0V, F0A, G1B, P2I, V5S, E3J, S1E, T2U, V3F</t>
+          <t>Z5C, M2E, I0K, W5X, V7I, Q2P, Q6J, U1W, E1C, Y2A, S8H, D7E, Q3A, Q1Y, P8A, Z0E, K7Y, P0T, U8X, D1C, K1M, D6J, Z0D, Z3O, N5Z, W6X, V2B, S5I, D6Z, N5I, W1E, E9G, Z5W, E4C, G5H, X9V, A2Z, A5M, E6A, K4N, X2K, W2B, Z5P, X2M, Z1S, P1B, Y4F, P0D, Y1A, F5N, F8I, X4M, K7Z, A1W, Q0B, V7K, D6R, C2Q, C6T, E6K, R2Y, W6M, J1V, F3C, M7S, Y4D, F6G, K3C, R7K, Q5R, P6R, M5K, F9Y, Y1B, S1H, D3F, H2H, G9B, Q8B, D6I, I8H, A1K, R5Z, I5R, X4L, K6D, R5W, H1P, M5B, R6V, D3W, D3Q, D3Y, I6H, C7J, C0Q, P5G, W3P, G2G, T2K, V3K, C4K, X3A, C5U, R5I, M8Y, V4Y, X1T, L2I, E2R, Y9C, Y1V, T3Q, C3J, F8X, U3F, R2D, O3C, F1H, T0V, F0A, G1B, P2I, V5S, E3J, S1E, T2U, V3F</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -4090,7 +4174,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Z5C, M2D, E5Z, S9Z, M0U, U6E, Y3K, N2G, D8L, M8N, N8P, E7L, A4F, P2F, Z7Q, R8C, O7R, C3A, C5A, Q8G, W2N, R2P, F7S, G4Z, W2X, L9E, X1U, T2N, I0C, K1P, A6I, G0G, X3T, W8M, Z3U, I7T, R5M, E3R, F6L, T1T, Q1A, P0Z, X1L, C8V, C1X, I6H, W2W, M0W, O6B, F3G, N7N, I0Y, Z1O, F1J, P6H, C1P, J1T, R2D, K7A, Q4Y, A5X, T1M, Q4F, Q3W, X4G, V6Q, P2D, U2M, Q4A, D3X, X1D, H2I, F6F, A0D, P6I, C3L, I5H, J9I, N1N, L1T, U3Q, I0M, Q2L, J1R, J2U, D3C, J3J, K2U, V8B, W5R, K3Y, E3A, I4Y, X9D, I9J, C7A, P9B, X4I, S1W, E4X, D6H, P0R, X9W, Q6X, L3A, A5Y, Q1Q, V2I, L1L, W1N, R1V, W2J, H1X, B1A, C1N, R3K, T2L, I3D, I2Z, A4W, B1X, R8H, F0X, E0E, A9Y, T1V, P5X, M9Z, K2X, B2Z, X3W, R9Z, Z5A, F3S, M8B, F8X, D9Y, Q0W, P5P, O1S, C7K, O8J, F7Z, O2H, N8M, I6C, D5M, P1J, F7C, T1Y, P0Y, Z4X, U0A, D3O, S5S, K2N, Q6Q, D7I, A2Q, E0C, Q5X, L3D, W8F</t>
+          <t>Z5C, M2D, E5Z, S9Z, M0U, U6E, Y3K, N2G, D8L, M8N, N8P, E7L, A4F, P2F, Z7Q, R8C, O7R, C3A, C5A, Q8G, W2N, R2P, F7S, G4Z, W2X, L9E, X1U, T2N, I0C, K1P, A6I, G0G, X3T, W8M, Z3U, I7T, R5M, E3R, F6L, T1T, Q1A, P0Z, X1L, C8V, C1X, I6H, W2W, M0W, O6B, F3G, N7N, I0Y, Z1O, F1J, P6H, C1P, J1T, R2D, K7A, Q4Y, A5X, T1M, Q4F, Q3W, X4G, V6Q, P2D, U2M, Q4A, D3X, X1D, H2I, F6F, A0D, P6I, C3L, I5H, J9I, N1N, L1T, U3Q, I0M, Q2L, J1R, J2U, D3C, J3J, K2U, V8B, W5R, K3Y, E3A, I4Y, X9D, I9J, C7A, P9B, X4I, S1W, E4X, D6H, P0R, X9W, Q6X, L3A, A5Y, Q1Q, V2I, L1L, W1N, R1V, W2J, H1X, B1A, C1N, R3K, T2L, I3D, I2Z, A4W, B1X, R8H, F0X, E0E, A9Y, T1V, P5X, M9Z, K2X, B2Z, X3W, R9Z, F3S, M8B, F8X, D9Y, Q0W, P5P, O1S, C7K, O8J, F7Z, O2H, N8M, I6C, D5M, P1J, F7C, T1Y, P0Y, Z4X, U0A, D3O, S5S, K2N, Q6Q, D7I, A2Q, E0C, Q5X, L3D, W8F</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -4230,7 +4314,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Z5F, M3V, O2G, W6Q, K8A, Q6X, D4Q, G3E, C4X, Q5G, U0C, W6M, C1K, V2B, L3C, Z1U, D6Z, Z0I, W4J, R8H, D2C, Z1O, F4G, V0T, Z1C, C4M, H8W, O1D, R8B, E2E, W6W, M9A, R7E, E3E, F5D, T2R, D6E, M7V, G4Z, E2I, Q7X, W0V, A2Q, F7B, J3U, X1O, I1N, R1Z, V2K, F8H, A5M, A1Y, W7D, E1Z, K1H, Q6K, E9H, K6E, Z5N, A6C, I5E, T2Z, D3Y, V8A, M0H, K1S, U2I, Q1W, N9S, G0Y, J3K, D1I, A1O, R8O, D5C, Z0U, F1Z, V5A, C8J, Y1H, V6P, F9C, Q4B, W3F, C7S, F8W, F8L, W4L, N5N, W7R, A6B, P2K, R2T, F6X, F5Q, H1I, Q6G, O6P, Z4S, C4Y, O1T, A6M, M8S, D5O, R1C, U3D, W7X, J9Z, J1C, R6Z, Y1W, H2F, U3Y, P5A, W9J, U6C, O8I, Z7V, F0T, Z3A, E3C, W6N, S5B, C6V, H1J, N8D, I0Y, V5S, E6I, A4K, D9Z, D3E, Z0R, F0B, H1W, X1Y, U3V, Z2W, Q9Y, Y1F, K0Q, Y1U, C2U, W1A, K3Z, Q5H, M0I, V2J, A0H, Z1M, P0A, P8C, K1F, Z1I, I4E, N2F, O6B, K3W, Y3I, F3Z, V1B, Z8J, C7B, K2A, W2D, V2U, J1V, F1C, V7O, Q7F, K3V, D8A, P6Y, P6A, V1L, P5Y, Y4O, K5P, D1J, N5F, B4Z, Q6Y, M5T, Z9M, N5U, Z4I, N4X, D9N, Z2J, K2E, J1X, K4E, I4M, A4L, G1M, D5J, W6C, R2Q, K6L, Q1Q, Z3Q, Z6K, C7Z, E5F, Q1A, D2O, Z3J, D7K, T1Q, F8N, C8X, Q1S, V6V, Q5V, J9P, P4Y, H2J, R2N, I4C, R1L, N3L, P2I, N6R, C4G, B1I, Z1Q, W7E, P2H, C4B, K7N, K6B, P2C, W5Q, E0Y, J4X, L1P, R2J, P6Z, N5H, F6Y, N1A, C7C, U3L, S5A, O4P, K6R, D6X, A5P, H8T, W8Y, V0U, I9Y, C2L, K0I, I2B, U7G, D2V, Z2X, K2K, K3Q, X2S, V6E, O5M, R6T, W3G, I7G, Z5X, Y9W, V8Q, V6D, E5W, G1H, R7K, W7S</t>
+          <t>Z5F, M3V, O2G, W6Q, K8A, Q6X, D4Q, G3E, C4X, Q5G, U0C, W6M, C1K, V2B, L3C, Z1U, D6Z, Z0I, W4J, R8H, D2C, Z1O, F4G, V0T, Z1C, C4M, H8W, O1D, R8B, E2E, W6W, M9A, R7E, E3E, F5D, T2R, D6E, M7V, G4Z, E2I, Q7X, W0V, A2Q, F7B, J3U, X1O, I1N, R1Z, V2K, F8H, A5M, A1Y, W7D, E1Z, K1H, Q6K, E9H, K6E, Z5N, A6C, I5E, T2Z, D3Y, V8A, M0H, K1S, U2I, Q1W, N9S, G0Y, J3K, D1I, A1O, R8O, D5C, Z0U, F1Z, V5A, C8J, Y1H, V6P, F9C, Q4B, W3F, C7S, F8W, F8L, W4L, N5N, W7R, A6B, P2K, R2T, F6X, F5Q, H1I, Q6G, O6P, Z4S, C4Y, O1T, A6M, M8S, D5O, R1C, U3D, W7X, J9Z, J1C, R6Z, Y1W, H2F, U3Y, P5A, W9J, U6C, O8I, Z7V, F0T, Z3A, E3C, W6N, S5B, C6V, H1J, N8D, I0Y, V5S, E6I, A4K, D9Z, D3E, Z0R, F0B, H1W, X1Y, U3V, Z2W, Q9Y, Y1F, K0Q, Y1U, C2U, W1A, K3Z, Q5H, V2J, A0H, Z1M, P0A, P8C, K1F, Z1I, I4E, N2F, O6B, K3W, Y3I, F3Z, V1B, Z8J, C7B, K2A, W2D, V2U, J1V, F1C, V7O, Q7F, K3V, D8A, P6Y, P6A, V1L, P5Y, Y4O, K5P, D1J, N5F, B4Z, Q6Y, M5T, Z9M, N5U, Z4I, N4X, D9N, Z2J, K2E, J1X, K4E, I4M, A4L, G1M, D5J, W6C, R2Q, K6L, Q1Q, Z3Q, Z6K, C7Z, E5F, Q1A, D2O, Z3J, D7K, T1Q, F8N, C8X, Q1S, V6V, Q5V, J9P, P4Y, H2J, R2N, I4C, R1L, N3L, P2I, N6R, C4G, B1I, Z1Q, W7E, P2H, C4B, K7N, K6B, P2C, W5Q, E0Y, J4X, L1P, R2J, P6Z, N5H, F6Y, N1A, C7C, U3L, S5A, O4P, K6R, D6X, A5P, H8T, W8Y, V0U, I9Y, C2L, K0I, I2B, U7G, D2V, Z2X, K2K, K3Q, X2S, V6E, O5M, R6T, W3G, I7G, Z5X, Y9W, V8Q, V6D, E5W, G1H, R7K, W7S</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -4342,7 +4426,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Z5B, M1I, Q5N, C0G, J2C, W1R, C7S, Y1C, X0A, K1C, W3W, C9Z, P6A, Q3A, D9C, Z5I, J2Z, V1C, R2M, F8V, X2M, O8L, Z4F, I6U, R1Y, N6P, K0V, C2E, E9J, I9H, D0R, A1W, E7C, O2G, Z5G, C6E, C1J, R9X, J4X, W4I, P2I, Q4Y, D3Z, B4K, M6C, E2B, R7J, C4I, Z9W, R4X, C1M, C7A, D3A, O6N, Q5K, W2M, M0I, C8W, L2R, Q1L, T0Z, Q7R, R2P, H1V, U3B, B1Z, D3Q, J9I, Q8N, V8Z, N7L, N5C, M9A, F1J, F7X, A1S, M9O, Z0X, L1N, E1N, Q7U, T2N, F1Z, O2K, X0Z, Z9A, Z0E, Z2L, K6D, V1B, M8D, I1Y, W3M, V0X, D9Q, H1J, C6V, Z2F, E9G, V7D, C2F, N1H, J3T, V6J, N3E, F9Q, V1M, C3G, E0U, C2O, Q8G, V7V, Q5Y, X4N, E6D, Z4Y, Z1Z, E0N, D9X, N7E, W8Y, E0C, N6Z, F3E, C6W, Y9Y, C9R, D0Q, X1M, K5Y, O7D, A4B, I3D, D2C, H8N, R5W, C1R, T0T, P5N, H1K, Y4B, W4N, D3C, Y3I, A0D, Q6Y, O0A, W4V</t>
+          <t>Z5B, M1I, Q5N, C0G, J2C, W1R, C7S, Y1C, X0A, K1C, W3W, C9Z, P6A, Q3A, D9C, Z5I, J2Z, V1C, R2M, F8V, X2M, O8L, Z4F, I6U, R1Y, N6P, K0V, C2E, E9J, I9H, D0R, A1W, E7C, O2G, Z5G, C6E, C1J, R9X, J4X, W4I, P2I, Q4Y, D3Z, B4K, M6C, E2B, R7J, C4I, Z9W, R4X, C1M, C7A, D3A, O6N, Q5K, W2M, C8W, L2R, Q1L, T0Z, Q7R, R2P, H1V, U3B, B1Z, D3Q, J9I, Q8N, V8Z, N7L, N5C, M9A, F1J, F7X, A1S, M9O, Z0X, L1N, E1N, Q7U, T2N, F1Z, O2K, X0Z, Z9A, Z0E, Z2L, K6D, V1B, M8D, I1Y, W3M, V0X, D9Q, H1J, C6V, Z2F, E9G, V7D, C2F, N1H, J3T, V6J, N3E, F9Q, V1M, C3G, E0U, C2O, Q8G, V7V, Q5Y, X4N, E6D, Z4Y, Z1Z, E0N, D9X, N7E, W8Y, E0C, N6Z, F3E, C6W, Y9Y, C9R, D0Q, X1M, K5Y, O7D, A4B, I3D, D2C, H8N, R5W, C1R, T0T, P5N, H1K, Y4B, W4N, D3C, Y3I, A0D, Q6Y, O0A, W4V</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -4406,7 +4490,11 @@
           <t>NMB68675387124893</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr"/>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4514,7 +4602,11 @@
           <t>WEB13675182237484</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -4538,7 +4630,11 @@
           <t>NMB18505876058372</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr"/>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -4554,7 +4650,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Z5C, M2D, Z7Y, R7D, P7S, D6G, R1O, M8U, F3F, I0A, E0Y, W6O, Z9A, G3F, K3J, C7A, Z3P, D1M, W4V, C8U, P7R, M8L, N1G, K7G, Z2J, W5W, Q8M, M7S, S1J, X3Z, W6K, N8I, G0U, L1L, I4G, J6C, C7C, A5R, C1C, U2L, D3E, M0K, B1X, Z2X, C8X, R0Z, P2L, J1A, C7B, X1S, K5Q, W2O, R6U, F1N, D6N, F6H, X2C, N0A, D3K, I2M, U1V, V2L, V4Y, D3P, J3D, L9E, Z4F, Z9Y, M1A, Z4X, M7U, K1O, V1M, E3V, Z7V, C5R, R5N, E9H, T1F, U6B, D5Y, M5T, Z2P, J9Y, B1E, D2J, E5J, A2H, V9Q, E1S, A2V, F1A, K5Y, C8Q, E2N, R4L, O6T, F3Y, D7F, E6D, Z8V, W5A, N3U, Q0I, P9P, Z0Y, F2U, E6J, B1F, W6G, A4Y, Q7Z, U3B, A2L, W1E, V7G, F8V, N5C, Z3Z, D5M, X4S, E7B, L2J, C2A, R3K, Z6I, Z1B, K3Q, R3Q, B5B, C3H, D9E, M9W, Z2M, P7V, A2Z, A4F, S1I, T1V, O1X, O4R, D0B, K6G, Y2A, V7X, U0Q, C7F, E7A, M5V, O8A, R2H, O4S, O0I, Q7I, J3S, W4C, P8B, N4A, E1Q, F5J, U6E, A1Z, F2Q, I1K, O7U, P5B, C9U, T0U, G0N, Z5O, F5U, I0S, J1O, O3D, X1E, N7Q, E7F, Z3O, W1H, N1P, C9B, N9X, C9N, Z9M, Z5A, O8E, P6Q, Z7T, L3A, C6J, T1L, C0Y, V2K, C5W, L1Y, U2K, V2G, L2I, T0W, W8F, U7L, Q6G, Z0J, I6I, R6Y, M5J, X3I</t>
+          <t>Z5C, M2D, Z7Y, R7D, P7S, D6G, R1O, M8U, F3F, I0A, E0Y, W6O, Z9A, G3F, K3J, C7A, Z3P, D1M, W4V, C8U, P7R, M8L, N1G, K7G, Z2J, W5W, Q8M, M7S, S1J, X3Z, W6K, N8I, G0U, L1L, I4G, J6C, C7C, A5R, C1C, U2L, D3E, M0K, B1X, Z2X, C8X, R0Z, P2L, J1A, C7B, X1S, K5Q, W2O, R6U, F1N, D6N, F6H, X2C, N0A, D3K, I2M, U1V, V2L, V4Y, D3P, J3D, L9E, Z4F, Z9Y, M1A, Z4X, M7U, K1O, V1M, E3V, Z7V, C5R, R5N, E9H, T1F, U6B, D5Y, M5T, Z2P, J9Y, B1E, D2J, E5J, A2H, V9Q, E1S, A2V, F1A, K5Y, C8Q, E2N, R4L, O6T, F3Y, D7F, E6D, Z8V, W5A, N3U, Q0I, P9P, Z0Y, F2U, E6J, B1F, W6G, A4Y, Q7Z, U3B, A2L, W1E, V7G, F8V, N5C, Z3Z, D5M, X4S, E7B, L2J, C2A, R3K, Z6I, Z1B, K3Q, R3Q, B5B, C3H, D9E, M9W, Z2M, P7V, A2Z, A4F, S1I, T1V, O1X, O4R, D0B, K6G, Y2A, V7X, U0Q, C7F, E7A, M5V, O8A, R2H, O4S, O0I, Q7I, J3S, W4C, P8B, N4A, E1Q, F5J, U6E, A1Z, F2Q, I1K, O7U, P5B, C9U, T0U, G0N, Z5O, F5U, I0S, J1O, O3D, X1E, N7Q, E7F, Z3O, W1H, N1P, C9B, N9X, C9N, Z9M, O8E, P6Q, Z7T, L3A, C6J, T1L, C0Y, V2K, C5W, L1Y, U2K, V2G, L2I, T0W, W8F, U7L, Q6G, Z0J, I6I, R6Y, M5J, X3I</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -4618,7 +4714,11 @@
           <t>WDB64172908761989</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr"/>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -4662,7 +4762,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Z5C, M2D, K1U, U2Y, D0X, M5K, W0M, K7K, S8C, K1X, E4A, V1A, K4H, A0A, R1V, W5K, J4A, R5O, I3D, C1J, I1W, R7F, R3G, Z2D, K5M, D1Z, W7J, X1H, D2P, S9Y, Q4B, P7V, C7P, O7T, R7K, D6Z, F2L, F1N, M9A, T0H, L4C, F2J, A3C, K0I, K7V, C8J, E3F, X2V, D6R, C1S, Z3K, O1A, C7T, C8Q, B2F, J3J, C5D, D6P, R2W, W7A, R2M, M0D, Z1U, E5T, M7H, Y9A, V8B, O2A, A4M, P9K, Z8Z, V1D, M5Y, A5I, P0V, J9S, D4Q, C8Z, Q1L, F9W, G5B, M5W, H8Z, I4E, F2B, A1M, V6E, K2C, W2N, K6S, O5O, P6H, A2C, E5H, J9I, A1W, I0I, Z5O, K2W, W0K, K5G, E0W, Z8V, N6R, F0O, I6U, B2B, Z3Z, F0G, K6I, Q1O, D1A, Z2U, Q8B, R0E, P8F, H8X, W6V, R8F, Y9V, Z2S, I5T, Z2O, E6B, F2W, R1S, H2K, H2I, Z1L, J8Y, A1H, I6C, N7V, K4K, W0L, Q7I, C3P, R7L, X3T, Z5V, U2P, W9P, I5F, Z0Z, I6K, N5F, O0E, F8W, H1W, K1P, F2U, W6Z, V1X, Z4U, Z5A, F2O, D6F, W4Q, P6L, U6B, S5E, Q7Y, U0B, R2C, W4G, P0H, M0T, O4D, A4Y, Z6F, A4D, F1U, N5D, G0U, W2H, K7Y, R0T, Z9M, O4B, E4T, G3E, D3M, W2J, I7X, Q6I, H2E, E4X, J3T, Z9Y, Q4L, W5E, B3G, D0L, F4J, D4C, X1K, P9S, G4Z, F3E, X1S, M9Y, G3G, D4A, Q5A, Q7P, R1N, I6I, D3R, V7Q, M9W, P5N, F6E, I1U, K2L, P6I, E5E, J3O, F5K, X3G, D7V, R1F, J1O, X4K, C3F, Z8R, A6D, L1T, C5O, W5U, U8C, Z2L, E1N, F1R, Q6G, G0M, Y9W, W2X, C9X, F7V, O7X, W0I, N0C, B1F, V3A, C4V, Q1P, E1J, T2Z, F1C, Z1A, P5G, X3U, O5U, W6M, T0Z, Y9Y, Q3M, F7S, G5H, B2D, I2B, X4S, P1D, M7V, F0N, P2T, P0S, A5X, T4A, N0X, T2L, S5A, D7A, M5L, R1L, R1D, I1Q, W3P, Q4Z, X1O, A2L, D6M, M5M, J9P, P9O, N3H, X4F, Z1C</t>
+          <t>Z5C, M2D, K1U, U2Y, D0X, M5K, W0M, K7K, S8C, K1X, E4A, V1A, K4H, A0A, R1V, W5K, J4A, R5O, I3D, C1J, I1W, R7F, R3G, Z2D, K5M, D1Z, W7J, X1H, D2P, S9Y, Q4B, P7V, C7P, O7T, R7K, D6Z, F2L, F1N, M9A, T0H, L4C, F2J, A3C, K0I, K7V, C8J, E3F, X2V, D6R, C1S, Z3K, O1A, C7T, C8Q, B2F, J3J, C5D, D6P, R2W, W7A, R2M, M0D, Z1U, E5T, M7H, Y9A, V8B, O2A, A4M, P9K, Z8Z, V1D, M5Y, A5I, P0V, J9S, D4Q, C8Z, Q1L, F9W, G5B, M5W, H8Z, I4E, F2B, A1M, V6E, K2C, W2N, K6S, O5O, P6H, A2C, E5H, J9I, A1W, I0I, Z5O, K2W, W0K, K5G, E0W, Z8V, N6R, F0O, I6U, B2B, Z3Z, F0G, K6I, Q1O, D1A, Z2U, Q8B, R0E, P8F, H8X, W6V, R8F, Y9V, Z2S, I5T, Z2O, E6B, F2W, R1S, H2K, H2I, Z1L, J8Y, A1H, I6C, N7V, K4K, W0L, Q7I, C3P, R7L, X3T, Z5V, U2P, W9P, I5F, Z0Z, I6K, N5F, O0E, F8W, H1W, K1P, F2U, W6Z, V1X, Z4U, F2O, D6F, W4Q, P6L, U6B, S5E, Q7Y, U0B, R2C, W4G, P0H, M0T, O4D, A4Y, Z6F, A4D, F1U, N5D, G0U, W2H, K7Y, R0T, Z9M, O4B, E4T, G3E, D3M, W2J, I7X, Q6I, H2E, E4X, J3T, Z9Y, Q4L, W5E, B3G, D0L, F4J, D4C, X1K, P9S, G4Z, F3E, X1S, M9Y, G3G, D4A, Q5A, Q7P, R1N, I6I, D3R, V7Q, M9W, P5N, F6E, I1U, K2L, P6I, E5E, J3O, F5K, X3G, D7V, R1F, J1O, X4K, C3F, Z8R, A6D, L1T, C5O, W5U, U8C, Z2L, E1N, F1R, Q6G, G0M, Y9W, W2X, C9X, F7V, O7X, W0I, N0C, B1F, V3A, C4V, Q1P, E1J, T2Z, F1C, Z1A, P5G, X3U, O5U, W6M, T0Z, Y9Y, Q3M, F7S, G5H, B2D, I2B, X4S, P1D, M7V, F0N, P2T, P0S, A5X, T4A, N0X, T2L, S5A, D7A, M5L, R1L, R1D, I1Q, W3P, Q4Z, X1O, A2L, D6M, M5M, J9P, P9O, N3H, X4F, Z1C</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4838,7 +4938,11 @@
           <t>W1T24266360390931</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr"/>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -4946,7 +5050,11 @@
           <t>W1T32194465952966</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr"/>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -5026,7 +5134,11 @@
           <t>WEB34232221714881</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr"/>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -5182,7 +5294,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Z5B, M1H, I5L, C6E, G9Y, F4X, C7J, E5A, I5E, J9R, W7E, W2A, F6X, I3L, I7M, F7V, Z4Q, O4E, C7D, C2N, F2Q, C1K, D3B, P0B, M0A, R7H, C2T, R5N, U3K, M9O, D6G, F9R, B5N, I6F, C2K, Z7V, O3A, D1G, P1D, T0F, D6F, K7S, N7B, T2A, O2H, C4S, I7V, I1G, E6B, V7U, T0U, V2V, U2M, T0W, P8C, O7A, C9X, Z4J, Q8U, K5U, N2S, Y1W, M8P, V0U, R3P, V5A, W7V, W0N, P9T, D4I, S8J, K2A, W1V, D9Q, F6J, Y4F, D2K, K9V, X2C, Z0X, N1X, E1K, K4C, O4C, Z4B, W1U, I6T, F1M, C6I, Z5O, K3J, R6C, U3F, C5A, Z4F, D3K, W3A, I4Q, L0Y, A9Z, C2S, N5C, R1I, O5T, K2B, I6L, N3M, F7Z, O5M, K6I, O3C, R2C, Q7Q, C8A, P5A, N0Z, J8Z, W5G, O7L, V6J, I2F, W2Y, U2R, I4N, R6T, M0I, T3P, K7I, Z3Z, E2A, U7L, C1H, C1L, N0I, I8Y, Z0J, Z8I, R5O, F3H, I4I, Z0L, C0B, Q4X, K6B, W5E, E0F, T3K, P6C, R1M, N1A, I7Y, W4C, E5V, D7D, E3L, I5O, J3J, P2L, X1Z, S5B, A4P, C8X, F0W, D3S, F7Q, B1A, Z7M, C2F, F9P, A1Z, L2B, G9B, R1X, A2G, M0H, Q5K, Z7Y, P0U, D7M, C6K, V2C, O6E, Z3Q, K5Y, A5F, W6G, N8K, F6M, Z0W, V5Z, V2S, V4Y, E1E, N1N, A1J, N8D, Z3P, A1F, C6G, J3C, B5J, Q6G, D0Y, K2W, D7N, C6S, Z3K, J6Z, Z7C, Q5P, K6F, W5K, V2P, U2V, R3Y, D6Z, I2H, W8Y, T1K, V2I, Q1S, U0C, W7U, A0B, F1K, K3E, X3Y, I5P, Q5L, N4M, W8M, D5J, O6T, K3T, E4Y, I7G</t>
+          <t>Z5B, M1H, I5L, C6E, G9Y, F4X, C7J, E5A, I5E, J9R, W7E, W2A, F6X, I3L, I7M, F7V, Z4Q, O4E, C7D, C2N, F2Q, C1K, D3B, P0B, M0A, R7H, C2T, R5N, U3K, M9O, D6G, F9R, B5N, I6F, C2K, Z7V, O3A, D1G, P1D, T0F, D6F, K7S, N7B, T2A, O2H, C4S, I7V, I1G, E6B, V7U, T0U, V2V, U2M, T0W, P8C, O7A, C9X, Z4J, Q8U, K5U, N2S, Y1W, M8P, V0U, R3P, V5A, W7V, W0N, P9T, D4I, S8J, K2A, W1V, D9Q, F6J, Y4F, D2K, K9V, X2C, Z0X, N1X, E1K, K4C, O4C, Z4B, W1U, I6T, F1M, C6I, Z5O, K3J, R6C, U3F, C5A, Z4F, D3K, W3A, I4Q, L0Y, A9Z, C2S, N5C, R1I, O5T, K2B, I6L, N3M, F7Z, O5M, K6I, O3C, R2C, Q7Q, C8A, P5A, N0Z, J8Z, W5G, O7L, V6J, I2F, W2Y, U2R, I4N, R6T, T3P, K7I, Z3Z, E2A, U7L, C1H, C1L, N0I, I8Y, Z0J, Z8I, R5O, F3H, I4I, Z0L, C0B, Q4X, K6B, W5E, E0F, T3K, P6C, R1M, N1A, I7Y, W4C, E5V, D7D, E3L, I5O, J3J, P2L, X1Z, S5B, A4P, C8X, F0W, D3S, F7Q, B1A, Z7M, C2F, F9P, A1Z, L2B, G9B, R1X, A2G, M0H, Q5K, Z7Y, P0U, D7M, C6K, V2C, O6E, Z3Q, K5Y, A5F, W6G, N8K, F6M, Z0W, V5Z, V2S, V4Y, E1E, N1N, A1J, N8D, Z3P, A1F, C6G, J3C, B5J, Q6G, D0Y, K2W, D7N, C6S, Z3K, J6Z, Z7C, Q5P, K6F, W5K, V2P, U2V, R3Y, D6Z, I2H, W8Y, T1K, V2I, Q1S, U0C, W7U, A0B, F1K, K3E, X3Y, I5P, Q5L, N4M, W8M, D5J, O6T, K3T, E4Y, I7G</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -5302,7 +5414,11 @@
           <t>WEB15711131661916</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr"/>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -5318,7 +5434,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Z5L, M3J, Z7P, F1Y, F5Z, R1W, W0P, M0A, F5Y, M7U, W0M, D9C, F0O, Z3A, V2T, D2U, J2Z, E6L, D4M, C9J, X3L, Z8V, P1B, T1L, E0U, C6D, W3M, Q8O, C9W, I2B, V7L, M8L, N0Y, E2E, I4B, C2A, V1K, P2I, F3W, K0A, D0L, R4Z, K4H, F3G, G1J, R8D, T2I, Z8E, Q8E, P1E, B2X, E0K, C6L, T1M, E5W, S5Z, N0B, A1C, J1F, O6S, Q6L, A6C, J8X, W6G, O1D, V1X, I6M, M8D, Q1E, X1X, C8M, N3G, P2K, L4B, D5V, A2F, Z7S, I4G, K0U, Q7D, T2J, U2L, Q8D, O2H, M9Y, T0X, V6R, Z1Z, A2B, W4Y, E1C, X4L, R3G, W0I, W6Y, X1Z, W0S, R0V, W5J, K8Y, W2P, C1W, X2X, E4W, X2M, E9G, N3M, F6M, V4A, C0G, F0Z, K2U, Q4E, Q8R, X1P, Z9V, Z5A, C2J, P8F, C5M, Q7I, V1F, Z7L, A1E, O0H, Z8M, R9Z, K7B, Z0F, X6A, Z8G, Y4X, A1N, Y6E, Z5W, M6C, Y1D, Z6G, H2H, W5U, P6A, I0E, K2V, C5Y, T3N, W5V, G0M, Q4X, Z4S, V6F, V1N, A1O, Q8U, G4I, Z9G, V8V, J6B, C5T, W2G, E0D, Q3Z, P6V, W5L, Q1N, L0U, V1E, D5R, E6B, N5C, W2I, K3V, Z0V, Z7V, Q3C, X4A, F1U, R7K, D5Z, I6A, C2N, Q4A, B4A, Z0S, Z0Z, T2E, A2M, Q4N, P6B, C3G, D8N, U2Q, O0A, C1Z, A1H, C5U, L3D, M1A, U0E, J1P, T3C, J2B, I7T</t>
+          <t>Z5L, M3J, Z7P, F1Y, F5Z, R1W, W0P, M0A, F5Y, M7U, W0M, D9C, F0O, Z3A, V2T, D2U, J2Z, E6L, D4M, C9J, X3L, Z8V, P1B, T1L, E0U, C6D, W3M, Q8O, C9W, I2B, V7L, M8L, N0Y, E2E, I4B, C2A, V1K, P2I, F3W, K0A, D0L, R4Z, K4H, F3G, G1J, R8D, T2I, Z8E, Q8E, P1E, B2X, E0K, C6L, T1M, E5W, S5Z, N0B, A1C, J1F, O6S, Q6L, A6C, J8X, W6G, O1D, V1X, I6M, M8D, Q1E, X1X, C8M, N3G, P2K, L4B, D5V, A2F, Z7S, I4G, K0U, Q7D, T2J, U2L, Q8D, O2H, M9Y, T0X, V6R, Z1Z, A2B, W4Y, E1C, X4L, R3G, W0I, W6Y, X1Z, W0S, R0V, W5J, K8Y, W2P, C1W, X2X, E4W, X2M, E9G, N3M, F6M, V4A, C0G, F0Z, K2U, Q4E, Q8R, X1P, Z9V, C2J, P8F, C5M, Q7I, V1F, Z7L, A1E, O0H, Z8M, R9Z, K7B, Z0F, X6A, Z8G, Y4X, A1N, Y6E, Z5W, M6C, Y1D, Z6G, H2H, W5U, P6A, I0E, K2V, C5Y, T3N, W5V, G0M, Q4X, Z4S, V6F, V1N, A1O, Q8U, G4I, Z9G, V8V, J6B, C5T, W2G, E0D, Q3Z, P6V, W5L, Q1N, L0U, V1E, D5R, E6B, N5C, W2I, K3V, Z0V, Z7V, Q3C, X4A, F1U, R7K, D5Z, I6A, C2N, Q4A, B4A, Z0S, Z0Z, T2E, A2M, Q4N, P6B, C3G, D8N, U2Q, O0A, C1Z, A1H, C5U, L3D, M1A, U0E, J1P, T3C, J2B, I7T</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -5326,7 +5442,11 @@
           <t>NMB54295891596434</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr"/>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -5342,7 +5462,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Z5L, M3L, Q7W, Q6G, O8A, G4C, W1Z, E3Q, O8I, K7V, O7O, A5I, Q3U, W7L, Q5A, I2A, W9J, Z4S, G5A, C1N, J2U, M5S, I2B, Q7C, V7V, S1J, A5B, P6A, O7D, O1R, Z6N, W3C, K5J, X9W, E0F, C5C, Z5A, P8M, M4Y, W2H, P9Z, F0B, Z5W, E4B, E3D, V4T, Q2T, Q9C, D5Z, Q4T, E5M, M0J, M1B, C8Y, K1M, D9W, I4H, E2J, F6T, W5R, P5G, L2B, P2A, H8N, Z7P, W2L, U0O, Z7J, Q4N, Q8Q, Z2O, T0U, Q2B, P8C, K5E, A4Q, P6V, H8Q, T3S, N1U, V6B, E9C, V7Q, V2N, G4H, Y9Z, C7B, Z8O, Q2P, N1Y, F4P, R3Y, D0I, L9W, K7F, K7S, R6Y, D5J, N9V, W3Q, F6D, C0T, U1F, Q4R, Q6I, L1Z, L3D, Z2Q, D4I, Q7L, L2J, K6N, X2J, F0O, P0S, O7E, B1U, O7Z, A4L, V6E, D3U, C8C, Z3Q, J9K, I6K, X4F, N6T, U1U, V7E, O1Z, A5J, X1D, G1F, E0E, A1Z, Q6R, J3D, X4G, J9B, K2L, K9Z, F8H, Z5G, G5Y, P9R, T1K, F2U, T1X, W4E, J9J, I2G, A5D, E9J, I9Z, L1S, J1A, W5H, E1A, F1P, A3C, C1Z, M0X, R8C, A4Y, F6A, I5W, R5M, I0Y, C5O, W2Y, Z2E, M9T, G4D, C4K, F1A, B1C, K0P, Q1I, W3U, K1A, O6S, O7V, N6E, D3F, F8J, A0A, N2D, T2E, Q7O, K6E, D3W, B2X, P0F, C7A, W1R, C9F, E9D, K5Q, D9A, O8T, I9I, F8M, J1T, U3N, Z5U, C2P, W7S, Q1K, X1Y, O4D, Z4P, S6F, C1S, U0B, Y4B, Z7V, D0U, Z7O, A4Z, Q0V, Q6A, L4C, K7Z, H2H, O2L, X1E, P4A, F4G, P2J, U2U, K6F, I8Z, B3K, A2X, I1Q, R2E, R2Y, K3R, Z1G, Y4H, N9X, L2C, N1Z, I5G, R1J, L1A</t>
+          <t>Z5L, M3L, Q7W, Q6G, O8A, G4C, W1Z, E3Q, O8I, K7V, O7O, A5I, Q3U, W7L, Q5A, I2A, W9J, Z4S, G5A, C1N, J2U, M5S, I2B, Q7C, V7V, S1J, A5B, P6A, O7D, O1R, Z6N, W3C, K5J, X9W, E0F, C5C, P8M, M4Y, W2H, P9Z, F0B, Z5W, E4B, E3D, V4T, Q2T, Q9C, D5Z, Q4T, E5M, M1B, C8Y, K1M, D9W, I4H, E2J, F6T, W5R, P5G, L2B, P2A, H8N, Z7P, W2L, U0O, Z7J, Q4N, Q8Q, Z2O, T0U, Q2B, P8C, K5E, A4Q, P6V, H8Q, T3S, N1U, V6B, E9C, V7Q, V2N, G4H, Y9Z, C7B, Z8O, Q2P, N1Y, F4P, R3Y, D0I, L9W, K7F, K7S, R6Y, D5J, N9V, W3Q, F6D, C0T, U1F, Q4R, Q6I, L1Z, L3D, Z2Q, D4I, Q7L, L2J, K6N, X2J, F0O, P0S, O7E, B1U, O7Z, A4L, V6E, D3U, C8C, Z3Q, J9K, I6K, X4F, N6T, U1U, V7E, O1Z, A5J, X1D, G1F, E0E, A1Z, Q6R, J3D, X4G, J9B, K2L, K9Z, F8H, Z5G, G5Y, P9R, T1K, F2U, T1X, W4E, J9J, I2G, A5D, E9J, I9Z, L1S, J1A, W5H, E1A, F1P, A3C, C1Z, M0X, R8C, A4Y, F6A, I5W, R5M, I0Y, C5O, W2Y, Z2E, M9T, G4D, C4K, F1A, B1C, K0P, Q1I, W3U, K1A, O6S, O7V, N6E, D3F, F8J, A0A, N2D, T2E, Q7O, K6E, D3W, B2X, P0F, C7A, W1R, C9F, E9D, K5Q, D9A, O8T, I9I, F8M, J1T, U3N, Z5U, C2P, W7S, Q1K, X1Y, O4D, Z4P, S6F, C1S, U0B, Y4B, Z7V, D0U, Z7O, A4Z, Q0V, Q6A, L4C, K7Z, H2H, O2L, X1E, P4A, F4G, P2J, U2U, K6F, I8Z, B3K, A2X, I1Q, R2E, R2Y, K3R, Z1G, Y4H, N9X, L2C, N1Z, I5G, R1J, L1A</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -5350,7 +5470,11 @@
           <t>W1T94110442710354</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr"/>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -5402,7 +5526,11 @@
           <t>NMB48051423370057</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr"/>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -5426,7 +5554,11 @@
           <t>WEB58983495409038</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr"/>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -5610,7 +5742,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Z5F, M3P, I4B, N7G, W1U, Q6X, Z8P, K9Z, D1C, N6R, K0L, I2U, C8X, D3K, M1C, N7M, U0A, W2Y, Z5O, X9V, I7G, Q2B, Z0H, N3U, H1N, C8A, D4C, T0V, V1K, Z2N, R5W, F4Y, B1Z, C9L, D8N, O0G, F1W, N5X, O7M, Z1I, C4B, M6D, Q3Y, E6G, N7F, D7A, T2D, Z7B, L1H, Z5G, F6Q, C2G, J2D, V8W, Z3U, P0W, Q5N, E4Y, H1B, A4Y, M0J, F2X, U0D, W0M, K3U, I2B, W0U, U1V, D6M, G3G, J2W, R4Y, Y6J, W4T, C0L, F1Z, W8C, D3Y, A1W, O8U, N3B, B2X, T3A, F5N, K8A, Z8T, J3Q, D0Z, U3L, K5L, Z1F, R2D, B9V, K1L, C9Y, W1X, J2O, C6X, J9K, R7F, V2U, D9L, W4E, V6C, P9K, Z7S, R2Z, M9W, A5G, W7M, I6D, A2N, I1E, M7S, D5P, H8W, R8O, J9F, E2B, C3B, P1I, C1K, N4Y, X1G, I0K, Z6M, F8D, F1J, T2U, C6D, I5Q, B2E, Y2A, A2V, R2N, Q5Y, L1N, Q7J, G5A, F1A, I9J, N2S, Q1P, P8C, W7J, O1V, C4K, N1U, F1N, K0Q, C4X, V0U, R4W, J4X, Q1G, V6E, D5N, K5P, Y1K, Z8W, N8D, F6B, D4U, A2H, J2H, Y1T, O2O, F0Y, A1G, C3K, R1S, P2M, N4B, A4Z, Q7P, Z1Z, R5P, P7Y, R8P, L2J, T0Z, D9G, C9V, O3C, O4C, F8X, L9C, K2N, D5C, J3V, P6Q, D2A, J3G, Z8I, C6M, Q8M, H2J, O2K, Z1T, U2I, Z0I, Q7S, O1T, Q5D, N3A, V1Q, W4R, U1A, M8C, J9N, A3D, P0D, W0N, Z4H, P6H, W0Q, Q8C, Q2A, F9C, N6Z, W7F, Q4M, E3D, M0U, V6V, L9Z, N7N, Z0R, F4P, V7P, L2R, Z9K, K1K, G5Z, W1B, C6N, W3K, Y4S, A0D, E3L, C2C, U2K, C3R, E0U, F6T, D2Z, K7Z, W9Q, N1P, C5F, Z0A, R2U</t>
+          <t>Z5F, M3P, I4B, N7G, W1U, Q6X, Z8P, K9Z, D1C, N6R, K0L, I2U, C8X, D3K, M1C, N7M, U0A, W2Y, Z5O, X9V, I7G, Q2B, Z0H, N3U, H1N, C8A, D4C, T0V, V1K, Z2N, R5W, F4Y, B1Z, C9L, D8N, O0G, F1W, N5X, O7M, Z1I, C4B, M6D, Q3Y, E6G, N7F, D7A, T2D, Z7B, L1H, Z5G, F6Q, C2G, J2D, V8W, Z3U, P0W, Q5N, E4Y, H1B, A4Y, F2X, U0D, W0M, K3U, I2B, W0U, U1V, D6M, G3G, J2W, R4Y, Y6J, W4T, C0L, F1Z, W8C, D3Y, A1W, O8U, N3B, B2X, T3A, F5N, K8A, Z8T, J3Q, D0Z, U3L, K5L, Z1F, R2D, B9V, K1L, C9Y, W1X, J2O, C6X, J9K, R7F, V2U, D9L, W4E, V6C, P9K, Z7S, R2Z, M9W, A5G, W7M, I6D, A2N, I1E, M7S, D5P, H8W, R8O, J9F, E2B, C3B, P1I, C1K, N4Y, X1G, I0K, Z6M, F8D, F1J, T2U, C6D, I5Q, B2E, Y2A, A2V, R2N, Q5Y, L1N, Q7J, G5A, F1A, I9J, N2S, Q1P, P8C, W7J, O1V, C4K, N1U, F1N, K0Q, C4X, V0U, R4W, J4X, Q1G, V6E, D5N, K5P, Y1K, Z8W, N8D, F6B, D4U, A2H, J2H, Y1T, O2O, F0Y, A1G, C3K, R1S, P2M, N4B, A4Z, Q7P, Z1Z, R5P, P7Y, R8P, L2J, T0Z, D9G, C9V, O3C, O4C, F8X, L9C, K2N, D5C, J3V, P6Q, D2A, J3G, Z8I, C6M, Q8M, H2J, O2K, Z1T, U2I, Z0I, Q7S, O1T, Q5D, N3A, V1Q, W4R, U1A, M8C, J9N, A3D, P0D, W0N, Z4H, P6H, W0Q, Q8C, Q2A, F9C, N6Z, W7F, Q4M, E3D, M0U, V6V, L9Z, N7N, Z0R, F4P, V7P, L2R, Z9K, K1K, G5Z, W1B, C6N, W3K, Y4S, A0D, E3L, C2C, U2K, C3R, E0U, F6T, D2Z, K7Z, W9Q, N1P, C5F, Z0A, R2U</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -5778,7 +5910,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Z5B, M1H, E3C, E1V, E9K, C7W, Z4W, N1I, A1G, M8Z, J2E, M5R, T1D, Q1X, E3M, T1Z, Q7B, C3G, V7I, C7D, P6E, W7L, F0K, Q6F, I1J, U3M, I2Z, M8U, S1J, K7N, Y6J, Z7L, W3D, Z2U, N4X, U2K, P7R, E4T, Z4Q, W6D, B5C, F5G, W8M, W1Z, Y4I, C3R, D3Q, E9L, F7D, Z1X, B1Z, C0F, S9B, I4J, K7H, N1V, P1A, V7J, O4B, K1S, F3V, V4A, G2G, C8P, I6C, W0U, K3U, W6W, M8Q, D3G, D2O, O2G, Q1J, M7U, Z9V, T1L, K4H, Q4K, W4I, N5M, V1S, N4E, C6A, Q1B, D0J, N3D, K4J, X1T, Q7N, R4D, K5L, C0Q, P4U, V3L, Z4N, Q7W, T1U, N7I, J1T, F2X, O7W, I5C, V1D, E6K, V6S, Z9Z, E6L, I5Z, M0U, R5D, R3Q, O5O, K8Z, F6B, C1Q, T4A, W0J, K7G, W1A, I1A, M0B, I2H, J3A, Q8A, E6Y, Q1W, K7Z, U1F, Z8N, C2K, Y1K, X2W, W2Y, Q0Y, Q6E, V2G, M0J, J4X, C0Y, I5E, D5O, V6H, S8H, N0B, A2B, F0Y, I2M, O2K, E3Q, D0A, J1E, B1C, P6G, M2H, D0V, Y1F, W9I, H2G, J3S, O3A, B1A, N7A, C2N, F6X, S5S, A5N, F8C, N3G, E1P, H2F, E9X, C1K, D4M, R4W, Q4F, T3B, U1P, E0V, D8L, R6Y, O4G, K0E, I0M, C9Q, J2U, R2Q, S1M, C4C, X1Q, O8A, S5Z, E8A, T4U, D1L, K3B, E5E, C3U, Q6W, V1N, T0N, X1J, G0D, F2E, W5Y, Z7U, P1I, D3K, O5M, N3H, O8K, F8F, S1E, Q1V, V3A, Q7X, V2A, U3P, Z3O, S5R, U8X, I4D, V2H, W4O, L4Z, A4T, I2I, I3L, D2U, H8N, X2R, P6V, K1E, B1B</t>
+          <t>Z5B, M1H, E3C, E1V, E9K, C7W, Z4W, N1I, A1G, M8Z, J2E, M5R, T1D, Q1X, E3M, T1Z, Q7B, C3G, V7I, C7D, P6E, W7L, F0K, Q6F, I1J, U3M, I2Z, M8U, S1J, K7N, Y6J, Z7L, W3D, Z2U, N4X, U2K, P7R, E4T, Z4Q, W6D, B5C, F5G, W8M, W1Z, Y4I, C3R, D3Q, E9L, F7D, Z1X, B1Z, C0F, S9B, I4J, K7H, N1V, P1A, V7J, O4B, K1S, F3V, V4A, G2G, C8P, I6C, W0U, K3U, W6W, M8Q, D3G, D2O, O2G, Q1J, M7U, Z9V, T1L, K4H, Q4K, W4I, N5M, V1S, N4E, C6A, Q1B, D0J, N3D, K4J, X1T, Q7N, R4D, K5L, C0Q, P4U, V3L, Z4N, Q7W, T1U, N7I, J1T, F2X, O7W, I5C, V1D, E6K, V6S, Z9Z, E6L, I5Z, M0U, R5D, R3Q, O5O, K8Z, F6B, C1Q, T4A, W0J, K7G, W1A, I1A, M0B, I2H, J3A, Q8A, E6Y, Q1W, K7Z, U1F, Z8N, C2K, Y1K, X2W, W2Y, Q0Y, Q6E, V2G, J4X, C0Y, I5E, D5O, V6H, S8H, N0B, A2B, F0Y, I2M, O2K, E3Q, D0A, J1E, B1C, P6G, M2H, D0V, Y1F, W9I, H2G, J3S, O3A, B1A, N7A, C2N, F6X, S5S, A5N, F8C, N3G, E1P, H2F, E9X, C1K, D4M, R4W, Q4F, T3B, U1P, E0V, D8L, R6Y, O4G, K0E, I0M, C9Q, J2U, R2Q, S1M, C4C, X1Q, O8A, S5Z, E8A, T4U, D1L, K3B, E5E, C3U, Q6W, V1N, T0N, X1J, G0D, F2E, W5Y, Z7U, P1I, D3K, O5M, N3H, O8K, F8F, S1E, Q1V, V3A, Q7X, V2A, U3P, Z3O, S5R, U8X, I4D, V2H, W4O, L4Z, A4T, I2I, I3L, D2U, H8N, X2R, P6V, K1E, B1B</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -5814,7 +5946,11 @@
           <t>WDB63883626217463</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr"/>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -5894,7 +6030,11 @@
           <t>NMB73188755928785</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr"/>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -5918,7 +6058,11 @@
           <t>WDB22332639481138</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr"/>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -5990,7 +6134,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Z5E, M3B, K2M, C6I, D7Q, Q2X, Y4A, E4X, W6W, E9D, D7Z, Z3T, M5T, G2C, D0P, C2G, J3H, T8A, T0D, Q6P, J8Y, K6C, K3S, N2E, Q7W, W3P, Z9I, I1M, Z5I, Z5A, C1P, Z7Z, M5G, Q8W, P8M, W4V, T3L, I3O, Z2H, V6U, Z1S, Z3N, D3Z, N3B, A6R, U3A, P1M, Q3M, Q7F, Z3F, R2E, E6I, Q6G, Q5V, W5N, W9Z, J3R, L9H, Q4R, I0W, Y3M, W0N, G2B, E6Y, L2N, M7U, V7T, U2G, C0M, R7D, K0F, R1S, K5V, D4A, W1Q, F0F, C7T, Z1K, D3X, A0H, O8B, W1V, J1K, V7K, I7G, W2X, Z5N, R8E, O4D, F2V, D8U, Z1Q, W2I, H1M, L2C, C1R, J9L, T3K, R3H, C8L, Z9A, T2F, F6Y, T0J, T2D, T1G, K1F, Q2A, W1P, I5R, O8E, F5L, A2A</t>
+          <t>Z5E, M3B, K2M, C6I, D7Q, Q2X, Y4A, E4X, W6W, E9D, D7Z, Z3T, M5T, G2C, D0P, C2G, J3H, T8A, T0D, Q6P, J8Y, K6C, K3S, N2E, Q7W, W3P, Z9I, I1M, Z5I, C1P, Z7Z, M5G, Q8W, P8M, W4V, T3L, I3O, Z2H, V6U, Z1S, Z3N, D3Z, N3B, A6R, U3A, P1M, Q3M, Q7F, Z3F, R2E, E6I, Q6G, Q5V, W5N, W9Z, J3R, L9H, Q4R, I0W, Y3M, W0N, G2B, E6Y, L2N, M7U, V7T, U2G, C0M, R7D, K0F, R1S, K5V, D4A, W1Q, F0F, C7T, Z1K, D3X, A0H, O8B, W1V, J1K, V7K, I7G, W2X, Z5N, R8E, O4D, F2V, D8U, Z1Q, W2I, H1M, L2C, C1R, J9L, T3K, R3H, C8L, Z9A, T2F, F6Y, T0J, T2D, T1G, K1F, Q2A, W1P, I5R, O8E, F5L, A2A</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -6074,7 +6218,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Z5C, M2A, Q1S, W7A, M8U, W1G, N9U, Q7K, Q2H, B2X, M6P, V6Q, M7F, O7D, P5F, X5G, Y4A, K1B, C1H, J3G, A6R, C7Y, Z4H, D0V, P8U, A1W, Q2Y, N2R, E4T, G4D, H1X, V5W, I5V, P6V, N3C, W3W, K2L, Z8J, L9E, D3O, Z4N, Q8P, F0D, D4S, E1C, C4S, P6L, Z1L, I1G, E3W, C4Y, T4C, A2N, Q2O, Q5Q, X4K, V1U, D3C, P8A, K2P, O2G, W3M, Y3I, X3P, Z9H, F6I, W5T, V5P, N8K, R8C, C4I, Q7F, W4J, Q0I, K3K, T0H, R5M, L9W, C3U, Z1H, W0Z, C0Q, T1K, I2Q, I5H, W4P, S8J, V6H, P2G, E4F, A6D, Q4R, V3W, D5L, W2Q, I4K, D3N, M5B, B2F, C2G, K5Y, E1E, Q9W, K1R, X4B, A3C, F2G, C9I, F1O, V7Y, W0V, A2M, W5M, Z5A, A6E, S9B, H1P, A4G, U1C, E1S, V3O, Y4J, F2B, I6N, W8M, X2S, Z4V, D0K, O8E, P9T, Z8L, Z6K, C5V, A1D, D9A, Z0O, W7E, R1C, Z5U, W0J, O2K, P4U, D7B, B2G, P7M, C1L, D5C, N4W, J2M, Q2U, Z0G, R2U, Z3B, V7C, C8J, J9C, Q2J, U1S, I5L, V9Q, Y1G, I5E, T2Q, Q1J, F0Q, P9P, I6J, E2J, H8X, L3A, F2J, Z1C, X4L, K1V, S9W, D1G, C5Y, D2Z, F2X, I8Z, D4T, T1C, O2R, U1P, Z0V, V2N, A0C, Z5V</t>
+          <t>Z5C, M2A, Q1S, W7A, M8U, W1G, N9U, Q7K, Q2H, B2X, M6P, V6Q, M7F, O7D, P5F, X5G, Y4A, K1B, C1H, J3G, A6R, C7Y, Z4H, D0V, P8U, A1W, Q2Y, N2R, E4T, G4D, H1X, V5W, I5V, P6V, N3C, W3W, K2L, Z8J, L9E, D3O, Z4N, Q8P, F0D, D4S, E1C, C4S, P6L, Z1L, I1G, E3W, C4Y, T4C, A2N, Q2O, Q5Q, X4K, V1U, D3C, P8A, K2P, O2G, W3M, Y3I, X3P, Z9H, F6I, W5T, V5P, N8K, R8C, C4I, Q7F, W4J, Q0I, K3K, T0H, R5M, L9W, C3U, Z1H, W0Z, C0Q, T1K, I2Q, I5H, W4P, S8J, V6H, P2G, E4F, A6D, Q4R, V3W, D5L, W2Q, I4K, D3N, M5B, B2F, C2G, K5Y, E1E, Q9W, K1R, X4B, A3C, F2G, C9I, F1O, V7Y, W0V, A2M, W5M, A6E, S9B, H1P, A4G, U1C, E1S, V3O, Y4J, F2B, I6N, W8M, X2S, Z4V, D0K, O8E, P9T, Z8L, Z6K, C5V, A1D, D9A, Z0O, W7E, R1C, Z5U, W0J, O2K, P4U, D7B, B2G, P7M, C1L, D5C, N4W, J2M, Q2U, Z0G, R2U, Z3B, V7C, C8J, J9C, Q2J, U1S, I5L, V9Q, Y1G, I5E, T2Q, Q1J, F0Q, P9P, I6J, E2J, H8X, L3A, F2J, Z1C, X4L, K1V, S9W, D1G, C5Y, D2Z, F2X, I8Z, D4T, T1C, O2R, U1P, Z0V, V2N, A0C, Z5V</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -6138,7 +6282,11 @@
           <t>NMB32370763079682</t>
         </is>
       </c>
-      <c r="F209" t="inlineStr"/>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -6246,7 +6394,11 @@
           <t>NMB74601920011870</t>
         </is>
       </c>
-      <c r="F213" t="inlineStr"/>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -6290,7 +6442,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Z5D, M2P, Q2M, Q8E, O5Y, O1F, I9J, Z4E, G1F, A5L, E0K, M7I, T2T, B4L, A5J, O2M, K1K, B2F, A5M, F9A, Z3B, W0V, J4X, V1Y, Q5V, P9A, F8Z, P1K, W3H, G1J, Y1F, I4A, I2K, H1P, V0T, W8E, C6D, E3C, Q1H, I4Y, E6C, Z1C, Q7O, E4G, B2X, Q1X, W5X, X2T, E5U, F5T, K0H, W6U, P9S, N8C, N6K, T1C, O6B, N0B, S9Z, T4U, S8F, Z2G, Q1F, C0Q, D0L, H2A, A2N, Q4C, Z8W, W3L, S1W, H8Q, J9Y, R4D, E9K, V1U, A1Q, Z6G, A1M, W3J, D7W, Q5S, C4X, O1H, I5F, M5K, I5V, M5R, K0U, V6Q, Z0W, L9B, Z4O, N0N, W1A, Z9V, V1B, Y3E, F6R, I2F, Z8A, O6H, D6I, W5I, T2J, F6G, U0O, O1C, Z2Q, M1E, D5Y, R1A, N7V, M9U, I7V, J9L, Q2A, Q6X, D2A, G2H, F9Q, M0J, Y1Y, F2X, P0R, E6Y, T8A, W2A, W4D, Z2L, D4H, E0Z, J3O, F9Y, D7E, J9N, T0Z, G1H, M8P, H2J, T3P, Z7S, Z8U, W2M, O7L, Z5S, W6N, F6W, Z5M, V5Y, F8G, M7T, J8W, I4Q, Q8W, X1V, E0X, Q9A, A6T, C3T, T1H, Z3D, F6Y, J1X, Q3E, N4C, E4D, T3M, Z9W, K1S, K5R, E2L, G3F, C5G, N7N, V1K, P9T, C0G, O8I, O1Z, K2X, Q2L, Q1G, I6E, U6B, E3I, S8A, T1V</t>
+          <t>Z5D, M2P, Q2M, Q8E, O5Y, O1F, I9J, Z4E, G1F, A5L, E0K, M7I, T2T, B4L, A5J, O2M, K1K, B2F, A5M, F9A, Z3B, W0V, J4X, V1Y, Q5V, P9A, F8Z, P1K, W3H, G1J, Y1F, I4A, I2K, H1P, V0T, W8E, C6D, E3C, Q1H, I4Y, E6C, Z1C, Q7O, E4G, B2X, Q1X, W5X, X2T, E5U, F5T, K0H, W6U, P9S, N8C, N6K, T1C, O6B, N0B, S9Z, T4U, S8F, Z2G, Q1F, C0Q, D0L, H2A, A2N, Q4C, Z8W, W3L, S1W, H8Q, J9Y, R4D, E9K, V1U, A1Q, Z6G, A1M, W3J, D7W, Q5S, C4X, O1H, I5F, M5K, I5V, M5R, K0U, V6Q, Z0W, L9B, Z4O, N0N, W1A, Z9V, V1B, Y3E, F6R, I2F, Z8A, O6H, D6I, W5I, T2J, F6G, U0O, O1C, Z2Q, M1E, D5Y, R1A, N7V, M9U, I7V, J9L, Q2A, Q6X, D2A, G2H, F9Q, Y1Y, F2X, P0R, E6Y, T8A, W2A, W4D, Z2L, D4H, E0Z, J3O, F9Y, D7E, J9N, T0Z, G1H, M8P, H2J, T3P, Z7S, Z8U, W2M, O7L, Z5S, W6N, F6W, Z5M, V5Y, F8G, M7T, J8W, I4Q, Q8W, X1V, E0X, Q9A, A6T, C3T, T1H, Z3D, F6Y, J1X, Q3E, N4C, E4D, T3M, Z9W, K1S, K5R, E2L, G3F, C5G, N7N, V1K, P9T, C0G, O8I, O1Z, K2X, Q2L, Q1G, I6E, U6B, E3I, S8A, T1V</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -6326,7 +6478,11 @@
           <t>WDB10503953260521</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr"/>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -6406,7 +6562,11 @@
           <t>WDB57094500721383</t>
         </is>
       </c>
-      <c r="F219" t="inlineStr"/>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -6478,7 +6638,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Z5F, M3V, D3C, D9E, K0T, D3P, I5B, M8Q, F8J, U0A, Q8E, X2Z, W3Y, O7V, K7O, E2N, E4E, F0L, D6H, W6C, V8Z, Q8D, W3N, Z1L, V1G, T1L, N3T, Z2X, L1C, E1K, L9I, E4I, V3W, N3S, Q8Z, H2C, A4K, Y9X, M8D, I4C, I5Q, W8Z, W6P, L2A, V6D, H8Q, V7H, P2I, X4H, Q1N, U2T, U0D, W9T, J3I, W3W, F5E, B5A, F1Y, O2B, Z4R, I1Q, A5F, I2B, F4X, R2X, Z2I, C9Y, T3A, W7I, N6Z, E2T, F6A, C7I, F2X, Q6H, C6N, O8L, A1L, U3K, G0W, F3P, T2I, R6M, K3S, R6X, O7G, Q4I, I6E, F0G, B5L, V2H, W7Z, F2H, Z3S, I7G, O6B, R4W, D0X, D7X, J9C, P5Y, W2K, K5E, Q7K, R8E, W6O, C6D, D9R, C6M, B2D, K6X, Q6C, I2E, M7V, X4I, I5M, P7U, V8N, V4T, D6F, L1X, M0I, G4B, C6C, E3M, Q1P, V2V, T3Q, K1D, T1Q, P1A, R7J, S5R, P2A</t>
+          <t>Z5F, M3V, D3C, D9E, K0T, D3P, I5B, M8Q, F8J, U0A, Q8E, X2Z, W3Y, O7V, K7O, E2N, E4E, F0L, D6H, W6C, V8Z, Q8D, W3N, Z1L, V1G, T1L, N3T, Z2X, L1C, E1K, L9I, E4I, V3W, N3S, Q8Z, H2C, A4K, Y9X, M8D, I4C, I5Q, W8Z, W6P, L2A, V6D, H8Q, V7H, P2I, X4H, Q1N, U2T, U0D, W9T, J3I, W3W, F5E, B5A, F1Y, O2B, Z4R, I1Q, A5F, I2B, F4X, R2X, Z2I, C9Y, T3A, W7I, N6Z, E2T, F6A, C7I, F2X, Q6H, C6N, O8L, A1L, U3K, G0W, F3P, T2I, R6M, K3S, R6X, O7G, Q4I, I6E, F0G, B5L, V2H, W7Z, F2H, Z3S, I7G, O6B, R4W, D0X, D7X, J9C, P5Y, W2K, K5E, Q7K, R8E, W6O, C6D, D9R, C6M, B2D, K6X, Q6C, I2E, M7V, X4I, I5M, P7U, V8N, V4T, D6F, L1X, G4B, C6C, E3M, Q1P, V2V, T3Q, K1D, T1Q, P1A, R7J, S5R, P2A</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -6758,7 +6918,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Z5B, M1J, S1U, K5R, R1U, S8E, U3Q, J9A, F2N, Q7Y, E3W, V7J, E9K, F1C, E2I, Y3O, N8P, D2U, Z1O, P2E, Q6H, K3O, X2E, J3J, W5F, P6Z, E6G, Z6L, Q1C, N3K, Z2G, J3V, H1K, A6F, U3D, D1T, N5A, T4U, W1H, N9Y, V1Q, Z0L, W0O, X1W, Q1Z, W3M, V4A, E5F, E9H, J2J, J9Q, D0A, N4Y, V7O, Z5W, F7Y, M0J, Q6R, Z5U, E4E, W1C, V1Z, W8C, C7G, L2M, U3L, W4Z, Q3F, D2C, N1H, A6D, P2Z, V1C, D3Q, Z4N, B1I, V2H, C4G, N6K, Q0C, C5J, P7S, L1C, F3E, E6A, C5A, K0Q, G5Y, O8O, Z0Z, R8E, D5Z, I6H, I2U, Z9D, X4A, T2L, U2P, W2I, J3F, C3F, M9V, L9I, D9G, W4H, J1Y, A4F, Q1M, M0T, A2Y, Z1N, Z2W, L1Q, R2Y, B1X, E0Y, Q1V, Z3W, E4W, B5N, C0U, S5G, Q4Q, N7F, D3T, V9Q, Y4F, I4A, A6B, L9G, F6C, M5R, T2D, A6T, Z0J, R8H, Z5Y, D6Z, X2I, L3D, K0X, D4U, C4S, Z0D, N5N, F1H, N6R, I6E, Q8Y, S1L, E1V, W7H, W6F, P5X, E9F, K5C, P2N, Z3J, L4A, K0V, V1N, Y4W, T1L, I7X, N6J, W0P, M8Z</t>
+          <t>Z5B, M1J, S1U, K5R, R1U, S8E, U3Q, J9A, F2N, Q7Y, E3W, V7J, E9K, F1C, E2I, Y3O, N8P, D2U, Z1O, P2E, Q6H, K3O, X2E, J3J, W5F, P6Z, E6G, Z6L, Q1C, N3K, Z2G, J3V, H1K, A6F, U3D, D1T, N5A, T4U, W1H, N9Y, V1Q, Z0L, W0O, X1W, Q1Z, W3M, V4A, E5F, E9H, J2J, J9Q, D0A, N4Y, V7O, Z5W, F7Y, Q6R, Z5U, E4E, W1C, V1Z, W8C, C7G, L2M, U3L, W4Z, Q3F, D2C, N1H, A6D, P2Z, V1C, D3Q, Z4N, B1I, V2H, C4G, N6K, Q0C, C5J, P7S, L1C, F3E, E6A, C5A, K0Q, G5Y, O8O, Z0Z, R8E, D5Z, I6H, I2U, Z9D, X4A, T2L, U2P, W2I, J3F, C3F, M9V, L9I, D9G, W4H, J1Y, A4F, Q1M, M0T, A2Y, Z1N, Z2W, L1Q, R2Y, B1X, E0Y, Q1V, Z3W, E4W, B5N, C0U, S5G, Q4Q, N7F, D3T, V9Q, Y4F, I4A, A6B, L9G, F6C, M5R, T2D, A6T, Z0J, R8H, Z5Y, D6Z, X2I, L3D, K0X, D4U, C4S, Z0D, N5N, F1H, N6R, I6E, Q8Y, S1L, E1V, W7H, W6F, P5X, E9F, K5C, P2N, Z3J, L4A, K0V, V1N, Y4W, T1L, I7X, N6J, W0P, M8Z</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -6786,7 +6946,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Z5L, M3J, F7Q, L9E, W8Y, F1E, V0S, F0E, V1E, E4C, E8L, P5G, V7V, T0W, L9Z, V7N, E5H, O4P, J3A, S1M, J9B, Q3M, N2G, A3C, X2V, Q1E, P6B, A1Y, R6Z, L1Z, Q7D, G2E, Z1O, B9Z, V4A, V2M, T5B, F9R, E0E, N7W, W0W, F7X, I8X, S1Y, O1F, P0S, C0Q, Z3B, J9D, Q1S, O2Q, V9H, F3C, W2V, N0C, K7V, Z0V, P8C, C9I, K5V, J3P, B5N, Q0I, G0U, Z1U, C9M, Q5V, D7P, I1I, W2S, I2U, A1Q, D3Z, D4T, C7P, Q6T, Z3P, Q4T, W5Y, K4K, F7I, C2L, O7U, V8R, X4H, Z2K, K6O, S5Q, Y4F, Q7L, J2W, W6M, P9G, N6R, B1E, Z0F, K1A, B9V, E3H, A6E, I4B, Z1F, U3K, E5T, I6H, C2T, K0T, J1K, E9W, Z3T, O5O, X2P, C5T, E6J, Y3M, T3A, P1M, G0O, N3B, N6T, O2I, K5P, Q3Z, Z4I, Q5Q, H1X, Q4K, O8U, O6D, K0O, F3K, C3U, D0S, B1G, P2L, Q8Z, F7A, D4B, G3H, E9J, E5A, N3K, W5M, W4G, F0V, G0D, V7J, I1V, X1K, V5Q, E4B, R2K, W7E, P9E, Z0A, F2J, M0L, C8R, I3D, L1T, C0T, W4H, W0V, T1R, V8B, Q0W, C7A, Q6D, Q7I, Z9H, W1E, N9Y, N4M, X2A, O8A, A5R, R2E, R9Z, E1E, I6L, T2I, A5J, C9Q, W5E, Z8Q, P2M, B2F, E2L, K6L, W1F, Q1B, Y4A, U1V, W7T, E6Y, V0T, L2B, Z5A, O8D, K0X, A2Z, V2G, V5R, Z2Y, F6L, W4O, L1I, Q7Q, P9P, V5X, V1W, P0B, Z8N, D0U, R3H, Q7H, R8H, Q3R, Y4L, F9W, C5N, X3V, Q4E, F7S, P0D, N3D, W3K, C8L, K6E, Z1C, W2B, W4J, G0R, L1B, U2T, W7R, U2R, X4I, Z4J, D3G, V8N, E9F, X1E, G1D, D1B, K1Q, I4H, J4V, E6B, I4Y, Z7Q, V6H, Q2S, W1P, N8P, K3C, H2J, P1N, N7N, A4L, N3S, W2D, W7I, Z6A, Z2L, F6X, K7K, E6I, Y3I, A4H, N4W, K1O, P8F, I2C, K1T, K8Z, Y1R, C7K, B1F, V2V, K4F, W6H, W8M, Z4H, I4M, Q3C, F6T, L9G, L1F, O7Z, P0X, A5E, R8K</t>
+          <t>Z5L, M3J, F7Q, L9E, W8Y, F1E, V0S, F0E, V1E, E4C, E8L, P5G, V7V, T0W, L9Z, V7N, E5H, O4P, J3A, S1M, J9B, Q3M, N2G, A3C, X2V, Q1E, P6B, A1Y, R6Z, L1Z, Q7D, G2E, Z1O, B9Z, V4A, V2M, T5B, F9R, E0E, N7W, W0W, F7X, I8X, S1Y, O1F, P0S, C0Q, Z3B, J9D, Q1S, O2Q, V9H, F3C, W2V, N0C, K7V, Z0V, P8C, C9I, K5V, J3P, B5N, Q0I, G0U, Z1U, C9M, Q5V, D7P, I1I, W2S, I2U, A1Q, D3Z, D4T, C7P, Q6T, Z3P, Q4T, W5Y, K4K, F7I, C2L, O7U, V8R, X4H, Z2K, K6O, S5Q, Y4F, Q7L, J2W, W6M, P9G, N6R, B1E, Z0F, K1A, B9V, E3H, A6E, I4B, Z1F, U3K, E5T, I6H, C2T, K0T, J1K, E9W, Z3T, O5O, X2P, C5T, E6J, Y3M, T3A, P1M, G0O, N3B, N6T, O2I, K5P, Q3Z, Z4I, Q5Q, H1X, Q4K, O8U, O6D, K0O, F3K, C3U, D0S, B1G, P2L, Q8Z, F7A, D4B, G3H, E9J, E5A, N3K, W5M, W4G, F0V, G0D, V7J, I1V, X1K, V5Q, E4B, R2K, W7E, P9E, Z0A, F2J, M0L, C8R, I3D, L1T, C0T, W4H, W0V, T1R, V8B, Q0W, C7A, Q6D, Q7I, Z9H, W1E, N9Y, N4M, X2A, O8A, A5R, R2E, R9Z, E1E, I6L, T2I, A5J, C9Q, W5E, Z8Q, P2M, B2F, E2L, K6L, W1F, Q1B, Y4A, U1V, W7T, E6Y, V0T, L2B, O8D, K0X, A2Z, V2G, V5R, Z2Y, F6L, W4O, L1I, Q7Q, P9P, V5X, V1W, P0B, Z8N, D0U, R3H, Q7H, R8H, Q3R, Y4L, F9W, C5N, X3V, Q4E, F7S, P0D, N3D, W3K, C8L, K6E, Z1C, W2B, W4J, G0R, L1B, U2T, W7R, U2R, X4I, Z4J, D3G, V8N, E9F, X1E, G1D, D1B, K1Q, I4H, J4V, E6B, I4Y, Z7Q, V6H, Q2S, W1P, N8P, K3C, H2J, P1N, N7N, A4L, N3S, W2D, W7I, Z6A, Z2L, F6X, K7K, E6I, Y3I, A4H, N4W, K1O, P8F, I2C, K1T, K8Z, Y1R, C7K, B1F, V2V, K4F, W6H, W8M, Z4H, I4M, Q3C, F6T, L9G, L1F, O7Z, P0X, A5E, R8K</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -6794,7 +6954,11 @@
           <t>WDB52029786085800</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr"/>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -6810,7 +6974,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Z5L, M3L, E8L, I6W, I6Y, K4J, M9O, D9W, Y4G, I9Z, C1T, D2W, W8B, L1C, N4X, K1H, K2U, W0O, W2X, R8E, X1Q, Z0P, I1E, Z0S, K0N, C8C, S5E, E5Y, H2C, J3P, O1W, Y4V, B2D, M5R, D9G, K5A, R2U, E1E, O8B, D7B, D3F, N5X, T2I, Z0W, Q1W, A4G, E4T, U5B, I4M, D7D, J3C, V0U, P2F, W0G, W6R, G0T, F8G, V6B, U1W, S9B, F8X, Z0Z, W0P, U3V, S5C, Z6J, H8Y, O8K, A4R, U3H, C3G, E4O, C3P, R5Y, V6X, V1Q, R6S, R2E, C1Z, O2M, W3Y, O6D, D7J, N4N, Z9F, C0T, I5E, A1C, M4D, W5T, M5G, C8X, G5A, X2C, I1G, F5N, E0N, K7Y, C7R, P8A, O5N, L9A, K3W, O2D, C4F, O5M, Q9Y, W7R, R2J, F6G, W2W, C5Q, I0Y, E6B, J4V, M0I, M7U, Z0L, E4G, O2S, J2B, Q6K, E6A, F1C, K3E, A1F, O1F, V7G, S1D, C2J, E1O, Z8D, S5D, E9G, F2Q, D3Y, L9W, Q3E, O9I, F2E, I1H, C4I, E9C, K4V, P9Z, J2H, K6B, V2A, M4Y, Q1U, N1J, X3C, X3Z, X4L, Q7U, O4L, Q0N, X3P, C6S, W4T, W2J, Z8H, F7Q, Z4R, N6K, G1J</t>
+          <t>Z5L, M3L, E8L, I6W, I6Y, K4J, M9O, D9W, Y4G, I9Z, C1T, D2W, W8B, L1C, N4X, K1H, K2U, W0O, W2X, R8E, X1Q, Z0P, I1E, Z0S, K0N, C8C, S5E, E5Y, H2C, J3P, O1W, Y4V, B2D, M5R, D9G, K5A, R2U, E1E, O8B, D7B, D3F, N5X, T2I, Z0W, Q1W, A4G, E4T, U5B, I4M, D7D, J3C, V0U, P2F, W0G, W6R, G0T, F8G, V6B, U1W, S9B, F8X, Z0Z, W0P, U3V, S5C, Z6J, H8Y, O8K, A4R, U3H, C3G, E4O, C3P, R5Y, V6X, V1Q, R6S, R2E, C1Z, O2M, W3Y, O6D, D7J, N4N, Z9F, C0T, I5E, A1C, M4D, W5T, M5G, C8X, G5A, X2C, I1G, F5N, E0N, K7Y, C7R, P8A, O5N, L9A, K3W, O2D, C4F, O5M, Q9Y, W7R, R2J, F6G, W2W, C5Q, I0Y, E6B, J4V, M7U, Z0L, E4G, O2S, J2B, Q6K, E6A, F1C, K3E, A1F, O1F, V7G, S1D, C2J, E1O, Z8D, S5D, E9G, F2Q, D3Y, L9W, Q3E, O9I, F2E, I1H, C4I, E9C, K4V, P9Z, J2H, K6B, V2A, M4Y, Q1U, N1J, X3C, X3Z, X4L, Q7U, O4L, Q0N, X3P, C6S, W4T, W2J, Z8H, F7Q, Z4R, N6K, G1J</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -6818,7 +6982,11 @@
           <t>NMB87558327145933</t>
         </is>
       </c>
-      <c r="F234" t="inlineStr"/>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -6898,7 +7066,11 @@
           <t>WDB19541968144805</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr"/>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -6942,7 +7114,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Z5C, M2D, Q1F, W4Z, V7E, U1R, K1J, F6P, T1D, P5Y, P9A, U1W, I2K, A1Q, J9K, V6S, X3Y, W1M, F3Q, I4L, N5L, X3Q, F8M, P9X, P6L, N0Z, H8W, C2V, F9W, C0Q, B2E, I5Q, E2T, P5A, Q2F, N5V, B1H, F2A, Z1R, K1R, F1N, Z2M, G1I, J9E, W5E, E5B, L3E, K2B, F1F, N8M, T3N, F5H, U9Z, F5I, F9Y, E4O, C9E, F6K, R2Z, Y1T, X1B, Q2J, Z2I, K1X, Y4V, Q4C, Q9Z, K7A, E0N, N7K, Z2G, K1W, V7Y, F6D, O7T, J1K, Z9W, Q0X, A6F, S5Q, I6L, Z0R, B5B, Q6S, F8G, K1V, Z1E, N0E, A3C, V8Q, U8C, M5U, F1S, S5A, D3O, A5P, F5A, Q9C, W3U, M0Z, G0B, F0S, Q4H, F6Y, C3L, H1P, M4D, X2X, J3P, P0C, H1Y, F4I, V2G, E1A, L2T, R5W, O7E, K1Y, E0D, M0C, O1A, D1C, K6X, K6Q, W7A, Z7W, K4K, R7H, C0G, V7K, C6J, U3V, M1E, I6F, A1Z, J2U, P8Z, I5F, S5J, N8I, I5R, D6Y, P0S, Z0O, R4L, J3V, L1F, Y1O, K2U, F6M, D3C, E9Z, S6F, I4R, I5Y, R3H, N2D, T2K, I2D, K8Z, K0V, W0Z, J3J, C4F, K1C, K1E, Z5V, I4K, Q8T, V1G, G5A, N1M, Q6V, H8X, P2D, O2I, R8H, Q5U, W2L, W9S, B1I, Z5W, Z5A, F9B, W0R, Z5I, K1A, X1Z, Y9V, D3E, E3W, I7G, E6L, C3P, D5O, D3X, V8X, O1O, F1T, F9Q, D9E, W0N, N4D, J6Z, Z6S, N5J, P5B, G4C, C8L, A4P, M8P, W3C, I2I, C9N, C4V, F5P, W7J, Z3K, A4S, Q0C, Y4P, O2R, I4E, L9B, K6D, N8K, E0K, P4A, C1Q, J1C, V1U, X3F, T1N, Q8D, M5X, C9X, C6U, C6Z, F8J, R4D, S5K, Y3E, Q5D, R1W, Z8H, C0W, C7Y, E7C, F7G, T1Z, E5L, K3R, C5S, X1K, Z0Y, H8R, W2F, Z2B, P0V, Y6A, J2A, D3D, O4J, P7U, R1D, A9Z, N7Q, E0Y, P5F, W3P, Z7R, V8A, O6T, K7C, F3K, E5H, I1C, J3T, M0F, Z8I, E3M, A3D, F7V, E1P, Q0V, G3A, K0Q, T0H, Y6E, J3D, D8A, Q2I, V7V, C2L, R8F, V2L, Z7Y</t>
+          <t>Z5C, M2D, Q1F, W4Z, V7E, U1R, K1J, F6P, T1D, P5Y, P9A, U1W, I2K, A1Q, J9K, V6S, X3Y, W1M, F3Q, I4L, N5L, X3Q, F8M, P9X, P6L, N0Z, H8W, C2V, F9W, C0Q, B2E, I5Q, E2T, P5A, Q2F, N5V, B1H, F2A, Z1R, K1R, F1N, Z2M, G1I, J9E, W5E, E5B, L3E, K2B, F1F, N8M, T3N, F5H, U9Z, F5I, F9Y, E4O, C9E, F6K, R2Z, Y1T, X1B, Q2J, Z2I, K1X, Y4V, Q4C, Q9Z, K7A, E0N, N7K, Z2G, K1W, V7Y, F6D, O7T, J1K, Z9W, Q0X, A6F, S5Q, I6L, Z0R, B5B, Q6S, F8G, K1V, Z1E, N0E, A3C, V8Q, U8C, M5U, F1S, S5A, D3O, A5P, F5A, Q9C, W3U, M0Z, G0B, F0S, Q4H, F6Y, C3L, H1P, M4D, X2X, J3P, P0C, H1Y, F4I, V2G, E1A, L2T, R5W, O7E, K1Y, E0D, M0C, O1A, D1C, K6X, K6Q, W7A, Z7W, K4K, R7H, C0G, V7K, C6J, U3V, M1E, I6F, A1Z, J2U, P8Z, I5F, S5J, N8I, I5R, D6Y, P0S, Z0O, R4L, J3V, L1F, Y1O, K2U, F6M, D3C, E9Z, S6F, I4R, I5Y, R3H, N2D, T2K, I2D, K8Z, K0V, W0Z, J3J, C4F, K1C, K1E, Z5V, I4K, Q8T, V1G, G5A, N1M, Q6V, H8X, P2D, O2I, R8H, Q5U, W2L, W9S, B1I, Z5W, F9B, W0R, Z5I, K1A, X1Z, Y9V, D3E, E3W, I7G, E6L, C3P, D5O, D3X, V8X, O1O, F1T, F9Q, D9E, W0N, N4D, J6Z, Z6S, N5J, P5B, G4C, C8L, A4P, M8P, W3C, I2I, C9N, C4V, F5P, W7J, Z3K, A4S, Q0C, Y4P, O2R, I4E, L9B, K6D, N8K, E0K, P4A, C1Q, J1C, V1U, X3F, T1N, Q8D, M5X, C9X, C6U, C6Z, F8J, R4D, S5K, Y3E, Q5D, R1W, Z8H, C0W, C7Y, E7C, F7G, T1Z, E5L, K3R, C5S, X1K, Z0Y, H8R, W2F, Z2B, P0V, Y6A, J2A, D3D, O4J, P7U, R1D, A9Z, N7Q, E0Y, P5F, W3P, Z7R, V8A, O6T, K7C, F3K, E5H, I1C, J3T, M0F, Z8I, E3M, A3D, F7V, E1P, Q0V, G3A, K0Q, T0H, Y6E, J3D, D8A, Q2I, V7V, C2L, R8F, V2L, Z7Y</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -7034,7 +7206,11 @@
           <t>WEB89368702562927</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr"/>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -7142,7 +7318,11 @@
           <t>W1T45624948667139</t>
         </is>
       </c>
-      <c r="F246" t="inlineStr"/>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -7214,7 +7394,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Z5E, M3C, Z9Y, C1U, Z4L, P0E, N3K, F1H, R1Q, C0O, O8D, Z7Q, E1F, P5A, P5X, O2C, O7L, E4X, Q6S, K5E, X1L, K9V, F7X, K3Y, A6R, R5R, D2O, I0U, D4U, D4C, K1Y, Q1O, L1F, Y4W, C1W, F4J, D3I, D7W, Z5A, O4J, K1Q, F4Z, Q3L, Z3W, D9R, Z8T, V1N, C9U, A4Y, B5E, W1A, O3B, Q1I, Q8A, F2U, P0Q, C0D, Q8L, F1O, D0E, F5G, W2C, F2C, V0Y, T0S, P1M, D3F, R5A, V6C, A6A, F2W, M8D, Q1C, Q8N, R1P, T3K, Y4Y, O8E, O6E, T0Q, H2E, H1K, N1N, C3K, K5K, M0W, K4V, A2G, Z0W, C0X, Q1G, X2Z, T2T, F2Q, T0Z, A3B, Z6E, G5F, G0G, C3J, K6R, J1T, U6D, U2L, Z0C, X4E, D9M, W3L, R1X, F6Q, I9I, K6S, Z0T, I2B, Q0I, J1V, N4E, C1L, O4M, K7V, D1T, F3P, I5P, X3O, N0H, A2C, K7D, W7R, V1M, I6L, R2C, W5U, W9P, F8B, E1I, P2B, Z8R, L9Z, C5T, N7W, C2P, Z2K, W3D, I5F, W8E, V7O, B9V, B2Z, T2Z, R5W, Z3B, I5Q, X4N, F0T, U7L, W9R, R2H, Z6G, Z8V, L0Y, M5K, Q1F, P0F, T2K, F1K, V3L, D9N, O7X, B4L, G1E, P1D, A3A, O7S, N4F, O6S, A5Q, E0C, H1I, T0I, F2Z, X1W, Z3O, Q1U, E9Z, E9D, Y9W, F6P, D1X, I9Y, F6N, W8P, O7I, B3G, N7C, O6N, C8W, R6C, F0S, M5N, K0D, P2P, J9Z, C3R, I5M, Z5P, P7P, P9P, Y1C, M6B, O6D, R1U, V2K, S8A, W5F, O0F, W7Y, M5Z, K0X, V0T, K6E, Q2V, J9B, W1X, G2D, X4G, G5G, T5A, L1P, M6D, U1F, M5R, Y3F, Q1Z, Q1B, F8V, P4Y, C5G, X3V, B1V, Q4N, A6I, K7S, S9Z, D3D, V5R, Z5Z, X3Y, X4C, R6U, R0T, I0Y, I5X, B1H, Q3T, S5K, P5P, D1U, M0E, R2Y, B2F, T0K, X2W, D1L, T0G, B0A, U0O, U2Q, D6W, E1P, U1V, J9N, Y1X, C7D, Q4L, N5N, F5J, Q6W, Z1V, T2A, C7I, F6L</t>
+          <t>Z5E, M3C, Z9Y, C1U, Z4L, P0E, N3K, F1H, R1Q, C0O, O8D, Z7Q, E1F, P5A, P5X, O2C, O7L, E4X, Q6S, K5E, X1L, K9V, F7X, K3Y, A6R, R5R, D2O, I0U, D4U, D4C, K1Y, Q1O, L1F, Y4W, C1W, F4J, D3I, D7W, O4J, K1Q, F4Z, Q3L, Z3W, D9R, Z8T, V1N, C9U, A4Y, B5E, W1A, O3B, Q1I, Q8A, F2U, P0Q, C0D, Q8L, F1O, D0E, F5G, W2C, F2C, V0Y, T0S, P1M, D3F, R5A, V6C, A6A, F2W, M8D, Q1C, Q8N, R1P, T3K, Y4Y, O8E, O6E, T0Q, H2E, H1K, N1N, C3K, K5K, M0W, K4V, A2G, Z0W, C0X, Q1G, X2Z, T2T, F2Q, T0Z, A3B, Z6E, G5F, G0G, C3J, K6R, J1T, U6D, U2L, Z0C, X4E, D9M, W3L, R1X, F6Q, I9I, K6S, Z0T, I2B, Q0I, J1V, N4E, C1L, O4M, K7V, D1T, F3P, I5P, X3O, N0H, A2C, K7D, W7R, V1M, I6L, R2C, W5U, W9P, F8B, E1I, P2B, Z8R, L9Z, C5T, N7W, C2P, Z2K, W3D, I5F, W8E, V7O, B9V, B2Z, T2Z, R5W, Z3B, I5Q, X4N, F0T, U7L, W9R, R2H, Z6G, Z8V, L0Y, M5K, Q1F, P0F, T2K, F1K, V3L, D9N, O7X, B4L, G1E, P1D, A3A, O7S, N4F, O6S, A5Q, E0C, H1I, T0I, F2Z, X1W, Z3O, Q1U, E9Z, E9D, Y9W, F6P, D1X, I9Y, F6N, W8P, O7I, B3G, N7C, O6N, C8W, R6C, F0S, M5N, K0D, P2P, J9Z, C3R, I5M, Z5P, P7P, P9P, Y1C, M6B, O6D, R1U, V2K, S8A, W5F, O0F, W7Y, M5Z, K0X, V0T, K6E, Q2V, J9B, W1X, G2D, X4G, G5G, T5A, L1P, M6D, U1F, M5R, Y3F, Q1Z, Q1B, F8V, P4Y, C5G, X3V, B1V, Q4N, A6I, K7S, S9Z, D3D, V5R, Z5Z, X3Y, X4C, R6U, R0T, I0Y, I5X, B1H, Q3T, S5K, P5P, D1U, M0E, R2Y, B2F, T0K, X2W, D1L, T0G, B0A, U0O, U2Q, D6W, E1P, U1V, J9N, Y1X, C7D, Q4L, N5N, F5J, Q6W, Z1V, T2A, C7I, F6L</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -7390,7 +7570,11 @@
           <t>NMB14264292803256</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr"/>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -7462,7 +7646,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Z5L, M3J, W0O, M7J, C2L, C0Z, D3Y, K2W, U3V, F1K, I4B, E5F, D6R, P6L, H2J, Z3Z, A6E, B5F, G3I, K2Z, R8F, O2G, C3M, Z5P, Q7A, V7H, E1M, A1M, P0B, G3N, Q6I, F0A, I5Y, C8Y, K4N, V7J, K9V, Y4X, V9A, I3L, S8A, Z5A, Z1H, W2S, E1G, N8K, F0K, J2Z, D5I, A6Q, L9F, Z3G, Q4R, A1Q, X9V, C8B, L1L, D9Q, P9B, N1Z, V8W, H8R, I1A, F7R, W3N, V7X, U1C, Z3S, D7F, C3F, Q1W, B3G, E2F, C3E, X3C, C0L, M5L, W2A, E3B, M0F, C9J, V6U, L9C, W4B, O7J, N4X, W5R, D0P, Y3E, E5I, B5B, Q1H, E3A, U1P, L2M, W2O, K6Q, V7M, M5H, Y4U, F5K, Z7L, X1Y, P6J, C2P, C3Q, O3C, R5N, T3L, X3R, H1X, R6M, I9I, E0V, W1C, N3U, K4U, D5O, C7T, C2R, I2N, Z8K, O2L, F0I, N6Z, G4H, R1R, Q6L, W9G, O5U, P9F, J1V, E1R, G2G</t>
+          <t>Z5L, M3J, W0O, M7J, C2L, C0Z, D3Y, K2W, U3V, F1K, I4B, E5F, D6R, P6L, H2J, Z3Z, A6E, B5F, G3I, K2Z, R8F, O2G, C3M, Z5P, Q7A, V7H, E1M, A1M, P0B, G3N, Q6I, F0A, I5Y, C8Y, K4N, V7J, K9V, Y4X, V9A, I3L, S8A, Z1H, W2S, E1G, N8K, F0K, J2Z, D5I, A6Q, L9F, Z3G, Q4R, A1Q, X9V, C8B, L1L, D9Q, P9B, N1Z, V8W, H8R, I1A, F7R, W3N, V7X, U1C, Z3S, D7F, C3F, Q1W, B3G, E2F, C3E, X3C, C0L, M5L, W2A, E3B, M0F, C9J, V6U, L9C, W4B, O7J, N4X, W5R, D0P, Y3E, E5I, B5B, Q1H, E3A, U1P, L2M, W2O, K6Q, V7M, M5H, Y4U, F5K, Z7L, X1Y, P6J, C2P, C3Q, O3C, R5N, T3L, X3R, H1X, R6M, I9I, E0V, W1C, N3U, K4U, D5O, C7T, C2R, I2N, Z8K, O2L, F0I, N6Z, G4H, R1R, Q6L, W9G, O5U, P9F, J1V, E1R, G2G</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -7470,7 +7654,11 @@
           <t>NMB72344209803907</t>
         </is>
       </c>
-      <c r="F258" t="inlineStr"/>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -7494,7 +7682,11 @@
           <t>WDB12124059592712</t>
         </is>
       </c>
-      <c r="F259" t="inlineStr"/>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -7510,7 +7702,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Z5L, M3L, D1C, D8A, W7V, T4A, P0S, R3Q, P0Y, S8B, Y4D, Q6Q, S5P, E1S, X9Z, Z0J, I2G, P2P, U1C, C2P, J8W, Q4D, F7G, W5D, T2Z, B5L, Y4V, F6T, G4I, W0V, T1H, F6P, Z4A, I6H, U3A, Q7B, Q1X, O8C, P6Q, Z7P, W6G, D0K, P6E, W2J, A2C, V2I, K1P, L2L, Z8K, Z1Z, F2O, W9S, Q8F, U3R, X1M, N1I, Q7A, N4L, E4M, E0F, E5B, J9F, C4P, W4E, F6N, P7T, F0Z, Z9Y, J6A, Z3X, O5N, I4E, R1Q, F2X, P2C, G1I, V1D, A2B, U3M, D9C, Q4J, I4Y, D6Y, Q1D, D1A, C6G, E9L, D1V, L1B, Q5A, F7I, U2F, C6C, Q4T, M0I, X2E, K4N, R5E, Y4I, X1V, G3A, E2N, A2O, F4Y, J2O, M0B, C2H, K4O, E9F, F7Y, F2U, Q2L, C1L, J1Z, F8C, V6P, V0Z, V8W, K6M, H1V, T3N, P8Z, Z2C, Z3L, J3D, R1U, G4D, E1C, G1B, W5C, W3B, W3L, Q2S, R7B, E5T, S5L, I6M, E6K, A2J, D3B, R7H, Z2Z, W7L, W5K, P2K, Z1J, K5G, J1R, R0Z, L9I, A2E, Z6B, R3P, K5V, C6E, K6L, D5X, X3Q, D0B, F6C, C1X, I4C, I4B, Q7F, R4Z, X1A, V1W, F3P, C9M, F1V, I5S, Q2E, K4L, B9W, C5U, D3Z, M1B, Y2A, R6X, E3V, N7O, F5K, A5W, Y1Y, C3K, R1R, C7Q, R1X, E0E, J1Q, E6I, A5I, A2F, A5H, G2H, E1B, W4O, Z0L, F6M, H1Y, N4G, R8O, N3M, Z5Q, Q5N, K0G, C4X, V7C, X9V, Q0Y, T1K, U3G, F8N, K3Q, V6A, C5P, U8Z, R1M, W7D, N6I, Z5P, P5F, D3S, C3R, Q6N, K0F, T0V, Z5T</t>
+          <t>Z5L, M3L, D1C, D8A, W7V, T4A, P0S, R3Q, P0Y, S8B, Y4D, Q6Q, S5P, E1S, X9Z, Z0J, I2G, P2P, U1C, C2P, J8W, Q4D, F7G, W5D, T2Z, B5L, Y4V, F6T, G4I, W0V, T1H, F6P, Z4A, I6H, U3A, Q7B, Q1X, O8C, P6Q, Z7P, W6G, D0K, P6E, W2J, A2C, V2I, K1P, L2L, Z8K, Z1Z, F2O, W9S, Q8F, U3R, X1M, N1I, Q7A, N4L, E4M, E0F, E5B, J9F, C4P, W4E, F6N, P7T, F0Z, Z9Y, J6A, Z3X, O5N, I4E, R1Q, F2X, P2C, G1I, V1D, A2B, U3M, D9C, Q4J, I4Y, D6Y, Q1D, D1A, C6G, E9L, D1V, L1B, Q5A, F7I, U2F, C6C, Q4T, X2E, K4N, R5E, Y4I, X1V, G3A, E2N, A2O, F4Y, J2O, M0B, C2H, K4O, E9F, F7Y, F2U, Q2L, C1L, J1Z, F8C, V6P, V0Z, V8W, K6M, H1V, T3N, P8Z, Z2C, Z3L, J3D, R1U, G4D, E1C, G1B, W5C, W3B, W3L, Q2S, R7B, E5T, S5L, I6M, E6K, A2J, D3B, R7H, Z2Z, W7L, W5K, P2K, Z1J, K5G, J1R, R0Z, L9I, A2E, Z6B, R3P, K5V, C6E, K6L, D5X, X3Q, D0B, F6C, C1X, I4C, I4B, Q7F, R4Z, X1A, V1W, F3P, C9M, F1V, I5S, Q2E, K4L, B9W, C5U, D3Z, M1B, Y2A, R6X, E3V, N7O, F5K, A5W, Y1Y, C3K, R1R, C7Q, R1X, E0E, J1Q, E6I, A5I, A2F, A5H, G2H, E1B, W4O, Z0L, F6M, H1Y, N4G, R8O, N3M, Z5Q, Q5N, K0G, C4X, V7C, X9V, Q0Y, T1K, U3G, F8N, K3Q, V6A, C5P, U8Z, R1M, W7D, N6I, Z5P, P5F, D3S, C3R, Q6N, K0F, T0V, Z5T</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
@@ -7518,7 +7710,11 @@
           <t>WDB55750311594623</t>
         </is>
       </c>
-      <c r="F260" t="inlineStr"/>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -7598,7 +7794,11 @@
           <t>NMB56309403508880</t>
         </is>
       </c>
-      <c r="F263" t="inlineStr"/>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -7670,7 +7870,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Z5E, M3D, F6D, K1S, W0M, L2I, K4F, Z4J, W1S, V1L, X3Z, E1H, K1H, G0K, Q8W, F5N, V2T, E9E, V1X, J3M, O4S, Q7J, Z7L, Z3E, O6J, D3W, Z7M, P1A, C9N, S5Q, Z3A, F6L, C0Z, R0V, V6C, N0N, D0E, I0U, W6H, C2O, P9Z, E8L, A6K, N0X, O2C, M8B, W1U, F7G, R4Y, V7S, T0T, O7Q, Z5O, X3Y, D6N, C0A, G0Z, K5O, V7C, Q2S, Q2F, Z9G, I1I, P0A, K7Y, D6Z, C2H, D1L, I1P, K5K, S1E, U2S, U1A, Q3D, E1R, F8L, L1Q, D0C, Q7R, J3U, O8M, F1I, Q0F, K5L, S5K, Z9E, P0X, K0V, F2U, R7K, V2A, K0L, C6P, Q2R, E6B, Q4F, D0I, D7B, W9Z, F7D, F5B, E4X, C6E, W2I, D0P, D2K, V3A, N3M, K6P, W6E, W4C, M6M, N1M, C4R, D6J, X4A, Z9Z, U8B, Q7D, T1D, E2J, N5M, W3B, I1Y, M9O, A2A, I7Y, R1H, E4F, E3V, Q3M, J3Y, V6I, P5P, C0O, V5T, P4W, Z8S, C6D, C7K, P1J, R1G, U1E, G5F, J1C, V9B, A1H, I5Y, D5J, P1C, C1X, R8B, W4Z, M7U, D6R, O6T, C6M, O8D, E1F, X2X, F7Q, Z6I, M0I, T3S, J2U, A5F, H1Q, Q5V, P8Y, Q4W, R9X, D5Q, N5A, A2F, E5K, N7F, N5V, M8Y, B1H, O0E, N1T, Q2I, N5D, W2Q, T1X, F7B, W4S, C1M, G0B, H1P, C6G, B5A, V9Q, W8C, I5H, A2L, T0N, C3F, A6B, V1K, Q9W, C3T, K1Q, L1C, A1T, K3Q, C4B, V7R, I1V, N9X, V4Y, D3U, V7F, C1Z, T1Z, C2E, E5G, O2Q, M1E, F5Q, P9C, N7L, H8U, F6W, Z2J, Z4U, Q8F, J9J, M5C, W2D, L9E, F2B, V2P, F7T, P9H, C6X, E3Z, X1V, O7B, N4G, O2D, R5I, L2M, R2K, Q8I, C8X, W1M</t>
+          <t>Z5E, M3D, F6D, K1S, W0M, L2I, K4F, Z4J, W1S, V1L, X3Z, E1H, K1H, G0K, Q8W, F5N, V2T, E9E, V1X, J3M, O4S, Q7J, Z7L, Z3E, O6J, D3W, Z7M, P1A, C9N, S5Q, Z3A, F6L, C0Z, R0V, V6C, N0N, D0E, I0U, W6H, C2O, P9Z, E8L, A6K, N0X, O2C, M8B, W1U, F7G, R4Y, V7S, T0T, O7Q, Z5O, X3Y, D6N, C0A, G0Z, K5O, V7C, Q2S, Q2F, Z9G, I1I, P0A, K7Y, D6Z, C2H, D1L, I1P, K5K, S1E, U2S, U1A, Q3D, E1R, F8L, L1Q, D0C, Q7R, J3U, O8M, F1I, Q0F, K5L, S5K, Z9E, P0X, K0V, F2U, R7K, V2A, K0L, C6P, Q2R, E6B, Q4F, D0I, D7B, W9Z, F7D, F5B, E4X, C6E, W2I, D0P, D2K, V3A, N3M, K6P, W6E, W4C, M6M, N1M, C4R, D6J, X4A, Z9Z, U8B, Q7D, T1D, E2J, N5M, W3B, I1Y, M9O, A2A, I7Y, R1H, E4F, E3V, Q3M, J3Y, V6I, P5P, C0O, V5T, P4W, Z8S, C6D, C7K, P1J, R1G, U1E, G5F, J1C, V9B, A1H, I5Y, D5J, P1C, C1X, R8B, W4Z, M7U, D6R, O6T, C6M, O8D, E1F, X2X, F7Q, Z6I, T3S, J2U, A5F, H1Q, Q5V, P8Y, Q4W, R9X, D5Q, N5A, A2F, E5K, N7F, N5V, M8Y, B1H, O0E, N1T, Q2I, N5D, W2Q, T1X, F7B, W4S, C1M, G0B, H1P, C6G, B5A, V9Q, W8C, I5H, A2L, T0N, C3F, A6B, V1K, Q9W, C3T, K1Q, L1C, A1T, K3Q, C4B, V7R, I1V, N9X, V4Y, D3U, V7F, C1Z, T1Z, C2E, E5G, O2Q, M1E, F5Q, P9C, N7L, H8U, F6W, Z2J, Z4U, Q8F, J9J, M5C, W2D, L9E, F2B, V2P, F7T, P9H, C6X, E3Z, X1V, O7B, N4G, O2D, R5I, L2M, R2K, Q8I, C8X, W1M</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
@@ -7762,7 +7962,11 @@
           <t>WEB93654034433516</t>
         </is>
       </c>
-      <c r="F269" t="inlineStr"/>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -7926,7 +8130,11 @@
           <t>W1T94299307726332</t>
         </is>
       </c>
-      <c r="F275" t="inlineStr"/>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -7970,7 +8178,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Z5L, M3H, M5O, H1N, Q6Z, F5B, O1C, K7S, D4U, Z5Y, O2S, E7L, P5H, Y3K, B1Z, F1Y, P2K, P1M, U3G, Q5K, C1C, D0J, V1B, W6U, M6O, U3V, A6H, Z7P, W3U, E4D, J2W, V1J, E5L, N8Q, R5Z, K3J, E3G, D4X, Y1A, G4D, F8F, O0A, V2G, V6V, M5H, O7Q, Z5K, W5X, R8D, C9C, I1T, Q7A, N0X, M2I, U6A, Z8A, R8C, C2T, E0F, A1Q, L2R, Z0K, X2M, Z6B, E2L, V2R, V4N, I6H, P6E, U2Y, Q5S, D8Z, W4O, P5X, I5J, F4Z, F6R, C5O, W7H, Q2I, D2L, W5Y, E5G, C1Z, V8A, L3A, O1M, D2C, F1C, X4K, Q7Z, Y4D, E5K, N4Y, Z3S, V7Z, E7F, P7Q, O7C, N0N, D0V, R8B, W2B, K7W, Y1Z, R5Y, C3G, V1Q, F0F, V8Y, V2V, Y9Z, Y4Z, E5H, Q7K, M7U, A4F, A2T, Z2R, O7R, X6A, K6K, A2E, P6G, K1Q, A9Z, E7T, A4M, H1B, E1F, D9Z, F2C, Q2F, V1I, Q6P, Q5A, V7G, Z6L, Z2H, V6T, Q6N, Z1H, F1K, V7V, Z4D, C4X, C0Z, I5H, A4A, Q1W, A1M, Q3W, D2N, W5H, Q7V, F7B, M1B, K2E, E4L, K9V, Q0H, N4D, S1L, K5U, F5G, W6Y, V3F, N7P, O7O, T0P, C4M, E4F, U5A, M0S, F1Q, Z5A, E3J, M9Z, Q6M</t>
+          <t>Z5L, M3H, M5O, H1N, Q6Z, F5B, O1C, K7S, D4U, Z5Y, O2S, E7L, P5H, Y3K, B1Z, F1Y, P2K, P1M, U3G, Q5K, C1C, D0J, V1B, W6U, M6O, U3V, A6H, Z7P, W3U, E4D, J2W, V1J, E5L, N8Q, R5Z, K3J, E3G, D4X, Y1A, G4D, F8F, O0A, V2G, V6V, M5H, O7Q, Z5K, W5X, R8D, C9C, I1T, Q7A, N0X, M2I, U6A, Z8A, R8C, C2T, E0F, A1Q, L2R, Z0K, X2M, Z6B, E2L, V2R, V4N, I6H, P6E, U2Y, Q5S, D8Z, W4O, P5X, I5J, F4Z, F6R, C5O, W7H, Q2I, D2L, W5Y, E5G, C1Z, V8A, L3A, O1M, D2C, F1C, X4K, Q7Z, Y4D, E5K, N4Y, Z3S, V7Z, E7F, P7Q, O7C, N0N, D0V, R8B, W2B, K7W, Y1Z, R5Y, C3G, V1Q, F0F, V8Y, V2V, Y9Z, Y4Z, E5H, Q7K, M7U, A4F, A2T, Z2R, O7R, X6A, K6K, A2E, P6G, K1Q, A9Z, E7T, A4M, H1B, E1F, D9Z, F2C, Q2F, V1I, Q6P, Q5A, V7G, Z6L, Z2H, V6T, Q6N, Z1H, F1K, V7V, Z4D, C4X, C0Z, I5H, A4A, Q1W, A1M, Q3W, D2N, W5H, Q7V, F7B, M1B, K2E, E4L, K9V, Q0H, N4D, S1L, K5U, F5G, W6Y, V3F, N7P, O7O, T0P, C4M, E4F, U5A, M0S, F1Q, E3J, M9Z, Q6M</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -7978,7 +8186,11 @@
           <t>WDB75619285356480</t>
         </is>
       </c>
-      <c r="F277" t="inlineStr"/>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -8022,7 +8234,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Z5B, M1J, X1C, W4P, Y9A, R4L, T8A, I5F, F1V, A1K, O1Y, V8A, P8D, K0A, N6T, N7G, F8C, W3H, D3H, P8M, Q1S, F0R, Y9W, N1M, S5I, S5D, J2J, A2T, C8S, F1I, M5Z, Q0I, W0F, X1W, S1S, M4Y, A1S, R6B, D2X, Z5A, S5F, J6Y, F8L, F1E, F0G, R1B, Q5N, Q1P, W7I, R6X, F1T, Z9K, S5E, P9A, X1A, C2V, R1D, Z6S, V7Q, Y4R, I0M, R7F, O8I, H8N, Z4Q, Q2O, Z4D, E4O, O7Z, W8F, C7M, N4G, V7U, C4R, N1U, K1K, F2O, K3J, R3P, N0E, Z8E, E5A, P2R, W7M, Z1R, V2B, O0G, G1Z, U3I, C1Y, V2U, P2I, Z3S, K7D, C1X, N8Q, K2C, I2R, K6I, I2Q</t>
+          <t>Z5B, M1J, X1C, W4P, Y9A, R4L, T8A, I5F, F1V, A1K, O1Y, V8A, P8D, K0A, N6T, N7G, F8C, W3H, D3H, P8M, Q1S, F0R, Y9W, N1M, S5I, S5D, J2J, A2T, C8S, F1I, M5Z, Q0I, W0F, X1W, S1S, M4Y, A1S, R6B, D2X, S5F, J6Y, F8L, F1E, F0G, R1B, Q5N, Q1P, W7I, R6X, F1T, Z9K, S5E, P9A, X1A, C2V, R1D, Z6S, V7Q, Y4R, I0M, R7F, O8I, H8N, Z4Q, Q2O, Z4D, E4O, O7Z, W8F, C7M, N4G, V7U, C4R, N1U, K1K, F2O, K3J, R3P, N0E, Z8E, E5A, P2R, W7M, Z1R, V2B, O0G, G1Z, U3I, C1Y, V2U, P2I, Z3S, K7D, C1X, N8Q, K2C, I2R, K6I, I2Q</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -8078,7 +8290,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Z5C, M2E, B5K, F9Z, Q8A, X3Q, Q7G, C0A, Q4E, Q0N, M0K, C1M, W1U, V8Y, J1R, Z8Q, L1B, T2J, W9T, I7T, D2V, V2C, M5K, P8C, C2N, R1M, I4N, R5H, Z7O, W0S, D1Q, V7F, C5J, B4Z, X3V, A6Q, V1C, N4M, Y4L, O1F, X6A, L1A, Q1T, F5L, D3H, K5U, Q2T, J2M, R5A, K0U, L1F, K8A, P0V, Z1O, N2I, U2U, A5X, R6U, Z5T, Z6A, W7D, I1G, G4E, S5A, M9S, L9V, N3C, X3O, W3G, Q3T, W5Y, J2U, O7R, N7Q, T2T, J2A, P2C, C7S, Q0W, P2N, N5I, P7U, D5Y, R2G, W2F, R7D, E2T, C2A, S5D, M8N, T0V, K5S, I6E, B4M, C7T, P1D, Q6J, Z8F, L1C, F6K, I4F, W8U, T0Z, C0F, C0D, T1K, S5K, V1Z, S9Y, E9L, C2H, I4C, D9Q, W9Z, O5N, L1Y, T2K, R1J, C2Y, J3R, W3L, C1B, E0U, Q7Q, D7N, O6N, Z4O, F1C, E8L, Q0B, W4J, M8L, R2E, T1U, N2D, G5F, O6R, D0I, Q6N, T3L, O1W, R1D, N7L, Z9Z, F9Q, I2G, C6G, Z5A, S5G, M9V, W1J, Z9F, T3S, Y1F, D4M, B4K, T1H, M5H, X1V, D6N, B5J, L9D, B2Z, P6B, K5N, P5P, Z3A, S5P, I6Y, M0J, O3A, V6U, W7X, Z3I, S5E, S1P, U1W, D0Q, Z5X, R5S, V5V, A2Z, N1H, O6P, A1N, E9K, G0Y, J2G, C0O, P4U, G1J, P9C, V5W, J3F, F2Z, P1C, O6G, R7J, Z4L, P9E, D5F, W8B, W8E, K1G, L1N, K3W, F0W, C7P, Z0P, M0T, M8Y, I6W, C6C, K1V, P0L, Q2M, A2O, V1D, O5M, F7V, Z8J, C1S, F7Y, P4Y, F2Y, T1L, M0B, F5I, O7W, Z7Z, U1R, S8D</t>
+          <t>Z5C, M2E, B5K, F9Z, Q8A, X3Q, Q7G, C0A, Q4E, Q0N, M0K, C1M, W1U, V8Y, J1R, Z8Q, L1B, T2J, W9T, I7T, D2V, V2C, M5K, P8C, C2N, R1M, I4N, R5H, Z7O, W0S, D1Q, V7F, C5J, B4Z, X3V, A6Q, V1C, N4M, Y4L, O1F, X6A, L1A, Q1T, F5L, D3H, K5U, Q2T, J2M, R5A, K0U, L1F, K8A, P0V, Z1O, N2I, U2U, A5X, R6U, Z5T, Z6A, W7D, I1G, G4E, S5A, M9S, L9V, N3C, X3O, W3G, Q3T, W5Y, J2U, O7R, N7Q, T2T, J2A, P2C, C7S, Q0W, P2N, N5I, P7U, D5Y, R2G, W2F, R7D, E2T, C2A, S5D, M8N, T0V, K5S, I6E, B4M, C7T, P1D, Q6J, Z8F, L1C, F6K, I4F, W8U, T0Z, C0F, C0D, T1K, S5K, V1Z, S9Y, E9L, C2H, I4C, D9Q, W9Z, O5N, L1Y, T2K, R1J, C2Y, J3R, W3L, C1B, E0U, Q7Q, D7N, O6N, Z4O, F1C, E8L, Q0B, W4J, M8L, R2E, T1U, N2D, G5F, O6R, D0I, Q6N, T3L, O1W, R1D, N7L, Z9Z, F9Q, I2G, C6G, S5G, M9V, W1J, Z9F, T3S, Y1F, D4M, B4K, T1H, M5H, X1V, D6N, B5J, L9D, B2Z, P6B, K5N, P5P, Z3A, S5P, I6Y, O3A, V6U, W7X, Z3I, S5E, S1P, U1W, D0Q, Z5X, R5S, V5V, A2Z, N1H, O6P, A1N, E9K, G0Y, J2G, C0O, P4U, G1J, P9C, V5W, J3F, F2Z, P1C, O6G, R7J, Z4L, P9E, D5F, W8B, W8E, K1G, L1N, K3W, F0W, C7P, Z0P, M0T, M8Y, I6W, C6C, K1V, P0L, Q2M, A2O, V1D, O5M, F7V, Z8J, C1S, F7Y, P4Y, F2Y, T1L, M0B, F5I, O7W, Z7Z, U1R, S8D</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -8282,7 +8494,11 @@
           <t>WEB32328699581060</t>
         </is>
       </c>
-      <c r="F288" t="inlineStr"/>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -8390,7 +8606,11 @@
           <t>WEB69534365810155</t>
         </is>
       </c>
-      <c r="F292" t="inlineStr"/>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -8574,7 +8794,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Z5F, M3V, V5A, O8B, Z6E, T2C, W1O, X1X, I6F, U3F, L2Q, E5A, C4L, E2N, Z8E, N8K, F5K, Y1A, R2W, N6P, D1M, C7W, J2B, G9B, Z8I, D7Z, P0L, Q7R, R3Q, K6Q, S1D, O4M, P5A, Q4W, A5L, Z2F, V6V, Q1V, X1P, D3H, Z6F, A1P, B4L, N2S, W5B, A9Z, A5X, E0Y, N8N, Q1T, U3B, V6F, D3W, F1M, E4G, V7A, Z3S, C3T, K6S, R1P, Q0C, O8L, R1O, Z9M, W5R, T3N, Q2H, U3N, F8Z, O6J, G2E, U2Y, L1P, A5F, V0X, U6E, E1N, E0D, C6F, E6J, P0S, P5F, L2T, V6P, G0Q, W2O, I5L, V2A, M4D, P2B, V5X, G0X, E5K, L4A, C4E, S1J, C0T, Z8Y, H2A, P9T, J2U, V6A, Q7Y, Z5A, J6A, J9J, Y1Z, Q2C, Z2U, Z3C, W8U, V3O, F0X, A6M, J1D, X2A, Q7M, B9Y, O3A, F9Z, K7Z, T2I, F8W, T0Q, O7I, Z1W, C7D, T2F, R1V, K1E, K3Z, M9O, O6U, P2D, M5U, Q2I, A2B, V6Q, K8X, W3N, J2W, A1O, C2G, R9X, Z5X, D5J, V3F, J1G, V0Y, X2Y, C5A, C7N, F0N, C6I, I0E, K0W, W5O, C6G, P1M, I2I, B0A, E1Q, D2M, J2O, F5D, F4H, W0V, Q1M, O6H, P9G, A2C, B5I, K6L, R6U, B3H, O0B, K0B, C9X, Q8E, F6D, V5O, Q4D, D7V, V6D, N3K</t>
+          <t>Z5F, M3V, V5A, O8B, Z6E, T2C, W1O, X1X, I6F, U3F, L2Q, E5A, C4L, E2N, Z8E, N8K, F5K, Y1A, R2W, N6P, D1M, C7W, J2B, G9B, Z8I, D7Z, P0L, Q7R, R3Q, K6Q, S1D, O4M, P5A, Q4W, A5L, Z2F, V6V, Q1V, X1P, D3H, Z6F, A1P, B4L, N2S, W5B, A9Z, A5X, E0Y, N8N, Q1T, U3B, V6F, D3W, F1M, E4G, V7A, Z3S, C3T, K6S, R1P, Q0C, O8L, R1O, Z9M, W5R, T3N, Q2H, U3N, F8Z, O6J, G2E, U2Y, L1P, A5F, V0X, U6E, E1N, E0D, C6F, E6J, P0S, P5F, L2T, V6P, G0Q, W2O, I5L, V2A, M4D, P2B, V5X, G0X, E5K, L4A, C4E, S1J, C0T, Z8Y, H2A, P9T, J2U, V6A, Q7Y, J6A, J9J, Y1Z, Q2C, Z2U, Z3C, W8U, V3O, F0X, A6M, J1D, X2A, Q7M, B9Y, O3A, F9Z, K7Z, T2I, F8W, T0Q, O7I, Z1W, C7D, T2F, R1V, K1E, K3Z, M9O, O6U, P2D, M5U, Q2I, A2B, V6Q, K8X, W3N, J2W, A1O, C2G, R9X, Z5X, D5J, V3F, J1G, V0Y, X2Y, C5A, C7N, F0N, C6I, I0E, K0W, W5O, C6G, P1M, I2I, B0A, E1Q, D2M, J2O, F5D, F4H, W0V, Q1M, O6H, P9G, A2C, B5I, K6L, R6U, B3H, O0B, K0B, C9X, Q8E, F6D, V5O, Q4D, D7V, V6D, N3K</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -8630,7 +8850,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Z5B, M1I, B5L, M2H, O4H, Q2G, O7Y, C4K, C3D, I1V, A2G, N9W, Q7Y, K5M, E9E, I2I, N7K, F2F, Z5W, O1B, F5T, U8A, P9F, F6E, D6X, R2L, C2T, I1M, A2Y, F2Z, T2T, E9F, V7M, O8M, T1W, N6U, K7P, E2R, A1J, G2D, P9R, Q4G, X4C, T1F, I4I, R1Q, W8C, C6V, U1P, T0Z, D6H, I5C, F1J, U9Z, T0X, I1C, Q2T, D4T, C8E, A1S, Q8V, F6I, D3C, C2H, N0E, E3S, B1G, O1F, Q2P, D6N, F0K, D7K, X2R, Z5K, C1X, S1J, M5F, I6F, R8P, G3Y, A5K, D5N, N7Q, Z0K, D3N, F1N, G3I, Z0H, Q6Y, G0A, I4H, D4I, D9T, C5Q, W6V, P2A, G3N, T1X, V8Q, K3W, P2J, K5L, Y3K, W4N, X2K, A1H, W1V, C7L, M6O, Z1V, S8F, D8M, F6L, J6B, Q1S, G9B, Q1Y, Q8L, B2C, A4B, V2J, K7K, W6X, E3T, N8Q, C2A, D7W, A6N, Z9Z, W6H, B1F, S1S, A0A, C8L, K1L, U3E, W1O, I5F, Q3F, R8J, Q4B, W0M, E4Y, N5H, P2Z, P7A, Z4G, U3I, P0Y, D3Z, C8Y, K5A, A4T, K3J, D1Q, B4K, Z9J, N6R, M5C, O2C, I5L, Q2I, J9K, N1T, A6Q, X3I, C2Z, E3A, F6R, Q5D, F8Z, W3A, J3A, Q6N, Q2C, Q8C, X4A, V0X, N3J, V6E, U2Q, O1D, D7X, F0N, R9Y, K6D, K6X, F3H, U3K, X1J, Q2L, P8U, A5I, K8X, Y3Z, Y3O, Z1B, I1U, N4M, L0A, I6B, F5D, C2K, N2R, A6I, R8B, K7D, Q4P, R1M, N0B, S8H, I2C, C6X, M0J, Z1M, A2I, K5E, R7J, V7F, O7I, U6D, M5H, K0G, P0W, D2U</t>
+          <t>Z5B, M1I, B5L, M2H, O4H, Q2G, O7Y, C4K, C3D, I1V, A2G, N9W, Q7Y, K5M, E9E, I2I, N7K, F2F, Z5W, O1B, F5T, U8A, P9F, F6E, D6X, R2L, C2T, I1M, A2Y, F2Z, T2T, E9F, V7M, O8M, T1W, N6U, K7P, E2R, A1J, G2D, P9R, Q4G, X4C, T1F, I4I, R1Q, W8C, C6V, U1P, T0Z, D6H, I5C, F1J, U9Z, T0X, I1C, Q2T, D4T, C8E, A1S, Q8V, F6I, D3C, C2H, N0E, E3S, B1G, O1F, Q2P, D6N, F0K, D7K, X2R, Z5K, C1X, S1J, M5F, I6F, R8P, G3Y, A5K, D5N, N7Q, Z0K, D3N, F1N, G3I, Z0H, Q6Y, G0A, I4H, D4I, D9T, C5Q, W6V, P2A, G3N, T1X, V8Q, K3W, P2J, K5L, Y3K, W4N, X2K, A1H, W1V, C7L, M6O, Z1V, S8F, D8M, F6L, J6B, Q1S, G9B, Q1Y, Q8L, B2C, A4B, V2J, K7K, W6X, E3T, N8Q, C2A, D7W, A6N, Z9Z, W6H, B1F, S1S, A0A, C8L, K1L, U3E, W1O, I5F, Q3F, R8J, Q4B, W0M, E4Y, N5H, P2Z, P7A, Z4G, U3I, P0Y, D3Z, C8Y, K5A, A4T, K3J, D1Q, B4K, Z9J, N6R, M5C, O2C, I5L, Q2I, J9K, N1T, A6Q, X3I, C2Z, E3A, F6R, Q5D, F8Z, W3A, J3A, Q6N, Q2C, Q8C, X4A, V0X, N3J, V6E, U2Q, O1D, D7X, F0N, R9Y, K6D, K6X, F3H, U3K, X1J, Q2L, P8U, A5I, K8X, Y3Z, Y3O, Z1B, I1U, N4M, L0A, I6B, F5D, C2K, N2R, A6I, R8B, K7D, Q4P, R1M, N0B, S8H, I2C, C6X, Z1M, A2I, K5E, R7J, V7F, O7I, U6D, M5H, K0G, P0W, D2U</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -8750,7 +8970,11 @@
           <t>WEB44427941409731</t>
         </is>
       </c>
-      <c r="F305" t="inlineStr"/>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -8802,7 +9026,11 @@
           <t>NMB57245777102047</t>
         </is>
       </c>
-      <c r="F307" t="inlineStr"/>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -8846,7 +9074,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Z5B, M1H, M0S, O2F, X1G, C7E, Z9M, J2B, L1Z, T1R, B2E, O6R, L1C, Z3A, I6Y, Q4Z, E0U, J8X, C6I, F9B, Z4L, A3D, E2J, L4A, K5M, Z5A, M2H, V6A, Z1F, R4Y, V5Q, V1X, Z2H, W6F, N7P, Y9X, W6P, E3C, D4A, F3P, V7J, M4D, D8Z, Q4S, O5N, P9S, F3Z, J1W, Z0K, Q4C, W4L, E6L, U3V, M9W, C9S, Z1T, V7W, H1P, I2V, E4D, W3R, W0O, S1W, Y9V, Q4F, E7F, P5B, D9L, T2Z, S1Y, C8T, B1A, E7T, N2S, E2R, C0D, X1U, U2R, H1B, F5U, E0K, N7I, R4L, R4P, F1C, Q2L, P8Y, I8X, D8L, Q5B, V6J, A6S, C6G, I5R, J2I, O2R, D5U, C9H, I1I, U3E, Z3Z, G0M, Z2W, X6A, I6F, E3T, D6E, W7S, O4J, T1Z, X2G, F6C, Q0I, S1M, C5V, P6P, C2G, Q4L, I1K, M5H, K5C, E2L, D9R, Y1A, K5E, X9Z, R6V, E9I, U2T, P1K, Z9K, Z9H, O1T, P0X, Z3Q, B2B, Z7A, W4U, D5M, V6W, C2T, T0I, Q5T, Z9Z, B2D, O1O, I2G, A5X, R5R, X2P, R7F, P6R, P6V, Z9B, Z2E, W4K, Z1E, V6Z, E1K, I5X, C1J, K1B, Y3K, I5L, Z3F, S1C, P9A, D9A, L2K, K2W, E9E, B1H, O7L, R8J, G1J, C3F, O0E, Z9W, R1P, L1I, R9Y, T0X, W3E, A4W, A2T, E4T, D5C, Z4N, D3B, Z3K, W7G, Z9I, W3W, Q5P, F8X, V1W, A6L</t>
+          <t>Z5B, M1H, M0S, O2F, X1G, C7E, Z9M, J2B, L1Z, T1R, B2E, O6R, L1C, Z3A, I6Y, Q4Z, E0U, J8X, C6I, F9B, Z4L, A3D, E2J, L4A, K5M, M2H, V6A, Z1F, R4Y, V5Q, V1X, Z2H, W6F, N7P, Y9X, W6P, E3C, D4A, F3P, V7J, M4D, D8Z, Q4S, O5N, P9S, F3Z, J1W, Z0K, Q4C, W4L, E6L, U3V, M9W, C9S, Z1T, V7W, H1P, I2V, E4D, W3R, W0O, S1W, Y9V, Q4F, E7F, P5B, D9L, T2Z, S1Y, C8T, B1A, E7T, N2S, E2R, C0D, X1U, U2R, H1B, F5U, E0K, N7I, R4L, R4P, F1C, Q2L, P8Y, I8X, D8L, Q5B, V6J, A6S, C6G, I5R, J2I, O2R, D5U, C9H, I1I, U3E, Z3Z, G0M, Z2W, X6A, I6F, E3T, D6E, W7S, O4J, T1Z, X2G, F6C, Q0I, S1M, C5V, P6P, C2G, Q4L, I1K, M5H, K5C, E2L, D9R, Y1A, K5E, X9Z, R6V, E9I, U2T, P1K, Z9K, Z9H, O1T, P0X, Z3Q, B2B, Z7A, W4U, D5M, V6W, C2T, T0I, Q5T, Z9Z, B2D, O1O, I2G, A5X, R5R, X2P, R7F, P6R, P6V, Z9B, Z2E, W4K, Z1E, V6Z, E1K, I5X, C1J, K1B, Y3K, I5L, Z3F, S1C, P9A, D9A, L2K, K2W, E9E, B1H, O7L, R8J, G1J, C3F, O0E, Z9W, R1P, L1I, R9Y, T0X, W3E, A4W, A2T, E4T, D5C, Z4N, D3B, Z3K, W7G, Z9I, W3W, Q5P, F8X, V1W, A6L</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -8874,7 +9102,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Z5L, M3M, W2D, W2K, R1H, W1G, V3O, G3H, P4U, A1X, G5Z, B5F, L2P, T1H, P7R, C3M, I1G, W9F, K2X, R1T, N4C, M2H, D9T, E9X, R8E, K1K, Z9K, Q2F, K4F, K2L, N1Y, L1D, C2E, F6F, R6Z, E5Z, Z6I, H1K, Q2M, R3K, Z7O, W0N, K0I, H8Y, W5R, A4P, E8A, Y1A, W3T, Z6G, H1X, N1H, I1P, N4L, E5U, Q2I, I7X, P1C, Z9G, E2N, X2C, K2U, A4U, W2L, W7I, Q1F, P9A, F5A, P2G, S5M, Q0F, W6E, O5M, M5W, J3L, Y4R, S5P, J3I, H1J, Z9A, I6W, T4U, O7G, G0S, V7V, N6E, D3H, J1D, V2D, I8Y, X1S, D6J, B9X, S5K, X3L, K0X, F4X, V1E, D9R, P2I, X4G, Q5B, N5H, F6H, E4X, C1W, U3A, C8P, H2A, X1V, C2N, A4F, A4B, S5I, K5C, O7L, I2G, E1Q, N7C, Q4Z, W3P, V9B, J2W, N4F, Z2E, Z8G, E1F, O5Y, Z1R, D6G, F5J, W1B, C1J, A6M, O2P, W2J, C5P, S1J, O8D, P5G, D5Y, U0E, N3H, Y1C, I6V, F2E, E5D, Q6L, C3N, F8H, P6B, Z8L, K2J, X3Y, Q8P, M5P, W2S, D5O, M9S, C7E, W6S, V1X, Z7L, W4Y, O4L, D2O, Q7O, P6X, W2F, F7A, S1O, I7H, X2R, X1Z, F1Y, Q1Y, Q6H, D9Z, E3X, C4G, F5G, F2B, M0I, Q3M, M8R, N3L, W6H, V5V, C2C, W3W, E3Q, C5G, D4W, D5Q, J1E, K6N, Q9Z, W1P, V2I, J2A, G0U, O2L, F8N, C7N</t>
+          <t>Z5L, M3M, W2D, W2K, R1H, W1G, V3O, G3H, P4U, A1X, G5Z, B5F, L2P, T1H, P7R, C3M, I1G, W9F, K2X, R1T, N4C, M2H, D9T, E9X, R8E, K1K, Z9K, Q2F, K4F, K2L, N1Y, L1D, C2E, F6F, R6Z, E5Z, Z6I, H1K, Q2M, R3K, Z7O, W0N, K0I, H8Y, W5R, A4P, E8A, Y1A, W3T, Z6G, H1X, N1H, I1P, N4L, E5U, Q2I, I7X, P1C, Z9G, E2N, X2C, K2U, A4U, W2L, W7I, Q1F, P9A, F5A, P2G, S5M, Q0F, W6E, O5M, M5W, J3L, Y4R, S5P, J3I, H1J, Z9A, I6W, T4U, O7G, G0S, V7V, N6E, D3H, J1D, V2D, I8Y, X1S, D6J, B9X, S5K, X3L, K0X, F4X, V1E, D9R, P2I, X4G, Q5B, N5H, F6H, E4X, C1W, U3A, C8P, H2A, X1V, C2N, A4F, A4B, S5I, K5C, O7L, I2G, E1Q, N7C, Q4Z, W3P, V9B, J2W, N4F, Z2E, Z8G, E1F, O5Y, Z1R, D6G, F5J, W1B, C1J, A6M, O2P, W2J, C5P, S1J, O8D, P5G, D5Y, U0E, N3H, Y1C, I6V, F2E, E5D, Q6L, C3N, F8H, P6B, Z8L, K2J, X3Y, Q8P, M5P, W2S, D5O, M9S, C7E, W6S, V1X, Z7L, W4Y, O4L, D2O, Q7O, P6X, W2F, F7A, S1O, I7H, X2R, X1Z, F1Y, Q1Y, Q6H, D9Z, E3X, C4G, F5G, F2B, Q3M, M8R, N3L, W6H, V5V, C2C, W3W, E3Q, C5G, D4W, D5Q, J1E, K6N, Q9Z, W1P, V2I, J2A, G0U, O2L, F8N, C7N</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -8882,7 +9110,11 @@
           <t>NMB63209848145305</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr"/>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -8898,7 +9130,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Z5B, M1H, I5E, P7R, P9S, Z7T, N2R, Q3X, A4B, Q1J, V1C, P8C, N3F, V7P, N0A, U3D, R6M, D5Z, N8N, J3K, D5B, I2I, Z9E, N6L, G4D, F0W, Y1Y, J8Y, H1N, V2K, J2H, N2H, L2A, P4W, Y4A, X3C, I6A, N4Z, A6T, F7I, R9Z, O7D, M9O, D6J, M9U, T1Q, W5O, J1Q, B5F, M0I, X3W, Y4R, K6R, Q0B, P1I, V2E, X1Y, X1U, W5X, P0Y, U2R, V7S, K2C, W3M, C5I, A2P, K0E, P0W, K0Q, B5I, A5W, R3K, R2P, J1F, K7T, O8M, V6G, W7U, Z7D, L2T, M8Z, V2A, W2Q, U3A, N0N, W8C, K8Y, T5A, Z7B, Q7M, N5X, Y1G, K6H, T2L, E6H, D9C, N0S, P7V, T3R, G1D, Q7G, O1O, G1C, P8Z, N5B, Z0P, C2E, H8U, R5R, D2T, U2G, C8G, R6Y, K3F, W5D, K3Y, B5C, Q6A, D2Y, J2U, W0W, A2E, Z7X, D3X, P4U, A6B, K0I, Z1G, C0F, P4A, Q5G, E2A, U3M, R2G, N8C, T1C, F0G, I1P, F1V, A5M, U2L, D2V, P1B, N3K, X2J, C9J, E3D, W7F, W4G, P2K, I9I, W2P, W0J, K1G, P6J, Z8K, C9T, D3R, Y1V, G0B, P5H, E1B, P5B, C7D, J2D, A5Q, M9S, E5D, I1G, Q1N, J5S, D7A, C8W, Z3H, R1N, V5R, W5J, Z9M, D6G, Y9Y, U3L, I4G, D0D, T0Q, K5T, W1U, D1X, K1L, Z3K, C6A, W3W, O5M, N6T, W2D, E3G, O1M, I2M, C5Y, R1S, I7M, G2B, Z4K, J3Y, G1H, C2L, Q1T, C2Z, R2X, Z7J, H2D, W3K, Q0A, N4G, A1K, Z2J, B2B, T3C, R1M, Q6T, Q2O, T2C, F3Z, C8C, Z9F, Z2A, A4S, V7I, P9K, I1Q, I7G, B5Z, Q4K, X9Y, H1V, W1F, Z6J, I9X, W7T, Z8Q, U6E, D3F, O7Q, C8Y, V7Y, K4H, P2S, I2H, O2D, C4I, V7Z, Q6H, R0R, H2B, B1A, F2T, W5B, I6T, D2P, K4E, M5H, M9V, M6C, H8X, N4W</t>
+          <t>Z5B, M1H, I5E, P7R, P9S, Z7T, N2R, Q3X, A4B, Q1J, V1C, P8C, N3F, V7P, N0A, U3D, R6M, D5Z, N8N, J3K, D5B, I2I, Z9E, N6L, G4D, F0W, Y1Y, J8Y, H1N, V2K, J2H, N2H, L2A, P4W, Y4A, X3C, I6A, N4Z, A6T, F7I, R9Z, O7D, M9O, D6J, M9U, T1Q, W5O, J1Q, B5F, X3W, Y4R, K6R, Q0B, P1I, V2E, X1Y, X1U, W5X, P0Y, U2R, V7S, K2C, W3M, C5I, A2P, K0E, P0W, K0Q, B5I, A5W, R3K, R2P, J1F, K7T, O8M, V6G, W7U, Z7D, L2T, M8Z, V2A, W2Q, U3A, N0N, W8C, K8Y, T5A, Z7B, Q7M, N5X, Y1G, K6H, T2L, E6H, D9C, N0S, P7V, T3R, G1D, Q7G, O1O, G1C, P8Z, N5B, Z0P, C2E, H8U, R5R, D2T, U2G, C8G, R6Y, K3F, W5D, K3Y, B5C, Q6A, D2Y, J2U, W0W, A2E, Z7X, D3X, P4U, A6B, K0I, Z1G, C0F, P4A, Q5G, E2A, U3M, R2G, N8C, T1C, F0G, I1P, F1V, A5M, U2L, D2V, P1B, N3K, X2J, C9J, E3D, W7F, W4G, P2K, I9I, W2P, W0J, K1G, P6J, Z8K, C9T, D3R, Y1V, G0B, P5H, E1B, P5B, C7D, J2D, A5Q, M9S, E5D, I1G, Q1N, J5S, D7A, C8W, Z3H, R1N, V5R, W5J, Z9M, D6G, Y9Y, U3L, I4G, D0D, T0Q, K5T, W1U, D1X, K1L, Z3K, C6A, W3W, O5M, N6T, W2D, E3G, O1M, I2M, C5Y, R1S, I7M, G2B, Z4K, J3Y, G1H, C2L, Q1T, C2Z, R2X, Z7J, H2D, W3K, Q0A, N4G, A1K, Z2J, B2B, T3C, R1M, Q6T, Q2O, T2C, F3Z, C8C, Z9F, Z2A, A4S, V7I, P9K, I1Q, I7G, B5Z, Q4K, X9Y, H1V, W1F, Z6J, I9X, W7T, Z8Q, U6E, D3F, O7Q, C8Y, V7Y, K4H, P2S, I2H, O2D, C4I, V7Z, Q6H, R0R, H2B, B1A, F2T, W5B, I6T, D2P, K4E, M5H, M9V, M6C, H8X, N4W</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -8962,7 +9194,11 @@
           <t>WDB48171558415910</t>
         </is>
       </c>
-      <c r="F313" t="inlineStr"/>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -9070,7 +9306,11 @@
           <t>WEB88998840436035</t>
         </is>
       </c>
-      <c r="F317" t="inlineStr"/>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -9094,7 +9334,11 @@
           <t>WEB28444563894252</t>
         </is>
       </c>
-      <c r="F318" t="inlineStr"/>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -9334,7 +9578,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Z5E, M3D, I2M, X4C, Q1E, W2N, F9Y, V4S, I5G, Z7J, F6J, C4P, Z8C, N2H, D1B, D7R, S1F, C3U, V7K, N1A, V4B, T3C, O8K, P9E, Q8W, R1I, I0E, G3B, P0Z, F6H, P6B, P0C, K7O, F7B, N4C, M8R, A6Q, R1V, K6K, S5B, W6F, Z9M, N0M, K3T, A5P, V7J, M5O, O1O, A5N, F1X, A4H, C9Y, X1K, M8Y, R5D, S5C, K6V, K5J, V8O, P9F, G2C, G4D, M9V, I5W, V0V, N1J, I5L, I2F, O3C, Q6H, C6X, P6X, E5M, L4B, Z7R, N3B, A6H, Q1M, J1D, W2G, I2E, K3K, D6G, Q8I, K6P, B2A, Z7Q, O2D, E5C, T1U, W7S, W9S, V0U, A2T, G9Y, C1G, Y3E, M7H, W6H, U2Y, E0F, W2P, Z4J, V6T, K3B, K6Q, B1V, Q1W, J9R, X3X, L2J, K2L, I5V, P7Y, Q1J, W6N, T0Z, T1C, Z4F, Q3C, T1R, H8X, W7N, B1G, K1M, E1M, K6I, Q3T, W7G, C0O, U9Z, Z9X, F9R, P5B, X4A, M0I, Q2U, F8G, F1W, I1C, Z4S, W2L, W0H, P5Z, Z4R, V1C, U2P, F0N, V2P, I6P, E7C, P9T, C8T, A1E, N8N, P2M, D2J, D1K, K6M, Z1O, C1P, Q3U, J3T, V0S, R9X, W6M, X9D, R6V, V1E, I2G, C0Q, Z5T, M8U, E0K, R8A, V7B, F6Y, R1M, C3E, Z0C, O6N, V6X, V0W</t>
+          <t>Z5E, M3D, I2M, X4C, Q1E, W2N, F9Y, V4S, I5G, Z7J, F6J, C4P, Z8C, N2H, D1B, D7R, S1F, C3U, V7K, N1A, V4B, T3C, O8K, P9E, Q8W, R1I, I0E, G3B, P0Z, F6H, P6B, P0C, K7O, F7B, N4C, M8R, A6Q, R1V, K6K, S5B, W6F, Z9M, N0M, K3T, A5P, V7J, M5O, O1O, A5N, F1X, A4H, C9Y, X1K, M8Y, R5D, S5C, K6V, K5J, V8O, P9F, G2C, G4D, M9V, I5W, V0V, N1J, I5L, I2F, O3C, Q6H, C6X, P6X, E5M, L4B, Z7R, N3B, A6H, Q1M, J1D, W2G, I2E, K3K, D6G, Q8I, K6P, B2A, Z7Q, O2D, E5C, T1U, W7S, W9S, V0U, A2T, G9Y, C1G, Y3E, M7H, W6H, U2Y, E0F, W2P, Z4J, V6T, K3B, K6Q, B1V, Q1W, J9R, X3X, L2J, K2L, I5V, P7Y, Q1J, W6N, T0Z, T1C, Z4F, Q3C, T1R, H8X, W7N, B1G, K1M, E1M, K6I, Q3T, W7G, C0O, U9Z, Z9X, F9R, P5B, X4A, Q2U, F8G, F1W, I1C, Z4S, W2L, W0H, P5Z, Z4R, V1C, U2P, F0N, V2P, I6P, E7C, P9T, C8T, A1E, N8N, P2M, D2J, D1K, K6M, Z1O, C1P, Q3U, J3T, V0S, R9X, W6M, X9D, R6V, V1E, I2G, C0Q, Z5T, M8U, E0K, R8A, V7B, F6Y, R1M, C3E, Z0C, O6N, V6X, V0W</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -9370,7 +9614,11 @@
           <t>WDB13352840392563</t>
         </is>
       </c>
-      <c r="F328" t="inlineStr"/>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -9498,7 +9746,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Z5L, M3L, I8Z, Z3T, U3I, G3B, U2L, X4K, F6Q, F6Y, W2O, W7R, N1V, D8M, X2K, M9T, C3V, K1K, C2A, U6B, Z3D, Q2E, D3Y, Z1L, P2A, Z6I, F2W, K4H, V7L, V1Z, V4T, Z1H, B1X, K6B, L1V, M6N, X2V, E1U, M9S, J3E, C9Y, F9A, F2J, I1J, O8N, Q7S, K6Y, I2V, E1V, D4Y, U3O, J3S, N7Q, I7M, W5F, Y3F, Y4H, C9U, I8Y, E5V, K7B, L9V, M6L, M7U, Y4P, Q7E, K6U, C6D, D6C, V6Z, G0G, R5S, Q6Z, M0J, E3I, Z8N, P0Z, A1M, Q2S, O4F, R8H, C6J, Z2H, R2D, K0P, D1X, C1Q, T0K, Q2U, Q6L, Y3O, I6C, W0T, V7M, F1R, C5D, N3F, I5X, Q1C, M7H, Q7W, I9L, C4X, Q7Y, E2T, J1Q, D9G, V6J, M6C, B1C, B4K, I7X, P5B, J9Z, Q4E, F1T, Z1S, E3B, A9Z, U0D, U0O, C7S, O8O, Q4N, F0P, V7C, G1C, Q1D, J1K, J6C, A2N, K2Z, K0F, W6U, R0E, E5E, I6Y, F6I, T3Q, G2H, D9T, O0I, J9I, P0B, E6Z, D3T, C5A, V2P, T2N, C1Z, N6L, Y1A, C0O, E5X, Q7B, O2L, S1I, R1H, R9Z, V4N, A2H, N1T, U2G, O4P, P9P, E3S, D3Z, Z0K, N8D, E9K, I4F, I6O, V0Z, Q9C, O8U, D2K, D4X, X2P, Z7Q, E3M, A4G, Z0J, F0T, C3F, Y4W, N4X, O7A, E4S, M2I, K2W, E3V, W4L, R4Z, D7Z, D5V, F3G, E5H, E4B, O2H, Q3E, M8Y, O6S, I9W, K2A, B1H, S5G, P5X, L1L, C1N, Z7R, S5E, M9Y, Z8J, F6D, M7V, N7V, I0F, O1Z, X1B, K6M, H1I, O5T, O6G, N8K, Y1G, C9X, O6Y, N5K, O2P, G1H, Q8W, N2G, I0U, C1H, K7A, I6L, N5H, Z7K, W2L, F5D, C7U, Q2N, N0Z, E3D, J9J, Q6A</t>
+          <t>Z5L, M3L, I8Z, Z3T, U3I, G3B, U2L, X4K, F6Q, F6Y, W2O, W7R, N1V, D8M, X2K, M9T, C3V, K1K, C2A, U6B, Z3D, Q2E, D3Y, Z1L, P2A, Z6I, F2W, K4H, V7L, V1Z, V4T, Z1H, B1X, K6B, L1V, M6N, X2V, E1U, M9S, J3E, C9Y, F9A, F2J, I1J, O8N, Q7S, K6Y, I2V, E1V, D4Y, U3O, J3S, N7Q, I7M, W5F, Y3F, Y4H, C9U, I8Y, E5V, K7B, L9V, M6L, M7U, Y4P, Q7E, K6U, C6D, D6C, V6Z, G0G, R5S, Q6Z, E3I, Z8N, P0Z, A1M, Q2S, O4F, R8H, C6J, Z2H, R2D, K0P, D1X, C1Q, T0K, Q2U, Q6L, Y3O, I6C, W0T, V7M, F1R, C5D, N3F, I5X, Q1C, M7H, Q7W, I9L, C4X, Q7Y, E2T, J1Q, D9G, V6J, M6C, B1C, B4K, I7X, P5B, J9Z, Q4E, F1T, Z1S, E3B, A9Z, U0D, U0O, C7S, O8O, Q4N, F0P, V7C, G1C, Q1D, J1K, J6C, A2N, K2Z, K0F, W6U, R0E, E5E, I6Y, F6I, T3Q, G2H, D9T, O0I, J9I, P0B, E6Z, D3T, C5A, V2P, T2N, C1Z, N6L, Y1A, C0O, E5X, Q7B, O2L, S1I, R1H, R9Z, V4N, A2H, N1T, U2G, O4P, P9P, E3S, D3Z, Z0K, N8D, E9K, I4F, I6O, V0Z, Q9C, O8U, D2K, D4X, X2P, Z7Q, E3M, A4G, Z0J, F0T, C3F, Y4W, N4X, O7A, E4S, M2I, K2W, E3V, W4L, R4Z, D7Z, D5V, F3G, E5H, E4B, O2H, Q3E, M8Y, O6S, I9W, K2A, B1H, S5G, P5X, L1L, C1N, Z7R, S5E, M9Y, Z8J, F6D, M7V, N7V, I0F, O1Z, X1B, K6M, H1I, O5T, O6G, N8K, Y1G, C9X, O6Y, N5K, O2P, G1H, Q8W, N2G, I0U, C1H, K7A, I6L, N5H, Z7K, W2L, F5D, C7U, Q2N, N0Z, E3D, J9J, Q6A</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
@@ -9506,7 +9754,11 @@
           <t>WDB12615219228418</t>
         </is>
       </c>
-      <c r="F333" t="inlineStr"/>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -9522,7 +9774,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Z5D, M2S, K3Q, C8Y, K7E, B3H, J4V, I6V, B1Z, Y9W, V1J, Q2T, E3H, R2P, W0S, F2T, P2K, F6M, Q2F, D9N, V6G, X2K, M0J, Q1F, G4C, Z0C, P0T, Q2A, W2S, V6X, O8D, Q0V, P9A, W3G, T1Z, W5Y, E5K, Z9F, X3W, Q2X, Y4U, S1L, R2C, D2J, W1A, G2E, R1M, F6W, G3I, I7G, P0X, Y4Z, M9X, S8C, B5A, Z3X, Q3T, I1M, H1L, R7L, G4H, D9R, J3C, R2R, G0N, K6W, R3G, L1T, Z7W, F5B, A4W, M5K, Q8L, N3C, E0Z, Q4S, V7I, J9O, W7V, Q5S, X1W, G1C, Z1U, V2K, W3C, V8Q, B5Z, V4A, A1T, T2J, D4S, O6R, Y3F, X2C, X6F, D3E, T0G, I1N, O5U, O4S, S5S, C8V, V5S, A6H, W6O, K5K, X3D, B9Z, Z8L, N5A, M5W, F0E, F6E, K3U, Q7K, C6L, P5X, M6O, T0Z, E4A, Z0G, P7T, A1A, I4E, F1Y, N3N, F1S, Q4B, D4Y, X2Y, C7W, E3Y, L2R, F7B, D4Z, Y2A, O1O, K1J, Q9Z, C8Q, K3C, D1L, T1F, L2M, K0A, D4I, Q8A, D8B, A6C, Q5U, E3T</t>
+          <t>Z5D, M2S, K3Q, C8Y, K7E, B3H, J4V, I6V, B1Z, Y9W, V1J, Q2T, E3H, R2P, W0S, F2T, P2K, F6M, Q2F, D9N, V6G, X2K, Q1F, G4C, Z0C, P0T, Q2A, W2S, V6X, O8D, Q0V, P9A, W3G, T1Z, W5Y, E5K, Z9F, X3W, Q2X, Y4U, S1L, R2C, D2J, W1A, G2E, R1M, F6W, G3I, I7G, P0X, Y4Z, M9X, S8C, B5A, Z3X, Q3T, I1M, H1L, R7L, G4H, D9R, J3C, R2R, G0N, K6W, R3G, L1T, Z7W, F5B, A4W, M5K, Q8L, N3C, E0Z, Q4S, V7I, J9O, W7V, Q5S, X1W, G1C, Z1U, V2K, W3C, V8Q, B5Z, V4A, A1T, T2J, D4S, O6R, Y3F, X2C, X6F, D3E, T0G, I1N, O5U, O4S, S5S, C8V, V5S, A6H, W6O, K5K, X3D, B9Z, Z8L, N5A, M5W, F0E, F6E, K3U, Q7K, C6L, P5X, M6O, T0Z, E4A, Z0G, P7T, A1A, I4E, F1Y, N3N, F1S, Q4B, D4Y, X2Y, C7W, E3Y, L2R, F7B, D4Z, Y2A, O1O, K1J, Q9Z, C8Q, K3C, D1L, T1F, L2M, K0A, D4I, Q8A, D8B, A6C, Q5U, E3T</t>
         </is>
       </c>
       <c r="E334" t="inlineStr">
@@ -9550,7 +9802,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Z5D, M2P, X6F, T1L, N5Z, I8Z, O2G, Z7V, Y4W, Z8D, C8Z, L1Z, X1S, H2F, J1C, E4O, Z8V, A2Y, M8P, H1Q, C0D, C9U, W6H, O4M, W6X, D2Y, J1K, V7R, M8Q, A1W, K2A, P9E, X1E, D3K, Y1H, Z8G, M0J, I2Z, R1P, P8B, D1G, A1F, L4Z, O5O, W0F, U0B, R6V, Z1N, J9Q, V4B, Q4G, F2M, C3M, K7E, O5U, C4P, O4D, O7T, P1M, M0E, N5A, Z2C, F7I, W8P, A2M, Z7W, P0T, V4S, V8W, Z2L, C9Y, E0F, Q2D, K2C, O4B, A6L, D6N, O6T, Q1T, J3S, Z0Z, Y1V, B2B, O2Q, N4F, Y4I, W8E, I7T, D5I, I6J, F0L, I6K, Q7D, V6Z, L1N, Z0E, Z3G, P2J, Q2N, F3K, S1F, K0F, P0S, N4E, F9W, D4B, M9O, F3H, W6E, R1J, K9Z, R1G, I0M, M7Q, R2K, Q2V, J1W, F0T, T1Y, D0B, Q4Z, D6C, Z9B, N4A, R4D, W1U, Q1V, E5K, A4P, G4I, Z6I, I2M, P5Y, S8E, C2R, H8W, C5D, C0F, G0A, A2T, O2S, G1E, M5T, F2H, O5T, S9W, Y9A, G3H, N5U, Z9C, Q4Y, E1S, J3J, K4H, Y1F, K2L, M8C, K1U, F9B, U6D, R1T, K7S, K8Y, I1V, R7F, Q4K, Z2D, C3K, P2H, Q0B, Q0V, K0B, W9Z, F4X, T0X, I7M, F1R, C2Z, D3R, J1A, K9V, D1A, O2C, E1L, B3G, O4C, Z3K, Z1O, B1H, P0H, X4L, A5R, G5G, M7S, X2G, A4V, A2I, A1P, J4V, L1D, L2Q, F6W, K6R</t>
+          <t>Z5D, M2P, X6F, T1L, N5Z, I8Z, O2G, Z7V, Y4W, Z8D, C8Z, L1Z, X1S, H2F, J1C, E4O, Z8V, A2Y, M8P, H1Q, C0D, C9U, W6H, O4M, W6X, D2Y, J1K, V7R, M8Q, A1W, K2A, P9E, X1E, D3K, Y1H, Z8G, I2Z, R1P, P8B, D1G, A1F, L4Z, O5O, W0F, U0B, R6V, Z1N, J9Q, V4B, Q4G, F2M, C3M, K7E, O5U, C4P, O4D, O7T, P1M, M0E, N5A, Z2C, F7I, W8P, A2M, Z7W, P0T, V4S, V8W, Z2L, C9Y, E0F, Q2D, K2C, O4B, A6L, D6N, O6T, Q1T, J3S, Z0Z, Y1V, B2B, O2Q, N4F, Y4I, W8E, I7T, D5I, I6J, F0L, I6K, Q7D, V6Z, L1N, Z0E, Z3G, P2J, Q2N, F3K, S1F, K0F, P0S, N4E, F9W, D4B, M9O, F3H, W6E, R1J, K9Z, R1G, I0M, M7Q, R2K, Q2V, J1W, F0T, T1Y, D0B, Q4Z, D6C, Z9B, N4A, R4D, W1U, Q1V, E5K, A4P, G4I, Z6I, I2M, P5Y, S8E, C2R, H8W, C5D, C0F, G0A, A2T, O2S, G1E, M5T, F2H, O5T, S9W, Y9A, G3H, N5U, Z9C, Q4Y, E1S, J3J, K4H, Y1F, K2L, M8C, K1U, F9B, U6D, R1T, K7S, K8Y, I1V, R7F, Q4K, Z2D, C3K, P2H, Q0B, Q0V, K0B, W9Z, F4X, T0X, I7M, F1R, C2Z, D3R, J1A, K9V, D1A, O2C, E1L, B3G, O4C, Z3K, Z1O, B1H, P0H, X4L, A5R, G5G, M7S, X2G, A4V, A2I, A1P, J4V, L1D, L2Q, F6W, K6R</t>
         </is>
       </c>
       <c r="E335" t="inlineStr">
@@ -9662,7 +9914,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Z5L, M3K, M0W, X4F, W1U, D0V, P9F, Z8F, R8D, V2M, P1N, R6Z, D1X, V1G, N3N, X1H, K6W, W0O, P6P, R1R, C6K, C8T, C7G, K7F, T2J, W4H, G2F, C8M, Z3J, N0D, K3C, E1M, P6R, E1Z, W1C, U1V, K7E, K3U, U2S, D4B, F0L, Q4W, R3H, K1H, O7T, R6V, A1G, I5Y, C9N, R2Z, H2E, K3Y, O6Y, M0E, C8Y, W4U, W5C, C2A, K5S, X1G, H1J, D4L, X2X, C4X, T3S, E2T, L0Y, K7J, D8M, Y4I, E1W, G2H, C0A, Z3R, G1J, F1M, E8A, G5B, Z0O, M9E, M6O, M8D, S1D, V7Y, D6F, F2T, G2C, A2F, Y3O, M0J, R1Q, P5A, J9F, F6D, Z2X, E3D, O6N, J3M, P7M, V0T, Q6S, D1W, F6R, Z3U, Q2E, Q0V, V6S, Q6W, T2N, E5T, Z2U, L2A, V2I, O0F, P0X, C7I, W0F, C0L, W5S, Q3R, E0X, Z8R, D6C, Z7Q, Z7Z, C6B, T2U, K6V, F6N, B5M, F9M, E1B, E3K, F9X, Q3E, X1E, F6M, D9Z, I4C, K4V, M4D, S9W, C2Y, V6C, A0B, W6K, Q9Y, T0U, O8K, S1L, I5L, Z4G, D1V, A6L, K0G, Z7U, X2C, V6Q, Z4R, N3B, D4H, H1Q, W3C, E6D, Q6P, F1U, D3M, D5E, Z1X, F5A, R8N, W3N, K3F, L1H, Q7T, F6T, O1V, A6M, S5R, X3V, D1Q, C5X, W0G, V1A, O6P, F2W, K0D, R1O, F0C, B4M, K5D, B5D, J1O, P0S, P6I, R5Z, I2D, J2X, Z5A, K7V, E3S, R8J, W0P, F2Y, Z0X</t>
+          <t>Z5L, M3K, M0W, X4F, W1U, D0V, P9F, Z8F, R8D, V2M, P1N, R6Z, D1X, V1G, N3N, X1H, K6W, W0O, P6P, R1R, C6K, C8T, C7G, K7F, T2J, W4H, G2F, C8M, Z3J, N0D, K3C, E1M, P6R, E1Z, W1C, U1V, K7E, K3U, U2S, D4B, F0L, Q4W, R3H, K1H, O7T, R6V, A1G, I5Y, C9N, R2Z, H2E, K3Y, O6Y, M0E, C8Y, W4U, W5C, C2A, K5S, X1G, H1J, D4L, X2X, C4X, T3S, E2T, L0Y, K7J, D8M, Y4I, E1W, G2H, C0A, Z3R, G1J, F1M, E8A, G5B, Z0O, M9E, M6O, M8D, S1D, V7Y, D6F, F2T, G2C, A2F, Y3O, R1Q, P5A, J9F, F6D, Z2X, E3D, O6N, J3M, P7M, V0T, Q6S, D1W, F6R, Z3U, Q2E, Q0V, V6S, Q6W, T2N, E5T, Z2U, L2A, V2I, O0F, P0X, C7I, W0F, C0L, W5S, Q3R, E0X, Z8R, D6C, Z7Q, Z7Z, C6B, T2U, K6V, F6N, B5M, F9M, E1B, E3K, F9X, Q3E, X1E, F6M, D9Z, I4C, K4V, M4D, S9W, C2Y, V6C, A0B, W6K, Q9Y, T0U, O8K, S1L, I5L, Z4G, D1V, A6L, K0G, Z7U, X2C, V6Q, Z4R, N3B, D4H, H1Q, W3C, E6D, Q6P, F1U, D3M, D5E, Z1X, F5A, R8N, W3N, K3F, L1H, Q7T, F6T, O1V, A6M, S5R, X3V, D1Q, C5X, W0G, V1A, O6P, F2W, K0D, R1O, F0C, B4M, K5D, B5D, J1O, P0S, P6I, R5Z, I2D, J2X, K7V, E3S, R8J, W0P, F2Y, Z0X</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
@@ -9670,7 +9922,11 @@
           <t>W1T79284647924366</t>
         </is>
       </c>
-      <c r="F339" t="inlineStr"/>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -9722,7 +9978,11 @@
           <t>WDB84682480100671</t>
         </is>
       </c>
-      <c r="F341" t="inlineStr"/>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -9766,7 +10026,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Z5E, M3C, J3U, V4S, X3Q, V6A, X2B, A1T, P9R, U8B, V1X, Q4G, Y3F, W1X, W7Y, I3D, C4L, V1L, Q2L, R5P, W2B, M7K, C6L, D1T, Z4U, Q8C, F1T, E4S, M7T, Q1B, G0S, A5B, F3P, M6N, J1W, W4E, R4X, J1S, B2X, V1W, A6T, D9G, Z0K, W5E, D3Q, D0E, R6X, Z5A, I7W, K5C, M8N, Z9K, V5Q, J9P, C1B, Y4X, B1D, V2V, U6A, V6I, M7Q, D1K, Q6C, Q1T, C5V, Z0R, W6U, Z2A, C3B, W5H, N5V, X9Y, C7C, E9K, Q5G, I7N, G0V, M7F, K1G, K3Z, L3D, Y1C, U2I, G0N, P2W, A3A, S8E, F9M, C6M, A2Q, D1G, R5O, A1X, C8Q, L3A, U2K, V4A, P0Q, W5B, I6J, T1E, W0Z, J3C, I4H, C5H, D2Y, B1U, V0V, C6U, E6B, N4Y, W3K, C3U, Q6J, L1Q, Y6A, K0G, Q6Z, K3F, F4X, O5N, U0O, O0H, X4M, Q6P, I9Z, I3L, J1X, M9X</t>
+          <t>Z5E, M3C, J3U, V4S, X3Q, V6A, X2B, A1T, P9R, U8B, V1X, Q4G, Y3F, W1X, W7Y, I3D, C4L, V1L, Q2L, R5P, W2B, M7K, C6L, D1T, Z4U, Q8C, F1T, E4S, M7T, Q1B, G0S, A5B, F3P, M6N, J1W, W4E, R4X, J1S, B2X, V1W, A6T, D9G, Z0K, W5E, D3Q, D0E, R6X, I7W, K5C, M8N, Z9K, V5Q, J9P, C1B, Y4X, B1D, V2V, U6A, V6I, M7Q, D1K, Q6C, Q1T, C5V, Z0R, W6U, Z2A, C3B, W5H, N5V, X9Y, C7C, E9K, Q5G, I7N, G0V, M7F, K1G, K3Z, L3D, Y1C, U2I, G0N, P2W, A3A, S8E, F9M, C6M, A2Q, D1G, R5O, A1X, C8Q, L3A, U2K, V4A, P0Q, W5B, I6J, T1E, W0Z, J3C, I4H, C5H, D2Y, B1U, V0V, C6U, E6B, N4Y, W3K, C3U, Q6J, L1Q, Y6A, K0G, Q6Z, K3F, F4X, O5N, U0O, O0H, X4M, Q6P, I9Z, I3L, J1X, M9X</t>
         </is>
       </c>
       <c r="E343" t="inlineStr">
@@ -9906,7 +10166,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Z5F, M3P, Y4U, C5J, M7R, W7E, E2R, C9M, P4A, Z7R, W4R, C6C, F3G, N5J, F1T, C4E, M9W, C6D, N6R, Q1M, K7Z, W3M, N1P, Z7A, Q6E, Y4H, A6H, S1P, O4J, I4B, I5G, V7J, X3R, Q7Z, Q4K, N1X, Z0T, T3L, B5J, X1S, E9D, D2X, C2U, O4P, Z7N, D1K, E3B, C3A, I9H, P7M, R5P, E0U, O0A, R8C, L2N, M5C, M9E, P9C, Y1F, Q4Z, P5Z, W2W, W5W, D7I, Y4D, W9F, E3J, A9Z, F8Z, I2E, Y1W, P0H, V2P, E5K, U8C, D4Z, F6K, D7Q, Z8W, Q3W, O2D, U2U, P6E, W4T, A6N, C2O, E2L, H8U, Z6I, Z0R, R1E, C6K, N5W, K2V, F6C, D4M, A1P, C5V, L4A, M4Y, K3R, T0K, Q2I, C3G, Z0E, B2G, W5E, A5S, C7E, F4G, K0Z, Z5O, V7A, S8J, D1B, A2Z, E0W, W5C, Y4B, C5A, K4K, K6H, F7G, I8X, P5P, P0C, O4G, C3K, Q4W, L1L, D0L, R5M, A4X, S5K, J5S, I7M, D5J, D3B, B1E, K6E, L9W, W0K, O6T, N6I, J3T, P1C, C4B, V3A, N2I, M8L, V6P, W3F, Z1I, O1Y, X4H, K3Y, O1D, C6F, I7X, M5O, Z1J, D4W, C5B, K3B, W5R, W0N, G4C, S1G, P6Q, Q5L, M0J, Z3K, G3N, R5N, C8G, V1A, R8K, C2S, Z5U, F2J, Z0O, K5P, O1O, N5D, C1K</t>
+          <t>Z5F, M3P, Y4U, C5J, M7R, W7E, E2R, C9M, P4A, Z7R, W4R, C6C, F3G, N5J, F1T, C4E, M9W, C6D, N6R, Q1M, K7Z, W3M, N1P, Z7A, Q6E, Y4H, A6H, S1P, O4J, I4B, I5G, V7J, X3R, Q7Z, Q4K, N1X, Z0T, T3L, B5J, X1S, E9D, D2X, C2U, O4P, Z7N, D1K, E3B, C3A, I9H, P7M, R5P, E0U, O0A, R8C, L2N, M5C, M9E, P9C, Y1F, Q4Z, P5Z, W2W, W5W, D7I, Y4D, W9F, E3J, A9Z, F8Z, I2E, Y1W, P0H, V2P, E5K, U8C, D4Z, F6K, D7Q, Z8W, Q3W, O2D, U2U, P6E, W4T, A6N, C2O, E2L, H8U, Z6I, Z0R, R1E, C6K, N5W, K2V, F6C, D4M, A1P, C5V, L4A, M4Y, K3R, T0K, Q2I, C3G, Z0E, B2G, W5E, A5S, C7E, F4G, K0Z, Z5O, V7A, S8J, D1B, A2Z, E0W, W5C, Y4B, C5A, K4K, K6H, F7G, I8X, P5P, P0C, O4G, C3K, Q4W, L1L, D0L, R5M, A4X, S5K, J5S, I7M, D5J, D3B, B1E, K6E, L9W, W0K, O6T, N6I, J3T, P1C, C4B, V3A, N2I, M8L, V6P, W3F, Z1I, O1Y, X4H, K3Y, O1D, C6F, I7X, M5O, Z1J, D4W, C5B, K3B, W5R, W0N, G4C, S1G, P6Q, Q5L, Z3K, G3N, R5N, C8G, V1A, R8K, C2S, Z5U, F2J, Z0O, K5P, O1O, N5D, C1K</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
@@ -10362,7 +10622,11 @@
           <t>NMB51770054164375</t>
         </is>
       </c>
-      <c r="F364" t="inlineStr"/>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -10386,7 +10650,11 @@
           <t>W1T67469030136596</t>
         </is>
       </c>
-      <c r="F365" t="inlineStr"/>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -10402,7 +10670,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Z5D, M2N, E0N, R8P, W7E, V1P, V5P, P9Z, E3H, Q5R, T0P, G5B, R4L, C3Q, S5L, O2C, B2D, C8I, D9E, G2H, W5J, B5E, Z4S, N4F, W9F, R1V, F9W, N8M, F2H, W0S, Q3U, N5B, F0K, K8C, A5D, F6C, A5G, W4I, R2N, V4S, P6F, Z8D, P6Z, A2Q, F6E, W0P, V7P, O2O, C3G, K0P, P0U, Z1S, K5Q, G2D, I7G, F7V, C5U, X2K, V7Y, T0F, L2J, C0R, W4F, F3C, E2F, C2U, C9U, F0G, C8U, D6P, Q6H, W1W, T0Z, K2V, Y4U, B9X, Q9Z, P2L, E2N, Q8V, I9J, U3P, Z2Z, V2F, W2A, W6O, W1A, V7F, Y1Z, U2R, U2E, Q2C, Z1J, F9T, A4M, E1R, J1T, Z8S, A4R, Y9V, I5M, F5T, T0J, Q6Q, O4M, C5Y, N3K, D9G, V5S, A6C, F7E, C8Y, W1Q, U2I, K6V, Z3N, Q0F, D6F, D2V, R8K, Y1D, G1C, S1I, D0P, C9I, V5W, R6V, O0G, Z7S, J8Y, W7L, G3G, O1S, D4S, L1V, W0Y, K7O, K8B, X3A, O7Y, Q7O, Q8X, F9C, G0V, U2U, E6E, T1H, E1M, K1P, V3W, G0O, Q6Z, E0Z, N4L, Z8U, E5H, E3X, R1R, W5Q, W7M, U3Y, Q2M, I1G, Q8T, W9L, F1N, S5J, T5A, X1I, Z0R, F7B, B1H, W7K, M5K, H1I, C6E, B3H, T2J, Z1V, Q1D, B1C, A1R, A6K, O5X, K2A, Q4C, Z1F, C4C, M5T, A5J, E4C, K5S, E5T, K6K, J2O, K6D, I0M, L1S, D3A, C5M, A5R, F7I, N2R, S1V, W3F, Z9M, I2Z, H8T, O7M, H6A, Q0Y, A1Z, N5E, K0A, K2K, K9V, K2U, M0I, Z3Y, H1B, Q2J, D1G, R0V, O1B, F2G, U0Q, Z2H, D7Y, S1P, Q1Q, M0Z, F0A, R6U, J6C, K6N, R5N</t>
+          <t>Z5D, M2N, E0N, R8P, W7E, V1P, V5P, P9Z, E3H, Q5R, T0P, G5B, R4L, C3Q, S5L, O2C, B2D, C8I, D9E, G2H, W5J, B5E, Z4S, N4F, W9F, R1V, F9W, N8M, F2H, W0S, Q3U, N5B, F0K, K8C, A5D, F6C, A5G, W4I, R2N, V4S, P6F, Z8D, P6Z, A2Q, F6E, W0P, V7P, O2O, C3G, K0P, P0U, Z1S, K5Q, G2D, I7G, F7V, C5U, X2K, V7Y, T0F, L2J, C0R, W4F, F3C, E2F, C2U, C9U, F0G, C8U, D6P, Q6H, W1W, T0Z, K2V, Y4U, B9X, Q9Z, P2L, E2N, Q8V, I9J, U3P, Z2Z, V2F, W2A, W6O, W1A, V7F, Y1Z, U2R, U2E, Q2C, Z1J, F9T, A4M, E1R, J1T, Z8S, A4R, Y9V, I5M, F5T, T0J, Q6Q, O4M, C5Y, N3K, D9G, V5S, A6C, F7E, C8Y, W1Q, U2I, K6V, Z3N, Q0F, D6F, D2V, R8K, Y1D, G1C, S1I, D0P, C9I, V5W, R6V, O0G, Z7S, J8Y, W7L, G3G, O1S, D4S, L1V, W0Y, K7O, K8B, X3A, O7Y, Q7O, Q8X, F9C, G0V, U2U, E6E, T1H, E1M, K1P, V3W, G0O, Q6Z, E0Z, N4L, Z8U, E5H, E3X, R1R, W5Q, W7M, U3Y, Q2M, I1G, Q8T, W9L, F1N, S5J, T5A, X1I, Z0R, F7B, B1H, W7K, M5K, H1I, C6E, B3H, T2J, Z1V, Q1D, B1C, A1R, A6K, O5X, K2A, Q4C, Z1F, C4C, M5T, A5J, E4C, K5S, E5T, K6K, J2O, K6D, I0M, L1S, D3A, C5M, A5R, F7I, N2R, S1V, W3F, Z9M, I2Z, H8T, O7M, H6A, Q0Y, A1Z, N5E, K0A, K2K, K9V, K2U, Z3Y, H1B, Q2J, D1G, R0V, O1B, F2G, U0Q, Z2H, D7Y, S1P, Q1Q, M0Z, F0A, R6U, J6C, K6N, R5N</t>
         </is>
       </c>
       <c r="E366" t="inlineStr">
@@ -10606,7 +10874,11 @@
           <t>WEB37895016015571</t>
         </is>
       </c>
-      <c r="F373" t="inlineStr"/>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -10630,7 +10902,11 @@
           <t>W1T99649061460893</t>
         </is>
       </c>
-      <c r="F374" t="inlineStr"/>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -10682,7 +10958,11 @@
           <t>WEB43800996951988</t>
         </is>
       </c>
-      <c r="F376" t="inlineStr"/>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -10810,7 +11090,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Z5F, M3N, P2D, Z2A, F2N, R1Q, J3E, Q0X, N0S, O4A, P9D, I1M, N0D, V1C, V1K, X9Y, P8F, P0A, J9K, A6Q, V5T, W2H, D1G, X1X, Q7P, X1Z, M0A, W2P, W0U, N8K, E3J, R8E, Z1F, L2J, C0E, Q6R, V6X, O1H, B5J, K3B, C3P, I9W, K7P, Y6J, R5E, P2H, X1O, H1Y, Z5Q, S9X, F1U, D7F, B1U, M7F, F0G, A2I, J1F, I5G, U8B, Q8G, X1F, Q1N, Y4Y, R8N, Q6W, W0S, W0Z, E8A, B3K, Z2L, J3P, A1F, M8Q, C6I, T1C, M5S, G9Z, N6T, K3Y, J8Z, E1W, P6L, Q4X, B1B, W9G, I6Z, Q6Y, W6L, I0E, P1C, H2F, K8C, D3S, L1P, N7N, X4A, T2S, F0I, R7B, G5Y, F7S, V1X, W2Q, I2E, Q8E, C5T, W1O, F6J, Y9W, I0C, C1C, I5X, I2D, Q4R, P7Q, W0O, F9M, T0X, V6Y, C6T, C8B, R1I, U2P, I6M, O2D, C2C, B5E, P5P, D7Q, Q8X, R2N, Z1R, I5A, C9C, O0G, N2I, T2C, J3S, M6O, J9R, C6A, W7M, Q3W, N2E, W5U, N5C, C0Y, Z8V, F7Q, G0V, W7V, K6U, W2G, N4G, W9C, C7T, Q8B, K0S, N4B, E0E, D5N, F3H, R4W, J2U, U2S, O5M, F2M, K7B, T3C, W6Z, E1U, B5Z, J1P, W1W, O0F, T1J, O8C, S9Y, E1D, D7N, N7G, X9W, T1M, V7K, W5O, G1F, L1C, C4M, U6A, R9X, P2I, L4C, P1J, E2B, H8R, W0Q, M0E, X6F, C6Q, J3C, W3Q, V8Y, N3N, C9Z, M8P, E6D, J4Z, U3H, M5H, E3L, K6L, Z5A, N3K, U5A, U3E, R1W, C2O, L1Q, F5C, G0D, K0O, G0O, I9X, E1B, Z7Y, V2L, K5V, O5O, C9M, P6Y, E3Z, T0W, M6N, C1K, J2I, Z7B, Z1S, E4L, C5F, X3O, A4S, R0T, Q9Z, O2M, V1M, X1A, U8D, R5N, K0W, B4A, Y1U, Z2K, E1Q, F7Y, G2E, C0B, I6L, C8H, F0V, G0K, Q7A, T0G, T2E, W3L, U0Q, O4P, P6P, Z9M, E9F, W2I, U0B, O8I, V1H, P6X, W9I, J1Q, I0Y, K3F, W3H, E9J, K5J, V7M, Z6K</t>
+          <t>Z5F, M3N, P2D, Z2A, F2N, R1Q, J3E, Q0X, N0S, O4A, P9D, I1M, N0D, V1C, V1K, X9Y, P8F, P0A, J9K, A6Q, V5T, W2H, D1G, X1X, Q7P, X1Z, M0A, W2P, W0U, N8K, E3J, R8E, Z1F, L2J, C0E, Q6R, V6X, O1H, B5J, K3B, C3P, I9W, K7P, Y6J, R5E, P2H, X1O, H1Y, Z5Q, S9X, F1U, D7F, B1U, M7F, F0G, A2I, J1F, I5G, U8B, Q8G, X1F, Q1N, Y4Y, R8N, Q6W, W0S, W0Z, E8A, B3K, Z2L, J3P, A1F, M8Q, C6I, T1C, M5S, G9Z, N6T, K3Y, J8Z, E1W, P6L, Q4X, B1B, W9G, I6Z, Q6Y, W6L, I0E, P1C, H2F, K8C, D3S, L1P, N7N, X4A, T2S, F0I, R7B, G5Y, F7S, V1X, W2Q, I2E, Q8E, C5T, W1O, F6J, Y9W, I0C, C1C, I5X, I2D, Q4R, P7Q, W0O, F9M, T0X, V6Y, C6T, C8B, R1I, U2P, I6M, O2D, C2C, B5E, P5P, D7Q, Q8X, R2N, Z1R, I5A, C9C, O0G, N2I, T2C, J3S, M6O, J9R, C6A, W7M, Q3W, N2E, W5U, N5C, C0Y, Z8V, F7Q, G0V, W7V, K6U, W2G, N4G, W9C, C7T, Q8B, K0S, N4B, E0E, D5N, F3H, R4W, J2U, U2S, O5M, F2M, K7B, T3C, W6Z, E1U, B5Z, J1P, W1W, O0F, T1J, O8C, S9Y, E1D, D7N, N7G, X9W, T1M, V7K, W5O, G1F, L1C, C4M, U6A, R9X, P2I, L4C, P1J, E2B, H8R, W0Q, M0E, X6F, C6Q, J3C, W3Q, V8Y, N3N, C9Z, M8P, E6D, J4Z, U3H, M5H, E3L, K6L, N3K, U5A, U3E, R1W, C2O, L1Q, F5C, G0D, K0O, G0O, I9X, E1B, Z7Y, V2L, K5V, O5O, C9M, P6Y, E3Z, T0W, M6N, C1K, J2I, Z7B, Z1S, E4L, C5F, X3O, A4S, R0T, Q9Z, O2M, V1M, X1A, U8D, R5N, K0W, B4A, Y1U, Z2K, E1Q, F7Y, G2E, C0B, I6L, C8H, F0V, G0K, Q7A, T0G, T2E, W3L, U0Q, O4P, P6P, Z9M, E9F, W2I, U0B, O8I, V1H, P6X, W9I, J1Q, I0Y, K3F, W3H, E9J, K5J, V7M, Z6K</t>
         </is>
       </c>
       <c r="E381" t="inlineStr">
@@ -10874,7 +11154,11 @@
           <t>WEB37379629070027</t>
         </is>
       </c>
-      <c r="F383" t="inlineStr"/>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -11066,7 +11350,11 @@
           <t>WDB81949956077542</t>
         </is>
       </c>
-      <c r="F390" t="inlineStr"/>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -11222,7 +11510,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>Z5E, M3C, N2R, E3G, U8X, V2S, J1F, J5S, R1P, Z8I, K3Y, C5V, O4A, R8K, Q8T, P2S, N1M, J2Z, P2C, J3Q, P0S, O6G, Z6B, Z7Y, Z5K, O4C, P9C, Z2W, M8U, Z5A, O6T, Q1H, P0H, Y4R, Y4I, O5T, K2C, O2R, Q0N, N0I, Q5H, R2D, N5A, K5B, S9W, K2K, H8W, W8C, V8O, K6X, Q6R, I2C, A4R, W4Q, Z0K, C9R, V8B, P9A, S1D, P8D, F2C, Q6M, Q6A, A9Z, Q7L, J2B, F5Y, R6V, J3F, K8C, E9D, D1B, K7P, A6J, F5F, E0X, Y6E, B4M, R3G, D1M, O1D, Y1W, O1W, Z7L, P2V, Z5H, C3Q, J3I, P2E, A2Y, V1J, N3T, Q8M, C2Z, F7S, O2K, U6B, X2W, R5M, F5Z, Q7R, T1J, X1M, Z8V, J1W, W1X, M9V, Y4J, L1N, Z1B, Y3M, M0F, H2G, N7A, P2N, R6T, L3Z, S1R, T1L, T3N, Y1H, M7S, C4K, K2P, A2T, Q7G, Z1S, C9J, G3A, O7Z, R2Q, O2P, Q6G, Q8Z, O1A, Q8X, W2Y, C5X, B4A, B3K, V8W, I5M, P8F, W4L, N0H, N7O, Z2M, C1B, V6H, E1J, P1E, B1G, L1B, C1U, U0C, A6P, L1I, E6E, B1I, P6Y, F0Z, C0B, N6T, O1U, Q9C, Q2V, D7A, K5L, U1E, C3J, K7F, C2G, C9B, Y4H, K7W, I7M, E4E, D5W, T1Z, C4S, C5G, T3A, E4Z, Z9J, K0Z, H2F</t>
+          <t>Z5E, M3C, N2R, E3G, U8X, V2S, J1F, J5S, R1P, Z8I, K3Y, C5V, O4A, R8K, Q8T, P2S, N1M, J2Z, P2C, J3Q, P0S, O6G, Z6B, Z7Y, Z5K, O4C, P9C, Z2W, M8U, O6T, Q1H, P0H, Y4R, Y4I, O5T, K2C, O2R, Q0N, N0I, Q5H, R2D, N5A, K5B, S9W, K2K, H8W, W8C, V8O, K6X, Q6R, I2C, A4R, W4Q, Z0K, C9R, V8B, P9A, S1D, P8D, F2C, Q6M, Q6A, A9Z, Q7L, J2B, F5Y, R6V, J3F, K8C, E9D, D1B, K7P, A6J, F5F, E0X, Y6E, B4M, R3G, D1M, O1D, Y1W, O1W, Z7L, P2V, Z5H, C3Q, J3I, P2E, A2Y, V1J, N3T, Q8M, C2Z, F7S, O2K, U6B, X2W, R5M, F5Z, Q7R, T1J, X1M, Z8V, J1W, W1X, M9V, Y4J, L1N, Z1B, Y3M, M0F, H2G, N7A, P2N, R6T, L3Z, S1R, T1L, T3N, Y1H, M7S, C4K, K2P, A2T, Q7G, Z1S, C9J, G3A, O7Z, R2Q, O2P, Q6G, Q8Z, O1A, Q8X, W2Y, C5X, B4A, B3K, V8W, I5M, P8F, W4L, N0H, N7O, Z2M, C1B, V6H, E1J, P1E, B1G, L1B, C1U, U0C, A6P, L1I, E6E, B1I, P6Y, F0Z, C0B, N6T, O1U, Q9C, Q2V, D7A, K5L, U1E, C3J, K7F, C2G, C9B, Y4H, K7W, I7M, E4E, D5W, T1Z, C4S, C5G, T3A, E4Z, Z9J, K0Z, H2F</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -11306,7 +11594,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>Z5F, M3N, Q1T, I5V, I5C, E1E, Z4J, A2P, B5N, V0V, N1A, W9C, C0A, C4F, R6V, I5T, P8A, Q3X, D4I, U3M, C8X, D7C, F0Q, W0M, M9E, N9V, Z5P, J0Z, Q9W, A4L, X4L, F2F, O4E, W8E, E4Z, W8U, F6E, O8J, Y6D, X1E, D1W, Z1Q, F1Q, Z2B, Q1O, V0X, Q0F, F1E, K7R, V7U, T1X, Y4G, N3U, U6E, W7R, Q5H, X4S, P9D, J3N, F8E, O8D, K2T, V6Q, B4M, Q3U, P0E, Z2W, O4F, U1E, Q6S, I4X, D3Z, G5Y, I5M, A2O, Y1V, I6Z, F1U, Z0H, Z2H, Q4F, N3S, G0A, G5Z, D9L, F1S, I3O, C9Q, F8D, J2X, C3R, Q5A, C6A, E9L, T1K, F2Z, V6X, W5J, K0Z, T2I, C2Y, U3P, R2Q, K6Q, F2P, F6G, F0A, B3G, F7S, M0J, W1P, Q4B, F9P, S5D, Z0X, Q7S, Z8J, J1E, T3L, P2F, Z4G, W4E, E4G, X3C, C8U, E0C, E8L, C0T, M0Z, E3Y, K5R, U2T, W7E, F2N, Q5K, I7M, A6B, F2O, D1P, D6Z, C4G, N8B, F1J, F7R, W6N, L9V, U1A, F4Y, Z8C, U5A, Z3F, T3M, Z3S, A5D, C0D, T0Z, K2K, S5K, F0T, N4N, A5E, K6K, F8G, M9W, G1E, V1D, I1T, G2F, P0A, W2J, N3F, E7L, B1X, E5Y, F0D, K0P, C5W, X9V, F0W, I7X, D2H, R4X, X1B, D5R, T3N, H1Y, N2F, B2F, C6G, K6Y, R5F, Y1E, V1G, V8A, D7P, A4W, D0V, K6W, J2B, U9Z, H8Z, Z5I, D6W, C1Q, U1V, F7Z, X3G, P2P, O8T, E1H, Z8E, Z4K, X2M, W3L, F7T, K3U, A1A, O6T, G3A, P0Z, M0A, D1N, W5U, J1Z, S8H, U3O, Z2S, O6H, W9Q, Y4P, E5U, T5V, V1Q, C8V, N7I, K8B, O4C</t>
+          <t>Z5F, M3N, Q1T, I5V, I5C, E1E, Z4J, A2P, B5N, V0V, N1A, W9C, C0A, C4F, R6V, I5T, P8A, Q3X, D4I, U3M, C8X, D7C, F0Q, W0M, M9E, N9V, Z5P, J0Z, Q9W, A4L, X4L, F2F, O4E, W8E, E4Z, W8U, F6E, O8J, Y6D, X1E, D1W, Z1Q, F1Q, Z2B, Q1O, V0X, Q0F, F1E, K7R, V7U, T1X, Y4G, N3U, U6E, W7R, Q5H, X4S, P9D, J3N, F8E, O8D, K2T, V6Q, B4M, Q3U, P0E, Z2W, O4F, U1E, Q6S, I4X, D3Z, G5Y, I5M, A2O, Y1V, I6Z, F1U, Z0H, Z2H, Q4F, N3S, G0A, G5Z, D9L, F1S, I3O, C9Q, F8D, J2X, C3R, Q5A, C6A, E9L, T1K, F2Z, V6X, W5J, K0Z, T2I, C2Y, U3P, R2Q, K6Q, F2P, F6G, F0A, B3G, F7S, W1P, Q4B, F9P, S5D, Z0X, Q7S, Z8J, J1E, T3L, P2F, Z4G, W4E, E4G, X3C, C8U, E0C, E8L, C0T, M0Z, E3Y, K5R, U2T, W7E, F2N, Q5K, I7M, A6B, F2O, D1P, D6Z, C4G, N8B, F1J, F7R, W6N, L9V, U1A, F4Y, Z8C, U5A, Z3F, T3M, Z3S, A5D, C0D, T0Z, K2K, S5K, F0T, N4N, A5E, K6K, F8G, M9W, G1E, V1D, I1T, G2F, P0A, W2J, N3F, E7L, B1X, E5Y, F0D, K0P, C5W, X9V, F0W, I7X, D2H, R4X, X1B, D5R, T3N, H1Y, N2F, B2F, C6G, K6Y, R5F, Y1E, V1G, V8A, D7P, A4W, D0V, K6W, J2B, U9Z, H8Z, Z5I, D6W, C1Q, U1V, F7Z, X3G, P2P, O8T, E1H, Z8E, Z4K, X2M, W3L, F7T, K3U, A1A, O6T, G3A, P0Z, M0A, D1N, W5U, J1Z, S8H, U3O, Z2S, O6H, W9Q, Y4P, E5U, T5V, V1Q, C8V, N7I, K8B, O4C</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -11342,7 +11630,11 @@
           <t>WDB47139503886394</t>
         </is>
       </c>
-      <c r="F400" t="inlineStr"/>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -11386,7 +11678,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>Z5C, M2A, I9Z, Q9Z, Z4T, R2I, K7W, Y9V, L9A, I4L, V4A, K6L, W3A, V8W, P8D, Q3W, P2N, D1M, U3B, C7N, Z0P, G3A, J3O, R4D, U3P, H8U, Z3B, E4L, N7B, W0S, K5V, F2U, D6F, O1S, Q7H, T0I, M5B, T0W, C1R, W4N, Y1P, E6G, O4H, P9D, D7W, K1D, Q6F, E6J, Q5B, D4I, Q4J, V1U, K1N, B9Z, C5T, Z3K, O1Y, K1C, T1F, F1B, D1D, H1K, E1M, Q0B, H6A, I0S, R5R, N7N, R5W, Y4O, D5O, C6W, W2I, C7K, W4J, R4Y, Q4M, D6R, V8V, E4C, F8Z, V6S, J3P, S5Q, O6P, Q1H, U2R, I6H, F2L, D9Q, F5H, I6C, B5Z, M0I, D3G, C5O, E6L, Y1W, P1J, K9V, G0B, N0S, Q3F, P9F, O8O, V7K, Q6X, T1U, P1A, R1W, O4R, V3A, Q1U, I4Y, S5Z, F9Y, S5D, Q1T, C7I, Z2E, R4L, G1C, X3C, P7Q, N1H, E0K, I7V, A2J, E7E, C8J, M4D, A1H, W0Q, U1E, N5B, J6C, R1Q, I6T, K6T, T1G, N5W, A1A, C8L, U1F, R8D, J8Y, Q5K, C8X, F1Y, Q8Q, D2Q, K5J, U0B, E4B, E5E, I4J, C7C, F8G, X3G, H8Q, A0D, N1A, M7U, H2B, W8M, E3E, F3P, V6B, K1H, Z4S, R2E, Z4F, X3T, H1N, B1Y, Z7Z, D3X</t>
+          <t>Z5C, M2A, I9Z, Q9Z, Z4T, R2I, K7W, Y9V, L9A, I4L, V4A, K6L, W3A, V8W, P8D, Q3W, P2N, D1M, U3B, C7N, Z0P, G3A, J3O, R4D, U3P, H8U, Z3B, E4L, N7B, W0S, K5V, F2U, D6F, O1S, Q7H, T0I, M5B, T0W, C1R, W4N, Y1P, E6G, O4H, P9D, D7W, K1D, Q6F, E6J, Q5B, D4I, Q4J, V1U, K1N, B9Z, C5T, Z3K, O1Y, K1C, T1F, F1B, D1D, H1K, E1M, Q0B, H6A, I0S, R5R, N7N, R5W, Y4O, D5O, C6W, W2I, C7K, W4J, R4Y, Q4M, D6R, V8V, E4C, F8Z, V6S, J3P, S5Q, O6P, Q1H, U2R, I6H, F2L, D9Q, F5H, I6C, B5Z, D3G, C5O, E6L, Y1W, P1J, K9V, G0B, N0S, Q3F, P9F, O8O, V7K, Q6X, T1U, P1A, R1W, O4R, V3A, Q1U, I4Y, S5Z, F9Y, S5D, Q1T, C7I, Z2E, R4L, G1C, X3C, P7Q, N1H, E0K, I7V, A2J, E7E, C8J, M4D, A1H, W0Q, U1E, N5B, J6C, R1Q, I6T, K6T, T1G, N5W, A1A, C8L, U1F, R8D, J8Y, Q5K, C8X, F1Y, Q8Q, D2Q, K5J, U0B, E4B, E5E, I4J, C7C, F8G, X3G, H8Q, A0D, N1A, M7U, H2B, W8M, E3E, F3P, V6B, K1H, Z4S, R2E, Z4F, X3T, H1N, B1Y, Z7Z, D3X</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
@@ -11478,7 +11770,11 @@
           <t>NMB21050253684912</t>
         </is>
       </c>
-      <c r="F405" t="inlineStr"/>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -11634,7 +11930,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Z5L, M3H, F2V, J1X, O1V, Z7M, C7A, G0R, D7J, Q1B, L4B, G1J, O8C, G3A, P8Y, Q6E, N0Z, P6D, I0K, E1M, C9E, P1L, C1Y, D0I, V8A, Z1N, Y1O, C5X, K0S, F0E, K7L, Y4J, V5P, P1C, O1F, Z7Z, B3K, T0F, N0X, K4J, P1J, Q6A, R4D, V8Z, I0E, Q3D, Y4Y, F6I, S9Y, I0C, Y6J, P8Z, A2T, X1R, M0W, O1A, R5O, Y6D, Z7R, S8C, W0R, Z5A, W3A, A5Q, X3V, J2R, O6P, W6R, N9Y, R4Y, I5C, O4B, V1M, D0D, N6I, K8X, N6R, E5W, W2J, B2A, V4S, K6R, U2E, D7B, J1B, K3F, I5G, C5P, U2T, E0Z, A2X, R1O, R7K, D1L, V7V, R1F, A4S, Y1E, Z3U, P5F, U0E, N7O, L1I, K6F, D1B, N5Y, I4H, K3B, J3S, W2V, A4Y, F1B, J8X, F3Y, Z6I, D6G, N9V, J9E, B5A, C4V, F3B, X9W, T2E, N6P, O8O, X3D, A1O, D3W, C5Q, O4R, N7B, N2I, F3V, R7J, F7D, O6S, Q1Q, F5D, K1B, L4C, Q8P, L1O, O4O, C8T, P5X, Q8Q, Z7S, R3H, I5S, Q6C, X1P, B4L, K5V, A5R, M0E, P8B, C5D, K3J, B2X, E4F, Q6R, C2O, D3H, L1S, P6A, X3A, X4A, D9M, M5W, Z2C, N5Z, J3V, A4B, G0U, D5L, L1C, N1Y, K6G, U1F, K5E, C3P, Z3R, O8T, Z7I, Q1G, V1G, P9P, U3Y, A1H, I3D, N8N, E1A, Z5S, D6E, M5H, D1C, N5U, Q3E, K4N, R7L, D1U, O7Y, P2D, A6K, V1Y, G9Y, W9P, K7Y, S1W, J1V, U1R, Z1Q</t>
+          <t>Z5L, M3H, F2V, J1X, O1V, Z7M, C7A, G0R, D7J, Q1B, L4B, G1J, O8C, G3A, P8Y, Q6E, N0Z, P6D, I0K, E1M, C9E, P1L, C1Y, D0I, V8A, Z1N, Y1O, C5X, K0S, F0E, K7L, Y4J, V5P, P1C, O1F, Z7Z, B3K, T0F, N0X, K4J, P1J, Q6A, R4D, V8Z, I0E, Q3D, Y4Y, F6I, S9Y, I0C, Y6J, P8Z, A2T, X1R, M0W, O1A, R5O, Y6D, Z7R, S8C, W0R, W3A, A5Q, X3V, J2R, O6P, W6R, N9Y, R4Y, I5C, O4B, V1M, D0D, N6I, K8X, N6R, E5W, W2J, B2A, V4S, K6R, U2E, D7B, J1B, K3F, I5G, C5P, U2T, E0Z, A2X, R1O, R7K, D1L, V7V, R1F, A4S, Y1E, Z3U, P5F, U0E, N7O, L1I, K6F, D1B, N5Y, I4H, K3B, J3S, W2V, A4Y, F1B, J8X, F3Y, Z6I, D6G, N9V, J9E, B5A, C4V, F3B, X9W, T2E, N6P, O8O, X3D, A1O, D3W, C5Q, O4R, N7B, N2I, F3V, R7J, F7D, O6S, Q1Q, F5D, K1B, L4C, Q8P, L1O, O4O, C8T, P5X, Q8Q, Z7S, R3H, I5S, Q6C, X1P, B4L, K5V, A5R, M0E, P8B, C5D, K3J, B2X, E4F, Q6R, C2O, D3H, L1S, P6A, X3A, X4A, D9M, M5W, Z2C, N5Z, J3V, A4B, G0U, D5L, L1C, N1Y, K6G, U1F, K5E, C3P, Z3R, O8T, Z7I, Q1G, V1G, P9P, U3Y, A1H, I3D, N8N, E1A, Z5S, D6E, M5H, D1C, N5U, Q3E, K4N, R7L, D1U, O7Y, P2D, A6K, V1Y, G9Y, W9P, K7Y, S1W, J1V, U1R, Z1Q</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -11642,7 +11938,11 @@
           <t>NMB31881944007447</t>
         </is>
       </c>
-      <c r="F411" t="inlineStr"/>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -11658,7 +11958,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Z5C, M2E, Q8U, Z8Y, Q1I, R1Z, C2J, K6T, R4X, N1A, I4Q, O8E, Q2Q, Q4P, M6D, L3A, K4K, C5X, X1L, A3A, K1E, D4Z, A2O, B2G, C7G, C1R, Y4B, A6N, B5D, H8W, E1L, P7A, U3Y, K0H, D8M, G5Z, Z4J, K1I, Q6W, E1Q, B2X, Q8V, C1V, N3U, D5Y, T1J, U6B, J3Q, W3M, F0F, I0C, X2I, I7H, C4M, E9X, I5E, M8L, D5J, O4F, Y2A, N1G, X3Z, D3A, Y1Y, P0C, O6S, B5B, D3V, S5B, I1J, U6E, Q4L, V1L, Y1A, F2L, L1I, N4G, A5S, N0A, A6A, W2H, B1C, W3H, Q8Q, C5Z, P0F, C1N, X2D, Q3W, D6P, R2P, Z7A, H1M, D6X, Q0Y, W5J, Z2S, I1M, N5A, J6A, Q5Z, G4Z, X1X, Q7V, U1P, F8D, E0D, F2Q, N9V, C2O, F8H, V6W, K3A, A4X, S5F, F6E, D3T, E0Y, U1V, T0Y, P6Z, K2W, D7X, R2L, Z2I, P2M, W6N, V0W, T1X, X2E, C1Q, J3G, D9T, Q8C, D2K, Z1C, C5I, A2J, Z7K, U8Z, Z9V, O7M, N4E, X2N, P9K, C1X, C8S, F9Y, P2J, M0I, Z7D, C0T, N9U, Q2A, W0V, T2V, N7A, O4G, F9R, E6K, F5K, A4M, J2X, V7N, V2T, F0W, E2I, V2S, F4H</t>
+          <t>Z5C, M2E, Q8U, Z8Y, Q1I, R1Z, C2J, K6T, R4X, N1A, I4Q, O8E, Q2Q, Q4P, M6D, L3A, K4K, C5X, X1L, A3A, K1E, D4Z, A2O, B2G, C7G, C1R, Y4B, A6N, B5D, H8W, E1L, P7A, U3Y, K0H, D8M, G5Z, Z4J, K1I, Q6W, E1Q, B2X, Q8V, C1V, N3U, D5Y, T1J, U6B, J3Q, W3M, F0F, I0C, X2I, I7H, C4M, E9X, I5E, M8L, D5J, O4F, Y2A, N1G, X3Z, D3A, Y1Y, P0C, O6S, B5B, D3V, S5B, I1J, U6E, Q4L, V1L, Y1A, F2L, L1I, N4G, A5S, N0A, A6A, W2H, B1C, W3H, Q8Q, C5Z, P0F, C1N, X2D, Q3W, D6P, R2P, Z7A, H1M, D6X, Q0Y, W5J, Z2S, I1M, N5A, J6A, Q5Z, G4Z, X1X, Q7V, U1P, F8D, E0D, F2Q, N9V, C2O, F8H, V6W, K3A, A4X, S5F, F6E, D3T, E0Y, U1V, T0Y, P6Z, K2W, D7X, R2L, Z2I, P2M, W6N, V0W, T1X, X2E, C1Q, J3G, D9T, Q8C, D2K, Z1C, C5I, A2J, Z7K, U8Z, Z9V, O7M, N4E, X2N, P9K, C1X, C8S, F9Y, P2J, Z7D, C0T, N9U, Q2A, W0V, T2V, N7A, O4G, F9R, E6K, F5K, A4M, J2X, V7N, V2T, F0W, E2I, V2S, F4H</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">
@@ -11806,7 +12106,11 @@
           <t>WDB17777585978238</t>
         </is>
       </c>
-      <c r="F417" t="inlineStr"/>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -11934,7 +12238,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>Z5E, M3E, C5C, C3D, J2W, Y4H, M0S, N4A, W7N, R1U, I4U, E3S, G3F, Y9W, X4L, E9L, N5E, Z3X, V7E, M5V, P2P, A1X, Q8O, F0E, X2C, G1E, Q5T, Z4U, T0S, D7R, Z4I, N1T, K5O, L1A, Q3D, F6Q, C4V, T2V, K4F, Z6B, Q2V, L2Q, I9W, W7F, W9P, W5I, S5Q, G0G, X1A, A0D, D2X, Q6R, C2L, E2B, X3T, K7N, J9Z, R1M, S1P, O7F, Z9D, D6X, Q6G, R1N, Z3G, A5R, J3A, M8D, Q1J, Z8T, W9S, N8D, Y1X, G1M, G1B, Y3I, W5R, E6H, P6X, O1D, D5Q, J6B, J9E, I7H, M0T, Q6N, C6F, J3T, C8D, C8G, O7L, J8Y, E1E, C8R, V7N, N5H, L2M, W9C, C1U, C2V, N6T, Z9Z, Z1C, Z0U, D5W, C1P, W5S, Z1U, N5M, Q5D, P0A, F4Y, K1W, A0H, A5G, W2D, M8A, C9Q, Z5I, I5E, G3N, D5P, N7B, M9Y, F5Z, Q1K, K3R, Y1O, M4D, J1E, B1U, F5T, M0I, O8E, F7Q, V1M, A1L, E1B, P5P, M5Z, D0D, Q7K, V1J, Q3F, Q6J, C4F, F6C, K1S, B1E, K0V, I0U, Z9E, J6A, T0V, C5P, G0N, O1X, M7R, A5S, O2A, Z4P, Y4U, S1O, T2T, J1X, F9Z, R2U, C8F, D9H, W0R, L0U, R1W, X3D, V8A, I1C, W4P, F1B, J1Y, E5V, V6C, C5M, E2A, D3Y, P6Z, R2J, W4E, D5R, O1Y, P1M, Z7A, B9Y, U3R, W3K, A1G, X3O, E0U</t>
+          <t>Z5E, M3E, C5C, C3D, J2W, Y4H, M0S, N4A, W7N, R1U, I4U, E3S, G3F, Y9W, X4L, E9L, N5E, Z3X, V7E, M5V, P2P, A1X, Q8O, F0E, X2C, G1E, Q5T, Z4U, T0S, D7R, Z4I, N1T, K5O, L1A, Q3D, F6Q, C4V, T2V, K4F, Z6B, Q2V, L2Q, I9W, W7F, W9P, W5I, S5Q, G0G, X1A, A0D, D2X, Q6R, C2L, E2B, X3T, K7N, J9Z, R1M, S1P, O7F, Z9D, D6X, Q6G, R1N, Z3G, A5R, J3A, M8D, Q1J, Z8T, W9S, N8D, Y1X, G1M, G1B, Y3I, W5R, E6H, P6X, O1D, D5Q, J6B, J9E, I7H, M0T, Q6N, C6F, J3T, C8D, C8G, O7L, J8Y, E1E, C8R, V7N, N5H, L2M, W9C, C1U, C2V, N6T, Z9Z, Z1C, Z0U, D5W, C1P, W5S, Z1U, N5M, Q5D, P0A, F4Y, K1W, A0H, A5G, W2D, M8A, C9Q, Z5I, I5E, G3N, D5P, N7B, M9Y, F5Z, Q1K, K3R, Y1O, M4D, J1E, B1U, F5T, O8E, F7Q, V1M, A1L, E1B, P5P, M5Z, D0D, Q7K, V1J, Q3F, Q6J, C4F, F6C, K1S, B1E, K0V, I0U, Z9E, J6A, T0V, C5P, G0N, O1X, M7R, A5S, O2A, Z4P, Y4U, S1O, T2T, J1X, F9Z, R2U, C8F, D9H, W0R, L0U, R1W, X3D, V8A, I1C, W4P, F1B, J1Y, E5V, V6C, C5M, E2A, D3Y, P6Z, R2J, W4E, D5R, O1Y, P1M, Z7A, B9Y, U3R, W3K, A1G, X3O, E0U</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -12054,7 +12358,11 @@
           <t>NMB60659679802754</t>
         </is>
       </c>
-      <c r="F426" t="inlineStr"/>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -12078,7 +12386,11 @@
           <t>WEB22860781682238</t>
         </is>
       </c>
-      <c r="F427" t="inlineStr"/>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
@@ -12326,7 +12638,11 @@
           <t>W1T23222616356329</t>
         </is>
       </c>
-      <c r="F436" t="inlineStr"/>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
@@ -12378,7 +12694,11 @@
           <t>NMB82174401589591</t>
         </is>
       </c>
-      <c r="F438" t="inlineStr"/>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
@@ -12534,7 +12854,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Z5B, M1H, Z4I, B4M, W9J, I5H, P2S, Q5A, I5V, P1L, Q7R, R8C, P8A, A4B, C5W, U2S, T3K, I6F, N4M, K8X, N2H, W4V, D2U, K6B, C2N, I1I, Q2N, Q8D, J9Z, W0J, Y1H, K4V, N3D, W1U, G2F, R0R, J9A, K6V, F5G, W3Y, A5Y, N4D, M0H, P6B, P2R, Z0F, M1E, W7A, Z9F, P0F, T4A, Y3E, K0V, E6Z, H1Y, Z8P, V7O, Z6G, A5R, J1P, D9L, N0M, Q6L, X1E, A1D, W4G, N3E, V9H, M0Z, F0Z, C8P, T1X, N8B, O7W, V7B, W9H, G3A, F5B, F0Y, G5H, Q7Y, W1M, K4H, E0K, Z0X, W5E, Q2P, J2W, D7X, M0L, B5C, R0E, W2W, F3K, F6M, F3W, I2N, I6V, U3G, V9A, N3J, I5Z, R2I, O5O, C6S, N6L, M0I, Z5U, M1C, E3G, A6L, M8L, K0N, C8V, P5F, W4H, C7Y, W2P, E5C, Q2I, R6Z, C7W, Y1E, S5Z, B5F, G0Q, V2E, W5R, I0U, X1G, J2G, C5J, B1U, O8E, U2E, J6Y, P2C, Q8G, A5A, D3F, B5I, T2T, F3B, D7L, A1C, P0U, F4I, V2D, L4B, W3C, Q5N, W9R, J3T, N6E, Z9Y, V5P, T5V, P9T, Y6E, D0X, W1R, D1U, W3K, G3Y, C9A, I2R, P5Z, E3K, Q0W, W1F, L9Z, F9X, H1K, I2M, F5D, V7C, R6S, F5Z, T0W, A4Y, V7I, Q8Q, E0Z, F7W, U0B, C0G, M8S, Z3I, U5B, R1T, Q0B, A6Q, U8X, K0E</t>
+          <t>Z5B, M1H, Z4I, B4M, W9J, I5H, P2S, Q5A, I5V, P1L, Q7R, R8C, P8A, A4B, C5W, U2S, T3K, I6F, N4M, K8X, N2H, W4V, D2U, K6B, C2N, I1I, Q2N, Q8D, J9Z, W0J, Y1H, K4V, N3D, W1U, G2F, R0R, J9A, K6V, F5G, W3Y, A5Y, N4D, M0H, P6B, P2R, Z0F, M1E, W7A, Z9F, P0F, T4A, Y3E, K0V, E6Z, H1Y, Z8P, V7O, Z6G, A5R, J1P, D9L, N0M, Q6L, X1E, A1D, W4G, N3E, V9H, M0Z, F0Z, C8P, T1X, N8B, O7W, V7B, W9H, G3A, F5B, F0Y, G5H, Q7Y, W1M, K4H, E0K, Z0X, W5E, Q2P, J2W, D7X, M0L, B5C, R0E, W2W, F3K, F6M, F3W, I2N, I6V, U3G, V9A, N3J, I5Z, R2I, O5O, C6S, N6L, Z5U, M1C, E3G, A6L, M8L, K0N, C8V, P5F, W4H, C7Y, W2P, E5C, Q2I, R6Z, C7W, Y1E, S5Z, B5F, G0Q, V2E, W5R, I0U, X1G, J2G, C5J, B1U, O8E, U2E, J6Y, P2C, Q8G, A5A, D3F, B5I, T2T, F3B, D7L, A1C, P0U, F4I, V2D, L4B, W3C, Q5N, W9R, J3T, N6E, Z9Y, V5P, T5V, P9T, Y6E, D0X, W1R, D1U, W3K, G3Y, C9A, I2R, P5Z, E3K, Q0W, W1F, L9Z, F9X, H1K, I2M, F5D, V7C, R6S, F5Z, T0W, A4Y, V7I, Q8Q, E0Z, F7W, U0B, C0G, M8S, Z3I, U5B, R1T, Q0B, A6Q, U8X, K0E</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
@@ -12590,7 +12910,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>Z5B, M1J, D2O, M9Z, C0L, J3R, Y4B, Z7J, E0F, T3K, Y4R, F1Y, V8N, C5E, F3Y, N5E, I5C, Q2M, W6Y, D7B, D0R, O4D, N5F, K4O, M9X, W2I, X2C, I6B, K1A, U3P, J9B, F3V, M7I, X9Z, K3B, R4L, P2K, F1N, D3N, I4B, E0E, J1Q, Z5Z, Q1H, T3L, Q1B, T1Z, Q7C, N5V, H8Q, E4E, B5D, F7R, A1P, I2P, W3W, W8C, B9W, W2A, I3L, D6G, F5N, F9Y, A3A, D8Z, E1Z, K6X, K9Z, I9H, E5G, X1R, V1G, F0A, Q0C, R1F, B5Z, Q6W, Q8C, R2H, M7U, A2I, W3N, E0C, Q6E, D9G, N6E, E0X, W6C, P0T, Z6J, J3H, Q1L, F2W, Q8W, Z2Q, R8K, F1B, Q8X, O9I, F7Y, G4C, I6O, X4C, I4E, B5L, I6A, X2F, X3R, J3P, Q7Q, W3Q, T1F, E7F, F7S, D5O, W1B, A6L, O6A, S8J, E5T, P0C, F1V, P2I, W1G, F0P, A2C, E3L, F5K, I4J, Z9E, K1B, Y4V, J3A, O7F, V5S, V5O, F7Z, C2Z, Y1T, V1M, Z0P, Z5W, Q4N, V7O, O5Y, A2Q, W1X, G4D, V7Z, A0H, Z1R, V6Y, N9X, C6P, W3H, W3E, K0S, U6C, A6N, Y9Y, Z8A, W6S, J6B, C7G, I9W, H8U, F2A, C8R, C5P, V6P, Z5H, M0J, K0F, D2J, V8Q, C5T, R4X, N0M, A5I, W8M, I2A, O8B, G2H, G3Y, D3O, X4N, Z6S, Z1Z, D7L, P5X, N4Y, J9Q, D5F, E2B, E2A, F6Y, K4N, O7O, M0D, M5V, Q1C, C0S, A6E, Z7S, O3A, L9E, D0P, K8Y, A2Y, V1N, K3U, E3K, D7W, W2K, P8B, V7V, A6B, L2A, V0R, E9C, V7P, W9C, I6C, E3W, C0D, N0B, Z7O, Q8Y, G3X, P7Y, O0B, P5B, Y4U, R6C, D4C, Y4S, C5U, A6H, C3T, K6R, W4R, H6A, J2K, S6F, H2D, P2W, A4G, F3P, T0F, E9X, W1O, C9T, Z8Y, Q2G, L1P, J2W, Q2A, R2J, K7R, F8B, I8X, C5Z, V7T, K5Q, K7G, B2F, F2N, D1D, V6E</t>
+          <t>Z5B, M1J, D2O, M9Z, C0L, J3R, Y4B, Z7J, E0F, T3K, Y4R, F1Y, V8N, C5E, F3Y, N5E, I5C, Q2M, W6Y, D7B, D0R, O4D, N5F, K4O, M9X, W2I, X2C, I6B, K1A, U3P, J9B, F3V, M7I, X9Z, K3B, R4L, P2K, F1N, D3N, I4B, E0E, J1Q, Z5Z, Q1H, T3L, Q1B, T1Z, Q7C, N5V, H8Q, E4E, B5D, F7R, A1P, I2P, W3W, W8C, B9W, W2A, I3L, D6G, F5N, F9Y, A3A, D8Z, E1Z, K6X, K9Z, I9H, E5G, X1R, V1G, F0A, Q0C, R1F, B5Z, Q6W, Q8C, R2H, M7U, A2I, W3N, E0C, Q6E, D9G, N6E, E0X, W6C, P0T, Z6J, J3H, Q1L, F2W, Q8W, Z2Q, R8K, F1B, Q8X, O9I, F7Y, G4C, I6O, X4C, I4E, B5L, I6A, X2F, X3R, J3P, Q7Q, W3Q, T1F, E7F, F7S, D5O, W1B, A6L, O6A, S8J, E5T, P0C, F1V, P2I, W1G, F0P, A2C, E3L, F5K, I4J, Z9E, K1B, Y4V, J3A, O7F, V5S, V5O, F7Z, C2Z, Y1T, V1M, Z0P, Z5W, Q4N, V7O, O5Y, A2Q, W1X, G4D, V7Z, A0H, Z1R, V6Y, N9X, C6P, W3H, W3E, K0S, U6C, A6N, Y9Y, Z8A, W6S, J6B, C7G, I9W, H8U, F2A, C8R, C5P, V6P, Z5H, K0F, D2J, V8Q, C5T, R4X, N0M, A5I, W8M, I2A, O8B, G2H, G3Y, D3O, X4N, Z6S, Z1Z, D7L, P5X, N4Y, J9Q, D5F, E2B, E2A, F6Y, K4N, O7O, M0D, M5V, Q1C, C0S, A6E, Z7S, O3A, L9E, D0P, K8Y, A2Y, V1N, K3U, E3K, D7W, W2K, P8B, V7V, A6B, L2A, V0R, E9C, V7P, W9C, I6C, E3W, C0D, N0B, Z7O, Q8Y, G3X, P7Y, O0B, P5B, Y4U, R6C, D4C, Y4S, C5U, A6H, C3T, K6R, W4R, H6A, J2K, S6F, H2D, P2W, A4G, F3P, T0F, E9X, W1O, C9T, Z8Y, Q2G, L1P, J2W, Q2A, R2J, K7R, F8B, I8X, C5Z, V7T, K5Q, K7G, B2F, F2N, D1D, V6E</t>
         </is>
       </c>
       <c r="E446" t="inlineStr">
@@ -12626,7 +12946,11 @@
           <t>NMB16209071001147</t>
         </is>
       </c>
-      <c r="F447" t="inlineStr"/>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
@@ -12678,7 +13002,11 @@
           <t>WEB65168982529271</t>
         </is>
       </c>
-      <c r="F449" t="inlineStr"/>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
@@ -12890,7 +13218,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>Z5D, M2S, E1S, P1L, Z7J, M9O, Z5I, G2H, B2G, N6E, K3R, X1O, C9Z, P9F, G5B, P9Y, A2L, W4U, C7Q, K0Z, J1Z, C5B, G1C, F0Q, V6Y, Z8L, O9G, I1A, U5B, X2E, E2L, X3I, C3B, D6N, X1D, D5W, U0D, K6D, P2I, W0T, U2K, K0V, X3R, C5E, D4H, M0J, R5I, Q6S, Q0N, F1A, J3Q, V2F, P0R, W2Y, I1V, Q2F, N5Y, Z2L, F6N, T3M, E3J, S5M, P1A, C1Z, A6T, U2R, T1B, L1O, O6H, R1Q, E0M, Z0P, R0E, C8P, I1Q, W5A, J3H, V0V, A6F, R0Z, U3E, K6W, Q4S, W8M, H1M, U3Q, C0L, R6M, S5Q, M5G, A1M, J1D, N4N, Q5X, W8P, C3Q, H1H, Y9V, E6G, C2E, F0O, P0B, Z7B, N3G, Q5B, D1Q, I6K, F5H, B4L, X3V, R6B, P2W, Z4J, H2I, E9F, W2P, C3V, D7J, Q2M, D7B, X3Y, R2S, C1X, G4H, Q5D, T1D, K7K, V8B, B1H, I7Y</t>
+          <t>Z5D, M2S, E1S, P1L, Z7J, M9O, Z5I, G2H, B2G, N6E, K3R, X1O, C9Z, P9F, G5B, P9Y, A2L, W4U, C7Q, K0Z, J1Z, C5B, G1C, F0Q, V6Y, Z8L, O9G, I1A, U5B, X2E, E2L, X3I, C3B, D6N, X1D, D5W, U0D, K6D, P2I, W0T, U2K, K0V, X3R, C5E, D4H, R5I, Q6S, Q0N, F1A, J3Q, V2F, P0R, W2Y, I1V, Q2F, N5Y, Z2L, F6N, T3M, E3J, S5M, P1A, C1Z, A6T, U2R, T1B, L1O, O6H, R1Q, E0M, Z0P, R0E, C8P, I1Q, W5A, J3H, V0V, A6F, R0Z, U3E, K6W, Q4S, W8M, H1M, U3Q, C0L, R6M, S5Q, M5G, A1M, J1D, N4N, Q5X, W8P, C3Q, H1H, Y9V, E6G, C2E, F0O, P0B, Z7B, N3G, Q5B, D1Q, I6K, F5H, B4L, X3V, R6B, P2W, Z4J, H2I, E9F, W2P, C3V, D7J, Q2M, D7B, X3Y, R2S, C1X, G4H, Q5D, T1D, K7K, V8B, B1H, I7Y</t>
         </is>
       </c>
       <c r="E457" t="inlineStr">
@@ -13198,7 +13526,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Z5L, M3J, A4M, P6Y, C7E, A1H, V6G, D5N, E0N, K1L, K5U, Q1K, D4U, Z3Z, T0K, Z7D, O6S, Z1W, W6W, U2P, K6S, E9D, E6K, Z4Y, F9T, F1N, D7V, S1H, W2J, N5X, C3B, Q2Y, T1X, C0Y, Q3L, D3T, M8C, K5P, N0S, Q2J, K3A, U3B, R1W, V6Z, J6B, E1E, Q7M, E4G, T2D, E4C, A4F, O7M, J3P, F9X, D6R, I1I, Q1F, J2O, U9Z, O4P, G1H, Y9C, M0J, L9G, M9E, Z2P, Q1C, X1H, W9R, W3J, K1H, Z9F, X3D, W6R, W7L, Q6F, R1X, K8A, R1E, O1D, W6U, L1N, S9Y, T0J, V7M, V4N, Z5P, A4Y, P5Z, M7U, S1S, Z0S, I9I, A2P, W1Q, I4A, M5X, W7N, D5X, X2M, T3R, H2K, J1S, U3H, E8L, T3Q, J2B, M9U, C6G, G3G, K6F, U3M, K4J, J9P, F6B, F0D, X1I, N0D, A5S, N8N, W5Y, K6B, S1G, Q4Z, C1L, E5H, F7Y, Y4J, K5L, N8B, G1E, E1G, S5J, E6Y, X3L, O8B, P8Y, Q6H, K7Q, X1L, T1M, F9A, Q4C, W6G, Z5T, Y9V, Z6E, I6Z, R2C, E6G, Z5Q, V8O, O3D, D4B, T2V, A1G, Q7S, T1I, J3F, O3C, F7G, Q2U, Q2F, D2P, V1G, D3Z, N8H, I4D, V4T, A9Z, S3A, N5J, Q6C, B9V, D3O, A2G, Q1Y, O2I, K7D, F2Y, C3E, A5L, Q0W, Z1L, P0S, W3T, G1F, N4L, E3K, Q4K, Q2Q, Z1M, O5U, X3G, J9Q, V2N, B1F, L4Z, M8Y, D7C, G5F, K5Q, W0T, B1E, K0X, C5Y, G2E, J2A, K4O, R1S, T2F, M7J, J1K, R5H, W0G, Z2L, Z8T, Z3U, X2F, Z4F, T1Y, Z7I, K0G, J9L, F2Q, F3S, N5N, I4F, U1F, I9Y, V1Z, D0D, T1B, Z0O, D8M, P4W, J3H, C7N, I4H, L4A, I8X, V2R, F8V, V1H, P2K, P0A, W6K, E4B, C2G, W4E, K1G, M0F, X3O, N7C, Z4W, J9X, Z3W, J2Y, W3D, Q8T, W0Y, I4X, V7X, C3P, E7F, U5B, E8A, P6X, R1B, Q7R, Q1V, A0C, E2R, P6I, J6Y, A1O, X2X</t>
+          <t>Z5L, M3J, A4M, P6Y, C7E, A1H, V6G, D5N, E0N, K1L, K5U, Q1K, D4U, Z3Z, T0K, Z7D, O6S, Z1W, W6W, U2P, K6S, E9D, E6K, Z4Y, F9T, F1N, D7V, S1H, W2J, N5X, C3B, Q2Y, T1X, C0Y, Q3L, D3T, M8C, K5P, N0S, Q2J, K3A, U3B, R1W, V6Z, J6B, E1E, Q7M, E4G, T2D, E4C, A4F, O7M, J3P, F9X, D6R, I1I, Q1F, J2O, U9Z, O4P, G1H, Y9C, L9G, M9E, Z2P, Q1C, X1H, W9R, W3J, K1H, Z9F, X3D, W6R, W7L, Q6F, R1X, K8A, R1E, O1D, W6U, L1N, S9Y, T0J, V7M, V4N, Z5P, A4Y, P5Z, M7U, S1S, Z0S, I9I, A2P, W1Q, I4A, M5X, W7N, D5X, X2M, T3R, H2K, J1S, U3H, E8L, T3Q, J2B, M9U, C6G, G3G, K6F, U3M, K4J, J9P, F6B, F0D, X1I, N0D, A5S, N8N, W5Y, K6B, S1G, Q4Z, C1L, E5H, F7Y, Y4J, K5L, N8B, G1E, E1G, S5J, E6Y, X3L, O8B, P8Y, Q6H, K7Q, X1L, T1M, F9A, Q4C, W6G, Z5T, Y9V, Z6E, I6Z, R2C, E6G, Z5Q, V8O, O3D, D4B, T2V, A1G, Q7S, T1I, J3F, O3C, F7G, Q2U, Q2F, D2P, V1G, D3Z, N8H, I4D, V4T, A9Z, S3A, N5J, Q6C, B9V, D3O, A2G, Q1Y, O2I, K7D, F2Y, C3E, A5L, Q0W, Z1L, P0S, W3T, G1F, N4L, E3K, Q4K, Q2Q, Z1M, O5U, X3G, J9Q, V2N, B1F, L4Z, M8Y, D7C, G5F, K5Q, W0T, B1E, K0X, C5Y, G2E, J2A, K4O, R1S, T2F, M7J, J1K, R5H, W0G, Z2L, Z8T, Z3U, X2F, Z4F, T1Y, Z7I, K0G, J9L, F2Q, F3S, N5N, I4F, U1F, I9Y, V1Z, D0D, T1B, Z0O, D8M, P4W, J3H, C7N, I4H, L4A, I8X, V2R, F8V, V1H, P2K, P0A, W6K, E4B, C2G, W4E, K1G, M0F, X3O, N7C, Z4W, J9X, Z3W, J2Y, W3D, Q8T, W0Y, I4X, V7X, C3P, E7F, U5B, E8A, P6X, R1B, Q7R, Q1V, A0C, E2R, P6I, J6Y, A1O, X2X</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -13206,7 +13534,11 @@
           <t>W1T98661055753711</t>
         </is>
       </c>
-      <c r="F468" t="inlineStr"/>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>OM 460</t>
+        </is>
+      </c>
     </row>
     <row r="469">
       <c r="A469" s="1" t="n">

</xml_diff>